<commit_message>
Jatai working to Venkat 07/07/2019
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -3227,7 +3227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3406,6 +3406,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3688,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="E160" workbookViewId="0">
+      <selection activeCell="H160" sqref="H160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4933,7 +4936,7 @@
       <c r="G48" s="51" t="s">
         <v>432</v>
       </c>
-      <c r="H48" s="54" t="s">
+      <c r="H48" s="84" t="s">
         <v>68</v>
       </c>
       <c r="I48" s="1"/>
@@ -4962,7 +4965,7 @@
       <c r="G49" s="35" t="s">
         <v>432</v>
       </c>
-      <c r="H49" s="55" t="s">
+      <c r="H49" s="84" t="s">
         <v>71</v>
       </c>
       <c r="I49" s="1"/>

</xml_diff>

<commit_message>
Jatai Ghanam BRH and other files 30/12/2019
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -4282,7 +4282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O186"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
@@ -9212,11 +9212,11 @@
   <dimension ref="B2:H268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="G56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomRight" activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9999,7 +9999,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="49" spans="2:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
@@ -10007,7 +10007,7 @@
       <c r="F49" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="35" t="s">
         <v>591</v>
       </c>
       <c r="H49" s="85" t="s">

</xml_diff>

<commit_message>
Various edits Jatai Ghanam Convention 21/02/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -6263,10 +6263,10 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H161" sqref="H161"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai Working edits 26/05/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5208" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jatai!$A$1:$R$174</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterate="1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6262,11 +6262,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F67" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12571,12 +12571,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J206" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K98" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai working files pushed 19/06/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5208" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="1702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="1701">
   <si>
     <t>Rules Observed from JatA Mani and JatA DarpaNam</t>
   </si>
@@ -4690,9 +4690,6 @@
   </si>
   <si>
     <t>u no elongation</t>
-  </si>
-  <si>
-    <t>no avRt.</t>
   </si>
   <si>
     <t>n not N</t>
@@ -6269,11 +6266,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B119" sqref="B119:B120"/>
+      <selection pane="bottomRight" activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6363,7 +6360,7 @@
         <v>1281</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G4" s="48"/>
       <c r="H4" s="11"/>
@@ -6399,7 +6396,7 @@
         <v>1281</v>
       </c>
       <c r="F5" s="64" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="11"/>
@@ -6435,7 +6432,7 @@
         <v>1281</v>
       </c>
       <c r="F6" s="64" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="G6" s="48"/>
       <c r="H6" s="11"/>
@@ -6512,7 +6509,7 @@
         <v>1104</v>
       </c>
       <c r="G8" s="80" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
@@ -6522,7 +6519,7 @@
         <v>461</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -6550,7 +6547,7 @@
         <v>1104</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
@@ -6624,7 +6621,7 @@
         <v>1114</v>
       </c>
       <c r="G11" s="64" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="9" t="s">
@@ -6653,7 +6650,7 @@
         <v>149</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>1289</v>
@@ -6665,7 +6662,7 @@
         <v>1115</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>251</v>
@@ -6702,7 +6699,7 @@
         <v>1114</v>
       </c>
       <c r="G13" s="64" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="9" t="s">
@@ -6740,7 +6737,7 @@
         <v>1146</v>
       </c>
       <c r="G14" s="64" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
@@ -7064,7 +7061,7 @@
         <v>435</v>
       </c>
       <c r="K23" s="43" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -7538,7 +7535,7 @@
         <v>1117</v>
       </c>
       <c r="G36" s="80" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="11" t="s">
@@ -8082,7 +8079,7 @@
         <v>1102</v>
       </c>
       <c r="G51" s="64" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="11" t="s">
@@ -8222,7 +8219,7 @@
         <v>148</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>1322</v>
@@ -8341,7 +8338,7 @@
         <v>1212</v>
       </c>
       <c r="F58" s="64" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="G58" s="48"/>
       <c r="H58" s="84" t="s">
@@ -8379,7 +8376,7 @@
         <v>1213</v>
       </c>
       <c r="F59" s="64" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="G59" s="48"/>
       <c r="H59" s="84" t="s">
@@ -8489,10 +8486,10 @@
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="64" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="G62" s="64" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="H62" s="11"/>
       <c r="I62" s="21" t="s">
@@ -8525,7 +8522,7 @@
         <v>1185</v>
       </c>
       <c r="F63" s="77" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="G63" s="77" t="s">
         <v>1110</v>
@@ -8561,7 +8558,7 @@
         <v>1186</v>
       </c>
       <c r="F64" s="77" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="G64" s="77" t="s">
         <v>1110</v>
@@ -8599,7 +8596,7 @@
         <v>1475</v>
       </c>
       <c r="F65" s="77" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="G65" s="10"/>
       <c r="H65" s="17"/>
@@ -8633,7 +8630,7 @@
         <v>1183</v>
       </c>
       <c r="F66" s="77" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="G66" s="10"/>
       <c r="H66" s="17"/>
@@ -8641,7 +8638,7 @@
         <v>18</v>
       </c>
       <c r="J66" s="140" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="K66" s="36" t="s">
         <v>17</v>
@@ -8709,7 +8706,7 @@
         <v>100</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>323</v>
@@ -8747,7 +8744,7 @@
         <v>100</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="I69" s="21" t="s">
         <v>324</v>
@@ -8785,7 +8782,7 @@
         <v>821</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>324</v>
@@ -8861,7 +8858,7 @@
         <v>1125</v>
       </c>
       <c r="H72" s="64" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="I72" s="21" t="s">
         <v>223</v>
@@ -8899,7 +8896,7 @@
         <v>100</v>
       </c>
       <c r="H73" s="64" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="I73" s="21" t="s">
         <v>317</v>
@@ -8946,7 +8943,7 @@
         <v>1129</v>
       </c>
       <c r="K74" s="138" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -9125,7 +9122,7 @@
       </c>
       <c r="G79" s="48"/>
       <c r="H79" s="11" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="I79" s="21" t="s">
         <v>295</v>
@@ -9163,7 +9160,7 @@
       </c>
       <c r="G80" s="48"/>
       <c r="H80" s="11" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I80" s="21" t="s">
         <v>224</v>
@@ -9236,10 +9233,10 @@
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="64" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="I82" s="21" t="s">
         <v>820</v>
@@ -9277,7 +9274,7 @@
       </c>
       <c r="G83" s="48"/>
       <c r="H83" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="I83" s="21" t="s">
         <v>331</v>
@@ -9315,7 +9312,7 @@
       </c>
       <c r="G84" s="48"/>
       <c r="H84" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="I84" s="21" t="s">
         <v>254</v>
@@ -9355,7 +9352,7 @@
         <v>191</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="I85" s="21" t="s">
         <v>254</v>
@@ -9393,7 +9390,7 @@
         <v>1131</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="I86" s="21" t="s">
         <v>330</v>
@@ -9641,7 +9638,7 @@
         <v>1181</v>
       </c>
       <c r="F93" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G93" s="9"/>
       <c r="H93" s="11" t="s">
@@ -9679,7 +9676,7 @@
         <v>1177</v>
       </c>
       <c r="F94" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G94" s="9"/>
       <c r="H94" s="11" t="s">
@@ -9715,7 +9712,7 @@
       </c>
       <c r="E95" s="9"/>
       <c r="F95" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G95" s="9"/>
       <c r="H95" s="11" t="s">
@@ -9791,7 +9788,7 @@
         <v>1274</v>
       </c>
       <c r="F97" s="64" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="G97" s="48"/>
       <c r="H97" s="11"/>
@@ -9903,7 +9900,7 @@
         <v>1180</v>
       </c>
       <c r="F100" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G100" s="9"/>
       <c r="H100" s="11"/>
@@ -9942,7 +9939,7 @@
         <v>1112</v>
       </c>
       <c r="G101" s="77" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="H101" s="84" t="s">
         <v>75</v>
@@ -10018,7 +10015,7 @@
       </c>
       <c r="F103" s="9"/>
       <c r="G103" s="64" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="H103" s="33" t="s">
         <v>811</v>
@@ -10059,7 +10056,7 @@
       </c>
       <c r="G104" s="48"/>
       <c r="H104" s="100" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="I104" s="79" t="s">
         <v>227</v>
@@ -10087,7 +10084,7 @@
         <v>1263</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>1264</v>
@@ -10125,7 +10122,7 @@
         <v>1263</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>1265</v>
@@ -10135,7 +10132,7 @@
       </c>
       <c r="G106" s="48"/>
       <c r="H106" s="33" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="I106" s="21" t="s">
         <v>234</v>
@@ -10163,7 +10160,7 @@
         <v>1263</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E107" s="9" t="s">
         <v>1266</v>
@@ -10173,7 +10170,7 @@
       </c>
       <c r="G107" s="48"/>
       <c r="H107" s="33" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="I107" s="21" t="s">
         <v>235</v>
@@ -10203,13 +10200,13 @@
         <v>1263</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E108" s="9" t="s">
         <v>1267</v>
       </c>
       <c r="F108" s="64" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G108" s="48"/>
       <c r="H108" s="11"/>
@@ -10239,14 +10236,14 @@
         <v>1263</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>1269</v>
       </c>
       <c r="F109" s="9"/>
       <c r="G109" s="64" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="H109" s="11"/>
       <c r="I109" s="21" t="s">
@@ -10275,13 +10272,13 @@
         <v>1263</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>1270</v>
       </c>
       <c r="F110" s="81" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G110" s="48"/>
       <c r="H110" s="11" t="s">
@@ -10313,13 +10310,13 @@
         <v>1263</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>1271</v>
       </c>
       <c r="F111" s="64" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G111" s="48"/>
       <c r="H111" s="11"/>
@@ -10355,7 +10352,7 @@
         <v>1229</v>
       </c>
       <c r="F112" s="64" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="G112" s="64" t="s">
         <v>1142</v>
@@ -10390,13 +10387,13 @@
         <v>1226</v>
       </c>
       <c r="E113" s="72" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F113" s="94" t="s">
+        <v>1671</v>
+      </c>
+      <c r="G113" s="139" t="s">
         <v>1676</v>
-      </c>
-      <c r="F113" s="94" t="s">
-        <v>1672</v>
-      </c>
-      <c r="G113" s="139" t="s">
-        <v>1677</v>
       </c>
       <c r="H113" s="11" t="s">
         <v>803</v>
@@ -10430,13 +10427,13 @@
         <v>1207</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="F114" s="64" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G114" s="139" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="H114" s="11" t="s">
         <v>802</v>
@@ -10470,10 +10467,10 @@
         <v>1225</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="F115" s="64" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G115" s="48"/>
       <c r="H115" s="11" t="s">
@@ -11037,7 +11034,7 @@
         <v>1196</v>
       </c>
       <c r="F131" s="77" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="G131" s="48"/>
       <c r="H131" s="17"/>
@@ -11523,11 +11520,11 @@
         <v>1175</v>
       </c>
       <c r="F145" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G145" s="9"/>
       <c r="H145" s="33" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="I145" s="21" t="s">
         <v>49</v>
@@ -11561,11 +11558,11 @@
         <v>1174</v>
       </c>
       <c r="F146" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G146" s="9"/>
       <c r="H146" s="33" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="I146" s="21" t="s">
         <v>245</v>
@@ -11593,13 +11590,13 @@
         <v>808</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>1182</v>
       </c>
       <c r="F147" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G147" s="9"/>
       <c r="H147" s="33" t="s">
@@ -11641,7 +11638,7 @@
         <v>62</v>
       </c>
       <c r="H148" s="33" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I148" s="90" t="s">
         <v>506</v>
@@ -11679,7 +11676,7 @@
       </c>
       <c r="G149" s="48"/>
       <c r="H149" s="33" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="I149" s="21" t="s">
         <v>312</v>
@@ -11751,7 +11748,7 @@
         <v>62</v>
       </c>
       <c r="H151" s="33" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I151" s="21" t="s">
         <v>256</v>
@@ -11780,7 +11777,7 @@
       <c r="D152" s="9"/>
       <c r="E152" s="9"/>
       <c r="F152" s="64" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="G152" s="9"/>
       <c r="H152" s="33"/>
@@ -11813,7 +11810,7 @@
         <v>1371</v>
       </c>
       <c r="F153" s="77" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="G153" s="10"/>
       <c r="H153" s="101" t="s">
@@ -11841,20 +11838,20 @@
         <v>60</v>
       </c>
       <c r="C154" s="9" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D154" s="9" t="s">
         <v>1651</v>
       </c>
-      <c r="D154" s="9" t="s">
+      <c r="E154" s="9" t="s">
         <v>1652</v>
       </c>
-      <c r="E154" s="9" t="s">
-        <v>1653</v>
-      </c>
       <c r="F154" s="77" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="G154" s="10"/>
       <c r="H154" s="61" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="I154" s="61" t="s">
         <v>1097</v>
@@ -11885,11 +11882,11 @@
         <v>1210</v>
       </c>
       <c r="F155" s="64" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="G155" s="48"/>
       <c r="H155" s="33" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="I155" s="21" t="s">
         <v>313</v>
@@ -11922,11 +11919,11 @@
         <v>1211</v>
       </c>
       <c r="F156" s="64" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="G156" s="48"/>
       <c r="H156" s="33" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="I156" s="21" t="s">
         <v>258</v>
@@ -11994,7 +11991,7 @@
         <v>1285</v>
       </c>
       <c r="F158" s="64" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="G158" s="48"/>
       <c r="H158" s="11"/>
@@ -12029,7 +12026,7 @@
         <v>1286</v>
       </c>
       <c r="F159" s="64" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="G159" s="48"/>
       <c r="H159" s="11"/>
@@ -12064,11 +12061,11 @@
         <v>1284</v>
       </c>
       <c r="F160" s="64" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="G160" s="48"/>
       <c r="H160" s="11" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I160" s="21" t="s">
         <v>231</v>
@@ -12336,7 +12333,7 @@
         <v>1258</v>
       </c>
       <c r="F168" s="64" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G168" s="48"/>
       <c r="H168" s="33"/>
@@ -12371,7 +12368,7 @@
         <v>1259</v>
       </c>
       <c r="F169" s="64" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G169" s="48"/>
       <c r="H169" s="33"/>
@@ -12406,7 +12403,7 @@
         <v>1259</v>
       </c>
       <c r="F170" s="64" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G170" s="48"/>
       <c r="H170" s="33"/>
@@ -12442,7 +12439,7 @@
         <v>1218</v>
       </c>
       <c r="F171" s="65" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G171" s="48"/>
       <c r="H171" s="33"/>
@@ -12478,7 +12475,7 @@
         <v>1219</v>
       </c>
       <c r="F172" s="64" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G172" s="48"/>
       <c r="H172" s="11"/>
@@ -12513,7 +12510,7 @@
         <v>1220</v>
       </c>
       <c r="F173" s="82" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="G173" s="99"/>
       <c r="H173" s="74"/>
@@ -12578,12 +12575,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K53" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -12653,7 +12650,7 @@
         <v>1383</v>
       </c>
       <c r="E5" s="64" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F5" s="64"/>
       <c r="G5" s="64" t="s">
@@ -12679,21 +12676,21 @@
         <v>132</v>
       </c>
       <c r="E6" s="64" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="F6" s="64"/>
       <c r="G6" s="64" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="15" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="K6" s="71" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.3">
@@ -12730,7 +12727,7 @@
         <v>131</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="64"/>
@@ -12787,10 +12784,10 @@
         <v>1393</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="G10" s="64" t="s">
         <v>1049</v>
@@ -12815,10 +12812,10 @@
         <v>1393</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="F11" s="78" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="G11" s="64" t="s">
         <v>1057</v>
@@ -12846,7 +12843,7 @@
         <v>1302</v>
       </c>
       <c r="F12" s="134" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="G12" s="64" t="s">
         <v>1055</v>
@@ -12868,19 +12865,19 @@
         <v>148</v>
       </c>
       <c r="D13" s="64" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>1574</v>
+      </c>
+      <c r="F13" s="78" t="s">
         <v>1593</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>1575</v>
-      </c>
-      <c r="F13" s="78" t="s">
-        <v>1594</v>
       </c>
       <c r="G13" s="64" t="s">
         <v>1058</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>597</v>
@@ -12889,7 +12886,7 @@
         <v>740</v>
       </c>
       <c r="K13" s="57" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -12964,7 +12961,7 @@
         <v>1407</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="G16" s="64" t="s">
         <v>1049</v>
@@ -12989,10 +12986,10 @@
         <v>1411</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F17" s="78" t="s">
         <v>1565</v>
-      </c>
-      <c r="F17" s="78" t="s">
-        <v>1566</v>
       </c>
       <c r="G17" s="64" t="s">
         <v>1056</v>
@@ -13089,7 +13086,7 @@
         <v>711</v>
       </c>
       <c r="K20" s="71" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.3">
@@ -13101,10 +13098,10 @@
         <v>143</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="F21" s="64" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="G21" s="64" t="s">
         <v>1056</v>
@@ -13156,13 +13153,13 @@
         <v>148</v>
       </c>
       <c r="D23" s="64" t="s">
+        <v>1559</v>
+      </c>
+      <c r="E23" s="64" t="s">
         <v>1560</v>
       </c>
-      <c r="E23" s="64" t="s">
+      <c r="F23" s="64" t="s">
         <v>1561</v>
-      </c>
-      <c r="F23" s="64" t="s">
-        <v>1562</v>
       </c>
       <c r="G23" s="64" t="s">
         <v>1056</v>
@@ -13245,10 +13242,10 @@
         <v>1411</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="G26" s="65" t="s">
         <v>1056</v>
@@ -13270,19 +13267,19 @@
         <v>148</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>1571</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>1572</v>
-      </c>
       <c r="F27" s="78" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="G27" s="64" t="s">
         <v>1057</v>
       </c>
       <c r="H27" s="130" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>593</v>
@@ -13300,19 +13297,19 @@
         <v>148</v>
       </c>
       <c r="D28" s="64" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>1571</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="F28" s="78" t="s">
         <v>1572</v>
-      </c>
-      <c r="F28" s="78" t="s">
-        <v>1573</v>
       </c>
       <c r="G28" s="64" t="s">
         <v>1057</v>
       </c>
       <c r="H28" s="130" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>594</v>
@@ -13330,7 +13327,7 @@
         <v>148</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E29" s="64"/>
       <c r="F29" s="64"/>
@@ -13351,7 +13348,7 @@
     <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.3">
       <c r="B30" s="15"/>
       <c r="C30" s="65" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D30" s="64" t="s">
         <v>1393</v>
@@ -13377,7 +13374,7 @@
     <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.3">
       <c r="B31" s="15"/>
       <c r="C31" s="65" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D31" s="64"/>
       <c r="E31" s="9" t="s">
@@ -13401,7 +13398,7 @@
     <row r="32" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" s="15"/>
       <c r="C32" s="64" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D32" s="64" t="s">
         <v>1467</v>
@@ -13429,7 +13426,7 @@
     <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.3">
       <c r="B33" s="15"/>
       <c r="C33" s="64" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D33" s="64"/>
       <c r="E33" s="9" t="s">
@@ -13453,7 +13450,7 @@
     <row r="34" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B34" s="15"/>
       <c r="C34" s="64" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D34" s="64"/>
       <c r="E34" s="9" t="s">
@@ -13516,7 +13513,7 @@
         <v>1420</v>
       </c>
       <c r="F36" s="64" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="G36" s="64" t="s">
         <v>1064</v>
@@ -13538,13 +13535,13 @@
         <v>791</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="E37" s="64" t="s">
         <v>1423</v>
       </c>
       <c r="F37" s="64" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="G37" s="64" t="s">
         <v>1065</v>
@@ -13569,7 +13566,7 @@
         <v>1382</v>
       </c>
       <c r="E38" s="69" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F38" s="69"/>
       <c r="G38" s="64" t="s">
@@ -13595,7 +13592,7 @@
         <v>1382</v>
       </c>
       <c r="E39" s="69" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="F39" s="69"/>
       <c r="G39" s="64" t="s">
@@ -13621,10 +13618,10 @@
         <v>714</v>
       </c>
       <c r="E40" s="65" t="s">
+        <v>1578</v>
+      </c>
+      <c r="F40" s="65" t="s">
         <v>1579</v>
-      </c>
-      <c r="F40" s="65" t="s">
-        <v>1580</v>
       </c>
       <c r="G40" s="64" t="s">
         <v>1060</v>
@@ -13648,7 +13645,7 @@
         <v>791</v>
       </c>
       <c r="D41" s="64" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>1419</v>
@@ -13674,22 +13671,22 @@
         <v>791</v>
       </c>
       <c r="D42" s="64" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="64"/>
       <c r="G42" s="64" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="J42" s="26" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="K42" s="71" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="43" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
@@ -13703,17 +13700,17 @@
       <c r="E43" s="9"/>
       <c r="F43" s="64"/>
       <c r="G43" s="64" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9" t="s">
+        <v>1596</v>
+      </c>
+      <c r="J43" s="25" t="s">
         <v>1597</v>
       </c>
-      <c r="J43" s="25" t="s">
-        <v>1598</v>
-      </c>
       <c r="K43" s="71" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="44" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -13748,7 +13745,7 @@
         <v>1385</v>
       </c>
       <c r="D45" s="64" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="E45" s="64" t="s">
         <v>1421</v>
@@ -14085,7 +14082,7 @@
         <v>777</v>
       </c>
       <c r="K56" s="71" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="57" spans="2:11" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.3">
@@ -14290,7 +14287,7 @@
         <v>1135</v>
       </c>
       <c r="D65" s="64" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>1438</v>
@@ -14344,13 +14341,13 @@
         <v>1384</v>
       </c>
       <c r="D67" s="64" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>1415</v>
       </c>
       <c r="F67" s="64" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="G67" s="64" t="s">
         <v>1058</v>
@@ -14378,7 +14375,7 @@
         <v>1395</v>
       </c>
       <c r="F68" s="64" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="G68" s="64" t="s">
         <v>1056</v>
@@ -14400,10 +14397,10 @@
         <v>1339</v>
       </c>
       <c r="D69" s="63" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E69" s="63" t="s">
         <v>1519</v>
-      </c>
-      <c r="E69" s="63" t="s">
-        <v>1520</v>
       </c>
       <c r="F69" s="63"/>
       <c r="G69" s="64" t="s">
@@ -14432,7 +14429,7 @@
         <v>1161</v>
       </c>
       <c r="F70" s="63" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="G70" s="64" t="s">
         <v>1044</v>
@@ -14454,10 +14451,10 @@
         <v>1339</v>
       </c>
       <c r="D71" s="64" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E71" s="64" t="s">
         <v>1514</v>
-      </c>
-      <c r="E71" s="64" t="s">
-        <v>1515</v>
       </c>
       <c r="F71" s="64"/>
       <c r="G71" s="64" t="s">
@@ -14483,10 +14480,10 @@
         <v>1156</v>
       </c>
       <c r="E72" s="63" t="s">
+        <v>1515</v>
+      </c>
+      <c r="F72" s="63" t="s">
         <v>1516</v>
-      </c>
-      <c r="F72" s="63" t="s">
-        <v>1517</v>
       </c>
       <c r="G72" s="64" t="s">
         <v>1044</v>
@@ -14536,13 +14533,13 @@
         <v>139</v>
       </c>
       <c r="D74" s="64" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="E74" s="64" t="s">
         <v>1422</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="G74" s="64" t="s">
         <v>1065</v>
@@ -14628,7 +14625,7 @@
         <v>1325</v>
       </c>
       <c r="F77" s="64" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="G77" s="64" t="s">
         <v>1056</v>
@@ -14681,7 +14678,7 @@
         <v>1412</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="F79" s="64" t="s">
         <v>1304</v>
@@ -14703,14 +14700,14 @@
     <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.3">
       <c r="B80" s="9"/>
       <c r="C80" s="64" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D80" s="64" t="s">
         <v>1386</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="64" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="G80" s="64" t="s">
         <v>1090</v>
@@ -14729,14 +14726,14 @@
     <row r="81" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B81" s="9"/>
       <c r="C81" s="64" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D81" s="64" t="s">
         <v>1386</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="64" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="G81" s="64" t="s">
         <v>1090</v>
@@ -14868,7 +14865,7 @@
         <v>7</v>
       </c>
       <c r="D86" s="64" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>1446</v>
@@ -14894,7 +14891,7 @@
         <v>7</v>
       </c>
       <c r="D87" s="64" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>1187</v>
@@ -14920,7 +14917,7 @@
         <v>7</v>
       </c>
       <c r="D88" s="64" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>1447</v>
@@ -14976,7 +14973,7 @@
         <v>7</v>
       </c>
       <c r="D90" s="64" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>1420</v>
@@ -15002,7 +14999,7 @@
         <v>7</v>
       </c>
       <c r="D91" s="64" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>1230</v>
@@ -15110,7 +15107,7 @@
         <v>7</v>
       </c>
       <c r="D95" s="64" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>1225</v>
@@ -15229,9 +15226,7 @@
       <c r="E99" s="9" t="s">
         <v>1504</v>
       </c>
-      <c r="F99" s="9" t="s">
-        <v>1505</v>
-      </c>
+      <c r="F99" s="9"/>
       <c r="G99" s="64" t="s">
         <v>1034</v>
       </c>
@@ -15239,11 +15234,11 @@
       <c r="I99" s="9" t="s">
         <v>505</v>
       </c>
-      <c r="J99" s="35" t="s">
+      <c r="J99" s="52" t="s">
         <v>1035</v>
       </c>
       <c r="K99" s="71" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="100" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -15255,20 +15250,20 @@
         <v>1263</v>
       </c>
       <c r="E100" s="63" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="F100" s="63" t="s">
         <v>1406</v>
       </c>
       <c r="G100" s="64" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="H100" s="26"/>
       <c r="I100" s="9" t="s">
         <v>49</v>
       </c>
       <c r="J100" s="26" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="K100" s="57" t="s">
         <v>876</v>
@@ -15446,11 +15441,11 @@
         <v>7</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="E107" s="9"/>
       <c r="F107" s="9" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="G107" s="64" t="s">
         <v>1037</v>
@@ -15459,13 +15454,13 @@
         <v>797</v>
       </c>
       <c r="I107" s="9" t="s">
+        <v>1507</v>
+      </c>
+      <c r="J107" s="26" t="s">
         <v>1508</v>
       </c>
-      <c r="J107" s="26" t="s">
+      <c r="K107" s="71" t="s">
         <v>1509</v>
-      </c>
-      <c r="K107" s="71" t="s">
-        <v>1510</v>
       </c>
     </row>
     <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
@@ -15474,7 +15469,7 @@
         <v>7</v>
       </c>
       <c r="D108" s="64" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="E108" s="9"/>
       <c r="F108" s="64"/>
@@ -15498,7 +15493,7 @@
         <v>7</v>
       </c>
       <c r="D109" s="64" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="E109" s="9"/>
       <c r="F109" s="64"/>
@@ -15522,7 +15517,7 @@
         <v>7</v>
       </c>
       <c r="D110" s="64" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="E110" s="9"/>
       <c r="F110" s="64"/>
@@ -15552,7 +15547,7 @@
         <v>1191</v>
       </c>
       <c r="F111" s="64" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="G111" s="64" t="s">
         <v>1049</v>
@@ -15580,7 +15575,7 @@
         <v>1191</v>
       </c>
       <c r="F112" s="64" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="G112" s="64" t="s">
         <v>1049</v>
@@ -15608,7 +15603,7 @@
         <v>1191</v>
       </c>
       <c r="F113" s="63" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="G113" s="64" t="s">
         <v>1049</v>
@@ -15621,16 +15616,16 @@
         <v>774</v>
       </c>
       <c r="K113" s="71" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="114" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="B114" s="9"/>
       <c r="C114" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D114" s="64" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>1429</v>
@@ -15653,7 +15648,7 @@
     <row r="115" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B115" s="9"/>
       <c r="C115" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D115" s="64" t="s">
         <v>1387</v>
@@ -15681,10 +15676,10 @@
     <row r="116" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B116" s="9"/>
       <c r="C116" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D116" s="64" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>1354</v>
@@ -15707,10 +15702,10 @@
     <row r="117" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B117" s="9"/>
       <c r="C117" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D117" s="64" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>1161</v>
@@ -15733,7 +15728,7 @@
     <row r="118" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B118" s="9"/>
       <c r="C118" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D118" s="64" t="s">
         <v>1387</v>
@@ -15759,7 +15754,7 @@
     <row r="119" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B119" s="9"/>
       <c r="C119" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D119" s="64" t="s">
         <v>1387</v>
@@ -15785,10 +15780,10 @@
     <row r="120" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B120" s="9"/>
       <c r="C120" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D120" s="64" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>1437</v>
@@ -15811,10 +15806,10 @@
     <row r="121" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B121" s="9"/>
       <c r="C121" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D121" s="64" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>1437</v>
@@ -15837,7 +15832,7 @@
     <row r="122" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B122" s="9"/>
       <c r="C122" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>1387</v>
@@ -15857,13 +15852,13 @@
         <v>662</v>
       </c>
       <c r="K122" s="71" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="123" spans="2:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.3">
       <c r="B123" s="9"/>
       <c r="C123" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>1387</v>
@@ -15889,13 +15884,13 @@
     <row r="124" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B124" s="9"/>
       <c r="C124" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D124" s="64" t="s">
         <v>1387</v>
       </c>
       <c r="E124" s="64" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="F124" s="64"/>
       <c r="G124" s="64" t="s">
@@ -15915,13 +15910,13 @@
     <row r="125" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B125" s="9"/>
       <c r="C125" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D125" s="64" t="s">
         <v>1387</v>
       </c>
       <c r="E125" s="64" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="F125" s="64"/>
       <c r="G125" s="64" t="s">
@@ -15941,7 +15936,7 @@
     <row r="126" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B126" s="9"/>
       <c r="C126" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D126" s="64" t="s">
         <v>1386</v>
@@ -15950,7 +15945,7 @@
         <v>1209</v>
       </c>
       <c r="F126" s="64" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="G126" s="64" t="s">
         <v>1078</v>
@@ -15969,7 +15964,7 @@
     <row r="127" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B127" s="9"/>
       <c r="C127" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D127" s="64" t="s">
         <v>1386</v>
@@ -15978,7 +15973,7 @@
         <v>1439</v>
       </c>
       <c r="F127" s="64" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="G127" s="64" t="s">
         <v>1077</v>
@@ -15997,7 +15992,7 @@
     <row r="128" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B128" s="9"/>
       <c r="C128" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D128" s="64"/>
       <c r="E128" s="9" t="s">
@@ -16021,10 +16016,10 @@
     <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
       <c r="B129" s="61"/>
       <c r="C129" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D129" s="64" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>1425</v>
@@ -16047,10 +16042,10 @@
     <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B130" s="9"/>
       <c r="C130" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D130" s="64" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>1287</v>
@@ -16073,10 +16068,10 @@
     <row r="131" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B131" s="9"/>
       <c r="C131" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D131" s="64" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="E131" s="9" t="s">
         <v>1428</v>
@@ -16099,13 +16094,13 @@
     <row r="132" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B132" s="9"/>
       <c r="C132" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D132" s="64" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E132" s="9" t="s">
         <v>1612</v>
-      </c>
-      <c r="E132" s="9" t="s">
-        <v>1613</v>
       </c>
       <c r="F132" s="64"/>
       <c r="G132" s="64" t="s">
@@ -16125,13 +16120,13 @@
     <row r="133" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B133" s="9"/>
       <c r="C133" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D133" s="64" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E133" s="9" t="s">
         <v>1612</v>
-      </c>
-      <c r="E133" s="9" t="s">
-        <v>1613</v>
       </c>
       <c r="F133" s="64"/>
       <c r="G133" s="64" t="s">
@@ -16151,13 +16146,13 @@
     <row r="134" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B134" s="9"/>
       <c r="C134" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D134" s="64" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E134" s="9" t="s">
         <v>1612</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>1613</v>
       </c>
       <c r="F134" s="64"/>
       <c r="G134" s="64" t="s">
@@ -16177,17 +16172,17 @@
     <row r="135" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B135" s="9"/>
       <c r="C135" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D135" s="64" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="E135" s="9" t="s">
         <v>1427</v>
       </c>
       <c r="F135" s="64"/>
       <c r="G135" s="64" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="H135" s="61"/>
       <c r="I135" s="61" t="s">
@@ -16203,7 +16198,7 @@
     <row r="136" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B136" s="9"/>
       <c r="C136" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D136" s="64"/>
       <c r="E136" s="9" t="s">
@@ -16227,7 +16222,7 @@
     <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B137" s="9"/>
       <c r="C137" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D137" s="64" t="s">
         <v>1387</v>
@@ -16236,7 +16231,7 @@
         <v>1440</v>
       </c>
       <c r="F137" s="64" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="G137" s="64" t="s">
         <v>1081</v>
@@ -16255,10 +16250,10 @@
     <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B138" s="9"/>
       <c r="C138" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D138" s="64" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>1304</v>
@@ -16281,7 +16276,7 @@
     <row r="139" spans="2:11" s="62" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B139" s="9"/>
       <c r="C139" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D139" s="64"/>
       <c r="E139" s="9" t="s">
@@ -16305,10 +16300,10 @@
     <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B140" s="9"/>
       <c r="C140" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D140" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E140" s="64"/>
       <c r="F140" s="64"/>
@@ -16371,7 +16366,7 @@
         <v>1494</v>
       </c>
       <c r="G142" s="64" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="H142" s="9"/>
       <c r="I142" s="9" t="s">
@@ -16486,7 +16481,7 @@
         <v>1417</v>
       </c>
       <c r="F146" s="131" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="G146" s="64" t="s">
         <v>1061</v>
@@ -16511,10 +16506,10 @@
         <v>143</v>
       </c>
       <c r="E147" s="9" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F147" s="9" t="s">
         <v>1581</v>
-      </c>
-      <c r="F147" s="9" t="s">
-        <v>1582</v>
       </c>
       <c r="G147" s="64" t="s">
         <v>1061</v>
@@ -16539,10 +16534,10 @@
         <v>1387</v>
       </c>
       <c r="E148" s="64" t="s">
+        <v>1617</v>
+      </c>
+      <c r="F148" s="64" t="s">
         <v>1618</v>
-      </c>
-      <c r="F148" s="64" t="s">
-        <v>1619</v>
       </c>
       <c r="G148" s="64" t="s">
         <v>1082</v>
@@ -16592,7 +16587,7 @@
         <v>60</v>
       </c>
       <c r="D150" s="64" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E150" s="64" t="s">
         <v>1416</v>
@@ -16704,11 +16699,11 @@
         <v>60</v>
       </c>
       <c r="D154" s="66" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="E154" s="66"/>
       <c r="F154" s="66" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G154" s="83" t="s">
         <v>1041</v>
@@ -16729,7 +16724,7 @@
         <v>1389</v>
       </c>
       <c r="C155" s="64" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D155" s="64" t="s">
         <v>1378</v>
@@ -16775,7 +16770,7 @@
         <v>709</v>
       </c>
       <c r="K156" s="71" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
@@ -16784,13 +16779,13 @@
         <v>719</v>
       </c>
       <c r="D157" s="64" t="s">
+        <v>1605</v>
+      </c>
+      <c r="E157" s="9" t="s">
         <v>1606</v>
       </c>
-      <c r="E157" s="9" t="s">
+      <c r="F157" s="64" t="s">
         <v>1607</v>
-      </c>
-      <c r="F157" s="64" t="s">
-        <v>1608</v>
       </c>
       <c r="G157" s="64" t="s">
         <v>1066</v>
@@ -16812,13 +16807,13 @@
         <v>719</v>
       </c>
       <c r="D158" s="64" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E158" s="64" t="s">
         <v>1543</v>
       </c>
-      <c r="E158" s="64" t="s">
+      <c r="F158" s="64" t="s">
         <v>1544</v>
-      </c>
-      <c r="F158" s="64" t="s">
-        <v>1545</v>
       </c>
       <c r="G158" s="64" t="s">
         <v>1051</v>
@@ -16843,10 +16838,10 @@
         <v>1381</v>
       </c>
       <c r="E159" s="64" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F159" s="129" t="s">
         <v>1541</v>
-      </c>
-      <c r="F159" s="129" t="s">
-        <v>1542</v>
       </c>
       <c r="G159" s="64" t="s">
         <v>1051</v>
@@ -16871,10 +16866,10 @@
         <v>1381</v>
       </c>
       <c r="E160" s="64" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F160" s="64" t="s">
         <v>1537</v>
-      </c>
-      <c r="F160" s="64" t="s">
-        <v>1538</v>
       </c>
       <c r="G160" s="64" t="s">
         <v>1051</v>
@@ -16899,10 +16894,10 @@
         <v>1381</v>
       </c>
       <c r="E161" s="64" t="s">
+        <v>1536</v>
+      </c>
+      <c r="F161" s="64" t="s">
         <v>1537</v>
-      </c>
-      <c r="F161" s="64" t="s">
-        <v>1538</v>
       </c>
       <c r="G161" s="64" t="s">
         <v>1051</v>
@@ -16927,7 +16922,7 @@
         <v>810</v>
       </c>
       <c r="E162" s="64" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F162" s="64" t="s">
         <v>19</v>
@@ -16955,10 +16950,10 @@
         <v>810</v>
       </c>
       <c r="E163" s="64" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F163" s="64" t="s">
         <v>1547</v>
-      </c>
-      <c r="F163" s="64" t="s">
-        <v>1548</v>
       </c>
       <c r="G163" s="64" t="s">
         <v>1052</v>
@@ -16985,10 +16980,10 @@
         <v>810</v>
       </c>
       <c r="E164" s="64" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F164" s="64" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="G164" s="64" t="s">
         <v>1052</v>
@@ -17015,10 +17010,10 @@
         <v>810</v>
       </c>
       <c r="E165" s="64" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F165" s="64" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="G165" s="64" t="s">
         <v>1052</v>
@@ -17045,10 +17040,10 @@
         <v>810</v>
       </c>
       <c r="E166" s="64" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F166" s="64" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G166" s="64" t="s">
         <v>1052</v>
@@ -17073,10 +17068,10 @@
         <v>1408</v>
       </c>
       <c r="E167" s="129" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F167" s="64" t="s">
         <v>1539</v>
-      </c>
-      <c r="F167" s="64" t="s">
-        <v>1540</v>
       </c>
       <c r="G167" s="64" t="s">
         <v>1051</v>
@@ -17098,10 +17093,10 @@
         <v>719</v>
       </c>
       <c r="D168" s="64" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E168" s="64" t="s">
         <v>1535</v>
-      </c>
-      <c r="E168" s="64" t="s">
-        <v>1536</v>
       </c>
       <c r="F168" s="64"/>
       <c r="G168" s="64" t="s">
@@ -17124,13 +17119,13 @@
         <v>719</v>
       </c>
       <c r="D169" s="69" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E169" s="9" t="s">
         <v>1584</v>
       </c>
-      <c r="E169" s="9" t="s">
+      <c r="F169" s="69" t="s">
         <v>1585</v>
-      </c>
-      <c r="F169" s="69" t="s">
-        <v>1586</v>
       </c>
       <c r="G169" s="64" t="s">
         <v>1062</v>
@@ -17155,7 +17150,7 @@
         <v>1381</v>
       </c>
       <c r="E170" s="64" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="F170" s="64"/>
       <c r="G170" s="64" t="s">
@@ -17195,7 +17190,7 @@
         <v>773</v>
       </c>
       <c r="K171" s="71" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
@@ -17204,10 +17199,10 @@
         <v>719</v>
       </c>
       <c r="D172" s="64" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E172" s="64" t="s">
         <v>1527</v>
-      </c>
-      <c r="E172" s="64" t="s">
-        <v>1528</v>
       </c>
       <c r="F172" s="64"/>
       <c r="G172" s="64" t="s">
@@ -17238,7 +17233,7 @@
         <v>1424</v>
       </c>
       <c r="F173" s="64" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="G173" s="64" t="s">
         <v>1066</v>
@@ -17318,10 +17313,10 @@
         <v>719</v>
       </c>
       <c r="D176" s="64" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E176" s="64" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="F176" s="64"/>
       <c r="G176" s="64" t="s">
@@ -17361,7 +17356,7 @@
         <v>708</v>
       </c>
       <c r="K177" s="71" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="178" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -17373,10 +17368,10 @@
         <v>143</v>
       </c>
       <c r="E178" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F178" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F178" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G178" s="64" t="s">
         <v>1053</v>
@@ -17401,10 +17396,10 @@
         <v>1149</v>
       </c>
       <c r="E179" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F179" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F179" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G179" s="64" t="s">
         <v>1053</v>
@@ -17429,10 +17424,10 @@
         <v>1149</v>
       </c>
       <c r="E180" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F180" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F180" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G180" s="64" t="s">
         <v>1047</v>
@@ -17445,7 +17440,7 @@
         <v>569</v>
       </c>
       <c r="K180" s="71" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="181" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -17457,10 +17452,10 @@
         <v>1149</v>
       </c>
       <c r="E181" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F181" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F181" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G181" s="64" t="s">
         <v>1053</v>
@@ -17485,10 +17480,10 @@
         <v>1149</v>
       </c>
       <c r="E182" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F182" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F182" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G182" s="64" t="s">
         <v>1053</v>
@@ -17501,7 +17496,7 @@
         <v>573</v>
       </c>
       <c r="K182" s="71" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="183" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -17513,10 +17508,10 @@
         <v>1149</v>
       </c>
       <c r="E183" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F183" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F183" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G183" s="64" t="s">
         <v>1053</v>
@@ -17541,10 +17536,10 @@
         <v>1149</v>
       </c>
       <c r="E184" s="64" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F184" s="64" t="s">
         <v>1553</v>
-      </c>
-      <c r="F184" s="64" t="s">
-        <v>1554</v>
       </c>
       <c r="G184" s="64" t="s">
         <v>1053</v>
@@ -17557,7 +17552,7 @@
         <v>718</v>
       </c>
       <c r="K184" s="71" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="185" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
@@ -17566,19 +17561,19 @@
         <v>60</v>
       </c>
       <c r="D185" s="9" t="s">
+        <v>1650</v>
+      </c>
+      <c r="E185" s="9" t="s">
         <v>1651</v>
       </c>
-      <c r="E185" s="9" t="s">
+      <c r="F185" s="9" t="s">
         <v>1652</v>
-      </c>
-      <c r="F185" s="9" t="s">
-        <v>1653</v>
       </c>
       <c r="G185" s="64" t="s">
         <v>1021</v>
       </c>
       <c r="H185" s="61" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="I185" s="61" t="s">
         <v>1097</v>
@@ -17587,7 +17582,7 @@
         <v>1096</v>
       </c>
       <c r="K185" s="71" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="186" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -17700,7 +17695,7 @@
         <v>719</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E190" s="63"/>
       <c r="F190" s="63"/>
@@ -17724,7 +17719,7 @@
         <v>719</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E191" s="67"/>
       <c r="F191" s="67"/>
@@ -17748,7 +17743,7 @@
         <v>719</v>
       </c>
       <c r="D192" s="64" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E192" s="64"/>
       <c r="F192" s="64"/>
@@ -17772,7 +17767,7 @@
         <v>719</v>
       </c>
       <c r="D193" s="64" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="E193" s="64"/>
       <c r="F193" s="64"/>
@@ -17796,7 +17791,7 @@
         <v>719</v>
       </c>
       <c r="D194" s="64" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="E194" s="64"/>
       <c r="F194" s="64"/>
@@ -17820,7 +17815,7 @@
         <v>719</v>
       </c>
       <c r="D195" s="64" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E195" s="64"/>
       <c r="F195" s="64"/>
@@ -17844,7 +17839,7 @@
         <v>719</v>
       </c>
       <c r="D196" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E196" s="64"/>
       <c r="F196" s="64"/>
@@ -17868,7 +17863,7 @@
         <v>719</v>
       </c>
       <c r="D197" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E197" s="64"/>
       <c r="F197" s="64"/>
@@ -17892,7 +17887,7 @@
         <v>719</v>
       </c>
       <c r="D198" s="64" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E198" s="64"/>
       <c r="F198" s="64"/>
@@ -17973,7 +17968,7 @@
     <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B201" s="9"/>
       <c r="C201" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D201" s="64"/>
       <c r="E201" s="9" t="s">
@@ -17997,7 +17992,7 @@
     <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B202" s="9"/>
       <c r="C202" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D202" s="64"/>
       <c r="E202" s="9" t="s">
@@ -18021,7 +18016,7 @@
     <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B203" s="9"/>
       <c r="C203" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D203" s="64"/>
       <c r="E203" s="9" t="s">
@@ -18045,7 +18040,7 @@
     <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B204" s="9"/>
       <c r="C204" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D204" s="64"/>
       <c r="E204" s="9" t="s">
@@ -18069,7 +18064,7 @@
     <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B205" s="9"/>
       <c r="C205" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D205" s="64"/>
       <c r="E205" s="9" t="s">
@@ -18093,7 +18088,7 @@
     <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="B206" s="9"/>
       <c r="C206" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D206" s="64"/>
       <c r="E206" s="9" t="s">
@@ -18117,7 +18112,7 @@
     <row r="207" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B207" s="72"/>
       <c r="C207" s="87" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D207" s="87"/>
       <c r="E207" s="72" t="s">
@@ -18141,7 +18136,7 @@
     <row r="208" spans="2:11" s="25" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B208" s="9"/>
       <c r="C208" s="64" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D208" s="64"/>
       <c r="E208" s="9"/>
@@ -18149,7 +18144,7 @@
         <v>1499</v>
       </c>
       <c r="G208" s="64" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="H208" s="9"/>
       <c r="I208" s="9" t="s">

</xml_diff>

<commit_message>
sIksha and new docs 21/06/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -6267,7 +6267,7 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="I64" sqref="I64"/>
@@ -12576,11 +12576,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="J50" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
TS 7 PP files and Jatai working 03/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -6277,7 +6277,7 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="K105" sqref="K105"/>
@@ -12586,11 +12586,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="K110" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="E102" sqref="E102"/>
+      <selection pane="bottomRight" activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai Working files 17/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -12586,11 +12586,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="K113" sqref="K113"/>
+      <selection pane="bottomRight" activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai file changes 20/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -12586,11 +12586,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="K99" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="E146" sqref="E146"/>
+      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Jatai Working edits 29/07/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5208" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -5352,13 +5352,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -5698,300 +5704,300 @@
   </cellStyleXfs>
   <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6276,29 +6282,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G102" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="G112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K105" sqref="K105"/>
+      <selection pane="bottomRight" activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="81.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="81.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="20.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6315,7 +6321,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="45.75">
       <c r="A3" s="1"/>
       <c r="B3" s="18" t="s">
         <v>1</v>
@@ -6355,7 +6361,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>131</v>
@@ -6391,7 +6397,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>131</v>
@@ -6427,7 +6433,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>131</v>
@@ -6463,7 +6469,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
         <v>148</v>
@@ -6501,7 +6507,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>148</v>
@@ -6539,7 +6545,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>148</v>
@@ -6577,7 +6583,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>148</v>
@@ -6613,7 +6619,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>148</v>
@@ -6651,7 +6657,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>148</v>
@@ -6691,7 +6697,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>148</v>
@@ -6729,7 +6735,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>148</v>
@@ -6767,7 +6773,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>148</v>
@@ -6793,7 +6799,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>148</v>
@@ -6829,7 +6835,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>148</v>
@@ -6865,7 +6871,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>148</v>
@@ -6901,7 +6907,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -6937,7 +6943,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>148</v>
@@ -6973,7 +6979,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="30.75">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
         <v>148</v>
@@ -7009,7 +7015,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="18">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
         <v>148</v>
@@ -7045,7 +7051,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30.75">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="s">
         <v>148</v>
@@ -7081,7 +7087,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="30.75">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>148</v>
@@ -7117,7 +7123,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="60.75">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>148</v>
@@ -7155,7 +7161,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="30.75">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
         <v>148</v>
@@ -7193,7 +7199,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="30.75">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
         <v>148</v>
@@ -7231,7 +7237,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="30.75">
       <c r="A28" s="1"/>
       <c r="B28" s="9" t="s">
         <v>148</v>
@@ -7269,7 +7275,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="45.75">
       <c r="A29" s="1"/>
       <c r="B29" s="9" t="s">
         <v>148</v>
@@ -7305,7 +7311,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="18">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>148</v>
@@ -7341,7 +7347,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="18">
       <c r="A31" s="1"/>
       <c r="B31" s="9" t="s">
         <v>148</v>
@@ -7379,7 +7385,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="18">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>148</v>
@@ -7417,7 +7423,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="45.75">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
         <v>148</v>
@@ -7453,7 +7459,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="75.75">
       <c r="A34" s="1"/>
       <c r="B34" s="9" t="s">
         <v>148</v>
@@ -7489,7 +7495,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="18">
       <c r="A35" s="1"/>
       <c r="B35" s="9" t="s">
         <v>148</v>
@@ -7527,7 +7533,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30.75">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
         <v>148</v>
@@ -7565,7 +7571,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="30.75">
       <c r="A37" s="1"/>
       <c r="B37" s="9" t="s">
         <v>148</v>
@@ -7601,7 +7607,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="45.75">
       <c r="A38" s="1"/>
       <c r="B38" s="9" t="s">
         <v>148</v>
@@ -7637,7 +7643,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="60.75">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
         <v>148</v>
@@ -7675,7 +7681,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="45.75">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
         <v>148</v>
@@ -7711,7 +7717,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="36">
       <c r="A41" s="1"/>
       <c r="B41" s="9" t="s">
         <v>148</v>
@@ -7747,7 +7753,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="18">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>148</v>
@@ -7783,7 +7789,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="30.75">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
         <v>148</v>
@@ -7819,7 +7825,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="18">
       <c r="A44" s="1"/>
       <c r="B44" s="9" t="s">
         <v>148</v>
@@ -7855,7 +7861,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="18">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
         <v>148</v>
@@ -7891,7 +7897,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="18">
       <c r="A46" s="1"/>
       <c r="B46" s="9" t="s">
         <v>148</v>
@@ -7925,7 +7931,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="18">
       <c r="A47" s="1"/>
       <c r="B47" s="9" t="s">
         <v>148</v>
@@ -7963,7 +7969,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="30.75">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
         <v>148</v>
@@ -7999,7 +8005,7 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="18">
       <c r="A49" s="1"/>
       <c r="B49" s="9" t="s">
         <v>148</v>
@@ -8035,7 +8041,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="30.75">
       <c r="A50" s="1"/>
       <c r="B50" s="9" t="s">
         <v>148</v>
@@ -8071,7 +8077,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="18">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
         <v>148</v>
@@ -8109,7 +8115,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="18">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>148</v>
@@ -8147,7 +8153,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="60.75">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
         <v>148</v>
@@ -8185,7 +8191,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="36">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
         <v>148</v>
@@ -8223,7 +8229,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="18">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
         <v>148</v>
@@ -8261,7 +8267,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30.75">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
         <v>791</v>
@@ -8299,7 +8305,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="18">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
         <v>791</v>
@@ -8333,7 +8339,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="30.75">
       <c r="A58" s="1"/>
       <c r="B58" s="9" t="s">
         <v>791</v>
@@ -8371,7 +8377,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="18">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
         <v>791</v>
@@ -8409,7 +8415,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="18">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
         <v>791</v>
@@ -8447,7 +8453,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="18">
       <c r="A61" s="1"/>
       <c r="B61" s="9" t="s">
         <v>791</v>
@@ -8485,7 +8491,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="18">
       <c r="A62" s="1"/>
       <c r="B62" s="8" t="s">
         <v>791</v>
@@ -8519,7 +8525,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="18">
       <c r="A63" s="1"/>
       <c r="B63" s="137" t="s">
         <v>15</v>
@@ -8555,7 +8561,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="18">
       <c r="A64" s="1"/>
       <c r="B64" s="137" t="s">
         <v>15</v>
@@ -8591,7 +8597,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="18">
       <c r="A65" s="1"/>
       <c r="B65" s="137" t="s">
         <v>15</v>
@@ -8627,7 +8633,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" ht="18">
       <c r="A66" s="1"/>
       <c r="B66" s="137" t="s">
         <v>15</v>
@@ -8661,7 +8667,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="30.75">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
         <v>98</v>
@@ -8697,7 +8703,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="60.75">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
         <v>98</v>
@@ -8735,7 +8741,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="30.75">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
         <v>98</v>
@@ -8773,7 +8779,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="30.75">
       <c r="A70" s="1"/>
       <c r="B70" s="9" t="s">
         <v>98</v>
@@ -8809,7 +8815,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="18">
       <c r="A71" s="1"/>
       <c r="B71" s="9" t="s">
         <v>98</v>
@@ -8849,7 +8855,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="18">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
         <v>98</v>
@@ -8887,7 +8893,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="30.75">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
         <v>98</v>
@@ -8925,7 +8931,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" ht="36" x14ac:dyDescent="0.9">
+    <row r="74" spans="1:18" ht="27">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
         <v>1339</v>
@@ -8963,7 +8969,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" ht="30.75">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
         <v>1339</v>
@@ -9001,7 +9007,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" ht="18">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
         <v>1339</v>
@@ -9037,7 +9043,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" ht="30.75">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
         <v>1339</v>
@@ -9075,7 +9081,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="30.75">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
         <v>1339</v>
@@ -9113,7 +9119,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="30.75">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
         <v>139</v>
@@ -9151,7 +9157,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="18">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
         <v>139</v>
@@ -9189,7 +9195,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="18">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
         <v>139</v>
@@ -9227,7 +9233,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="30.75">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
         <v>139</v>
@@ -9265,7 +9271,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="18">
       <c r="A83" s="1"/>
       <c r="B83" s="9" t="s">
         <v>1318</v>
@@ -9303,7 +9309,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="36">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
         <v>1318</v>
@@ -9341,7 +9347,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="18">
       <c r="A85" s="1"/>
       <c r="B85" s="9" t="s">
         <v>1318</v>
@@ -9381,7 +9387,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="30.75">
       <c r="A86" s="1"/>
       <c r="B86" s="9" t="s">
         <v>1318</v>
@@ -9419,7 +9425,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="30.75">
       <c r="A87" s="1"/>
       <c r="B87" s="9" t="s">
         <v>1318</v>
@@ -9455,7 +9461,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="18">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
         <v>1318</v>
@@ -9491,7 +9497,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="30.75">
       <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
         <v>7</v>
@@ -9527,7 +9533,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="30.75">
       <c r="A90" s="1"/>
       <c r="B90" s="9" t="s">
         <v>7</v>
@@ -9563,7 +9569,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="30.75">
       <c r="A91" s="1"/>
       <c r="B91" s="9" t="s">
         <v>7</v>
@@ -9599,7 +9605,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="30.75">
       <c r="A92" s="1"/>
       <c r="B92" s="9" t="s">
         <v>7</v>
@@ -9635,7 +9641,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="18">
       <c r="A93" s="1"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
@@ -9671,7 +9677,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="18">
       <c r="A94" s="1"/>
       <c r="B94" s="8" t="s">
         <v>7</v>
@@ -9709,7 +9715,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="18">
       <c r="A95" s="1"/>
       <c r="B95" s="8" t="s">
         <v>7</v>
@@ -9745,7 +9751,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="30.75">
       <c r="A96" s="1"/>
       <c r="B96" s="9" t="s">
         <v>7</v>
@@ -9783,7 +9789,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="18">
       <c r="A97" s="1"/>
       <c r="B97" s="9" t="s">
         <v>7</v>
@@ -9819,7 +9825,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="18">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9857,7 +9863,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="18">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
         <v>7</v>
@@ -9895,7 +9901,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="30.75">
       <c r="A100" s="1"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
@@ -9931,7 +9937,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="30.75">
       <c r="A101" s="1"/>
       <c r="B101" s="9" t="s">
         <v>7</v>
@@ -9971,7 +9977,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="18">
       <c r="A102" s="1"/>
       <c r="B102" s="9" t="s">
         <v>7</v>
@@ -10009,7 +10015,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="30.75">
       <c r="A103" s="1"/>
       <c r="B103" s="9" t="s">
         <v>7</v>
@@ -10047,7 +10053,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="45.75">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
         <v>7</v>
@@ -10085,7 +10091,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="30.75">
       <c r="A105" s="1"/>
       <c r="B105" s="9" t="s">
         <v>7</v>
@@ -10123,7 +10129,7 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="36">
       <c r="A106" s="1"/>
       <c r="B106" s="9" t="s">
         <v>7</v>
@@ -10161,7 +10167,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="18">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10199,7 +10205,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="18">
       <c r="A108" s="1" t="s">
         <v>1169</v>
       </c>
@@ -10237,7 +10243,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18" ht="18.75" thickBot="1">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
         <v>7</v>
@@ -10273,7 +10279,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18" ht="31.5" thickBot="1">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
         <v>7</v>
@@ -10311,7 +10317,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:18" ht="31.5" thickBot="1">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
         <v>7</v>
@@ -10347,7 +10353,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18" ht="18.75" thickBot="1">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
         <v>7</v>
@@ -10385,7 +10391,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:18" ht="18.75" thickBot="1">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
         <v>7</v>
@@ -10425,7 +10431,7 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" ht="30.75">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
         <v>7</v>
@@ -10465,7 +10471,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="18">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>7</v>
@@ -10503,7 +10509,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" ht="18">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
         <v>7</v>
@@ -10539,7 +10545,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="18">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
         <v>7</v>
@@ -10575,7 +10581,7 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" ht="18">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
         <v>19</v>
@@ -10615,7 +10621,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" ht="18">
       <c r="A119" s="1"/>
       <c r="B119" s="63" t="s">
         <v>19</v>
@@ -10653,7 +10659,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" ht="18">
       <c r="A120" s="1"/>
       <c r="B120" s="63" t="s">
         <v>19</v>
@@ -10687,7 +10693,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" ht="18">
       <c r="A121" s="1"/>
       <c r="B121" s="63" t="s">
         <v>19</v>
@@ -10721,7 +10727,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:18" ht="18.75" thickBot="1">
       <c r="A122" s="1"/>
       <c r="B122" s="63" t="s">
         <v>19</v>
@@ -10755,7 +10761,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:18" ht="18.75" thickBot="1">
       <c r="A123" s="1"/>
       <c r="B123" s="63" t="s">
         <v>19</v>
@@ -10789,7 +10795,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:18" ht="18.75" thickBot="1">
       <c r="A124" s="1"/>
       <c r="B124" s="63" t="s">
         <v>19</v>
@@ -10823,7 +10829,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:18" ht="31.5" thickBot="1">
       <c r="A125" s="1"/>
       <c r="B125" s="63" t="s">
         <v>19</v>
@@ -10857,7 +10863,7 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:18" ht="31.5" thickBot="1">
       <c r="A126" s="1"/>
       <c r="B126" s="63" t="s">
         <v>19</v>
@@ -10891,7 +10897,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:18" ht="18.75" thickBot="1">
       <c r="A127" s="1"/>
       <c r="B127" s="63" t="s">
         <v>19</v>
@@ -10925,7 +10931,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:18" ht="18.75" thickBot="1">
       <c r="A128" s="1"/>
       <c r="B128" s="63" t="s">
         <v>19</v>
@@ -10959,7 +10965,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" ht="31.5" thickBot="1">
       <c r="A129" s="1"/>
       <c r="B129" s="63" t="s">
         <v>19</v>
@@ -10993,7 +10999,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" ht="30.75">
       <c r="A130" s="1"/>
       <c r="B130" s="9" t="s">
         <v>19</v>
@@ -11029,7 +11035,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" ht="18">
       <c r="A131" s="1"/>
       <c r="B131" s="9" t="s">
         <v>19</v>
@@ -11065,7 +11071,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" ht="18">
       <c r="A132" s="1"/>
       <c r="B132" s="9" t="s">
         <v>19</v>
@@ -11099,7 +11105,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" ht="18">
       <c r="A133" s="1"/>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -11133,7 +11139,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" ht="30.75">
       <c r="A134" s="1"/>
       <c r="B134" s="9" t="s">
         <v>19</v>
@@ -11167,7 +11173,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" ht="18">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
         <v>19</v>
@@ -11201,7 +11207,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" ht="18">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
         <v>19</v>
@@ -11235,7 +11241,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" ht="18">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
         <v>19</v>
@@ -11269,7 +11275,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" ht="18">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11303,7 +11309,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" ht="18.75" thickBot="1">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
         <v>19</v>
@@ -11337,7 +11343,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" ht="18.75" thickBot="1">
       <c r="A140" s="1"/>
       <c r="B140" s="9" t="s">
         <v>19</v>
@@ -11373,7 +11379,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" ht="18">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
         <v>19</v>
@@ -11409,7 +11415,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" ht="18">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
         <v>19</v>
@@ -11445,7 +11451,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" ht="18">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
         <v>19</v>
@@ -11481,7 +11487,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" ht="18">
       <c r="A144" s="1"/>
       <c r="B144" s="9" t="s">
         <v>19</v>
@@ -11515,7 +11521,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" ht="18">
       <c r="A145" s="1"/>
       <c r="B145" s="8" t="s">
         <v>60</v>
@@ -11553,7 +11559,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" ht="30.75">
       <c r="A146" s="1"/>
       <c r="B146" s="8" t="s">
         <v>60</v>
@@ -11591,7 +11597,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" ht="30.75">
       <c r="A147" s="1"/>
       <c r="B147" s="8" t="s">
         <v>60</v>
@@ -11629,7 +11635,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:18" ht="18.75" thickBot="1">
       <c r="A148" s="1"/>
       <c r="B148" s="9" t="s">
         <v>60</v>
@@ -11667,7 +11673,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:18" ht="31.5" thickBot="1">
       <c r="A149" s="1"/>
       <c r="B149" s="9" t="s">
         <v>60</v>
@@ -11704,7 +11710,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:18" ht="18.75" thickBot="1">
       <c r="A150" s="1"/>
       <c r="B150" s="9" t="s">
         <v>60</v>
@@ -11741,7 +11747,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" ht="30.75">
       <c r="A151" s="1"/>
       <c r="B151" s="9" t="s">
         <v>60</v>
@@ -11776,7 +11782,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" ht="30.75">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11807,7 +11813,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" ht="18">
       <c r="A153" s="1"/>
       <c r="B153" s="8" t="s">
         <v>60</v>
@@ -11842,7 +11848,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:18" ht="18">
       <c r="A154" s="1"/>
       <c r="B154" s="8" t="s">
         <v>60</v>
@@ -11877,7 +11883,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:18" ht="30.75">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
         <v>60</v>
@@ -11914,7 +11920,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" ht="18">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
         <v>60</v>
@@ -11951,7 +11957,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:18" ht="30.75">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
         <v>719</v>
@@ -11986,7 +11992,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:18" ht="30.6" customHeight="1">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>719</v>
@@ -12021,7 +12027,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:18" ht="30.75">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
         <v>719</v>
@@ -12056,7 +12062,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:18" ht="18.75" thickBot="1">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>719</v>
@@ -12093,7 +12099,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:18" ht="36.75" thickBot="1">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
         <v>719</v>
@@ -12130,7 +12136,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:18" ht="46.5" thickBot="1">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
         <v>719</v>
@@ -12165,7 +12171,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:18" ht="18.75" thickBot="1">
       <c r="A163" s="1"/>
       <c r="B163" s="8" t="s">
         <v>719</v>
@@ -12198,7 +12204,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:18" ht="18.75" thickBot="1">
       <c r="A164" s="1"/>
       <c r="B164" s="8" t="s">
         <v>719</v>
@@ -12231,7 +12237,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:18" ht="18.75" thickBot="1">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
         <v>719</v>
@@ -12264,7 +12270,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:18" ht="31.5" thickBot="1">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
         <v>719</v>
@@ -12299,7 +12305,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:18" ht="31.5" thickBot="1">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
         <v>719</v>
@@ -12328,7 +12334,7 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:18" ht="18.75" thickBot="1">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
         <v>719</v>
@@ -12363,7 +12369,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:18" ht="31.5" thickBot="1">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
         <v>719</v>
@@ -12398,7 +12404,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:18" ht="18.75" thickBot="1">
       <c r="A170" s="1"/>
       <c r="B170" s="9" t="s">
         <v>719</v>
@@ -12434,7 +12440,7 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:18" ht="46.5" thickBot="1">
       <c r="A171" s="1"/>
       <c r="B171" s="9" t="s">
         <v>719</v>
@@ -12470,7 +12476,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:18" ht="18">
       <c r="A172" s="1"/>
       <c r="B172" s="9" t="s">
         <v>719</v>
@@ -12506,7 +12512,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" s="24" customFormat="1" ht="18">
       <c r="B173" s="70" t="s">
         <v>719</v>
       </c>
@@ -12534,7 +12540,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="174" spans="1:18" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:18" s="24" customFormat="1" ht="18">
       <c r="B174" s="70"/>
       <c r="C174" s="9"/>
       <c r="D174" s="69"/>
@@ -12546,7 +12552,7 @@
       <c r="J174" s="9"/>
       <c r="K174" s="11"/>
     </row>
-    <row r="175" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:18" ht="18.75">
       <c r="B175" s="72"/>
       <c r="C175" s="72"/>
       <c r="D175" s="72"/>
@@ -12558,7 +12564,7 @@
       <c r="J175" s="72"/>
       <c r="K175" s="73"/>
     </row>
-    <row r="176" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:18" ht="18.75">
       <c r="B176" s="72"/>
       <c r="C176" s="72"/>
       <c r="D176" s="72"/>
@@ -12585,28 +12591,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K99" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="77.88671875" style="130" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="77.85546875" style="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" ht="20.25">
       <c r="B2" s="2" t="s">
         <v>775</v>
       </c>
@@ -12619,7 +12625,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="4" spans="2:11" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="45.75">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -12651,7 +12657,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="27" customHeight="1">
       <c r="B5" s="9"/>
       <c r="C5" s="61" t="s">
         <v>131</v>
@@ -12677,7 +12683,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:11" ht="26.25">
       <c r="B6" s="9"/>
       <c r="C6" s="61" t="s">
         <v>131</v>
@@ -12703,7 +12709,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="30">
       <c r="B7" s="9"/>
       <c r="C7" s="61" t="s">
         <v>131</v>
@@ -12731,7 +12737,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="30">
       <c r="B8" s="9"/>
       <c r="C8" s="61" t="s">
         <v>131</v>
@@ -12755,7 +12761,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="30">
       <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
@@ -12785,7 +12791,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="30">
       <c r="B10" s="9"/>
       <c r="C10" s="61" t="s">
         <v>148</v>
@@ -12813,7 +12819,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="30.75">
       <c r="B11" s="9"/>
       <c r="C11" s="61" t="s">
         <v>148</v>
@@ -12841,7 +12847,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="18">
       <c r="B12" s="9"/>
       <c r="C12" s="61" t="s">
         <v>148</v>
@@ -12869,7 +12875,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="45.75">
       <c r="B13" s="9"/>
       <c r="C13" s="61" t="s">
         <v>148</v>
@@ -12899,7 +12905,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="20.45" customHeight="1">
       <c r="B14" s="9" t="s">
         <v>148</v>
       </c>
@@ -12929,7 +12935,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="30">
       <c r="B15" s="9" t="s">
         <v>148</v>
       </c>
@@ -12959,7 +12965,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:11" ht="26.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -12987,7 +12993,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="30.75">
       <c r="B17" s="9"/>
       <c r="C17" s="61" t="s">
         <v>148</v>
@@ -13015,7 +13021,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="18">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -13043,7 +13049,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="30">
       <c r="B19" s="9" t="s">
         <v>148</v>
       </c>
@@ -13073,7 +13079,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:11" ht="26.25">
       <c r="B20" s="25"/>
       <c r="C20" s="66" t="s">
         <v>148</v>
@@ -13099,7 +13105,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="30">
       <c r="B21" s="9"/>
       <c r="C21" s="61" t="s">
         <v>148</v>
@@ -13127,7 +13133,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="30">
       <c r="B22" s="9" t="s">
         <v>148</v>
       </c>
@@ -13157,7 +13163,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="30">
       <c r="B23" s="9"/>
       <c r="C23" s="61" t="s">
         <v>148</v>
@@ -13185,7 +13191,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="18">
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
         <v>148</v>
@@ -13213,7 +13219,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="30">
       <c r="B25" s="9" t="s">
         <v>148</v>
       </c>
@@ -13243,7 +13249,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="30">
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
         <v>148</v>
@@ -13271,7 +13277,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" ht="30.75">
       <c r="B27" s="15"/>
       <c r="C27" s="62" t="s">
         <v>148</v>
@@ -13301,7 +13307,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" ht="30.75">
       <c r="B28" s="15"/>
       <c r="C28" s="62" t="s">
         <v>148</v>
@@ -13331,7 +13337,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="18">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>148</v>
@@ -13355,7 +13361,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" ht="30">
       <c r="B30" s="15"/>
       <c r="C30" s="62" t="s">
         <v>1628</v>
@@ -13381,7 +13387,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" ht="30">
       <c r="B31" s="15"/>
       <c r="C31" s="62" t="s">
         <v>1628</v>
@@ -13405,7 +13411,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" ht="18">
       <c r="B32" s="15"/>
       <c r="C32" s="61" t="s">
         <v>1628</v>
@@ -13433,7 +13439,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" ht="30">
       <c r="B33" s="15"/>
       <c r="C33" s="61" t="s">
         <v>1628</v>
@@ -13457,7 +13463,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="18">
       <c r="B34" s="15"/>
       <c r="C34" s="61" t="s">
         <v>1628</v>
@@ -13481,7 +13487,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" ht="30">
       <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>791</v>
@@ -13509,7 +13515,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="30">
       <c r="B36" s="15" t="s">
         <v>1465</v>
       </c>
@@ -13539,7 +13545,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="30">
       <c r="B37" s="9"/>
       <c r="C37" s="61" t="s">
         <v>791</v>
@@ -13567,7 +13573,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" ht="18">
       <c r="B38" s="9"/>
       <c r="C38" s="66" t="s">
         <v>791</v>
@@ -13593,7 +13599,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" ht="18">
       <c r="B39" s="9"/>
       <c r="C39" s="66" t="s">
         <v>791</v>
@@ -13619,7 +13625,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" ht="18">
       <c r="B40" s="9"/>
       <c r="C40" s="61" t="s">
         <v>791</v>
@@ -13647,7 +13653,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" ht="30">
       <c r="B41" s="9" t="s">
         <v>791</v>
       </c>
@@ -13675,7 +13681,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:11" ht="26.25">
       <c r="B42" s="9"/>
       <c r="C42" s="61" t="s">
         <v>791</v>
@@ -13699,7 +13705,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:11" ht="26.25">
       <c r="B43" s="9"/>
       <c r="C43" s="61" t="s">
         <v>791</v>
@@ -13723,7 +13729,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" ht="18">
       <c r="B44" s="9"/>
       <c r="C44" s="61" t="s">
         <v>1385</v>
@@ -13749,7 +13755,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" ht="18">
       <c r="B45" s="9"/>
       <c r="C45" s="61" t="s">
         <v>1385</v>
@@ -13777,7 +13783,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" ht="18">
       <c r="B46" s="9"/>
       <c r="C46" s="61" t="s">
         <v>1385</v>
@@ -13805,7 +13811,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" ht="30">
       <c r="B47" s="9"/>
       <c r="C47" s="61" t="s">
         <v>1385</v>
@@ -13831,7 +13837,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" ht="30">
       <c r="B48" s="8" t="s">
         <v>15</v>
       </c>
@@ -13861,7 +13867,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B49" s="8" t="s">
         <v>15</v>
       </c>
@@ -13891,7 +13897,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
@@ -13921,7 +13927,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B51" s="8" t="s">
         <v>15</v>
       </c>
@@ -13951,7 +13957,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B52" s="8" t="s">
         <v>15</v>
       </c>
@@ -13981,7 +13987,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B53" s="8" t="s">
         <v>15</v>
       </c>
@@ -14011,7 +14017,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B54" s="9" t="s">
         <v>15</v>
       </c>
@@ -14039,7 +14045,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
@@ -14067,7 +14073,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="24" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25">
       <c r="B56" s="9" t="s">
         <v>15</v>
       </c>
@@ -14095,7 +14101,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B57" s="9"/>
       <c r="C57" s="61" t="s">
         <v>1135</v>
@@ -14119,7 +14125,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B58" s="9"/>
       <c r="C58" s="61" t="s">
         <v>1135</v>
@@ -14143,7 +14149,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B59" s="9"/>
       <c r="C59" s="61" t="s">
         <v>1135</v>
@@ -14167,7 +14173,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B60" s="9"/>
       <c r="C60" s="61" t="s">
         <v>1135</v>
@@ -14191,7 +14197,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B61" s="9"/>
       <c r="C61" s="61" t="s">
         <v>1135</v>
@@ -14215,7 +14221,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B62" s="9"/>
       <c r="C62" s="61" t="s">
         <v>1135</v>
@@ -14241,7 +14247,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B63" s="9"/>
       <c r="C63" s="61" t="s">
         <v>1135</v>
@@ -14267,7 +14273,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B64" s="9"/>
       <c r="C64" s="61" t="s">
         <v>1135</v>
@@ -14291,7 +14297,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" ht="30">
       <c r="B65" s="9"/>
       <c r="C65" s="61" t="s">
         <v>1135</v>
@@ -14319,7 +14325,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" ht="18">
       <c r="B66" s="9"/>
       <c r="C66" s="61" t="s">
         <v>1135</v>
@@ -14345,7 +14351,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" ht="45">
       <c r="B67" s="9"/>
       <c r="C67" s="61" t="s">
         <v>1384</v>
@@ -14373,7 +14379,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="68" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" ht="45">
       <c r="B68" s="9"/>
       <c r="C68" s="61" t="s">
         <v>1339</v>
@@ -14401,7 +14407,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" ht="30">
       <c r="B69" s="25"/>
       <c r="C69" s="61" t="s">
         <v>1339</v>
@@ -14427,7 +14433,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" ht="30">
       <c r="B70" s="25"/>
       <c r="C70" s="9" t="s">
         <v>1339</v>
@@ -14455,7 +14461,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" ht="30">
       <c r="B71" s="9"/>
       <c r="C71" s="61" t="s">
         <v>1339</v>
@@ -14481,7 +14487,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" ht="30">
       <c r="B72" s="25"/>
       <c r="C72" s="60" t="s">
         <v>1339</v>
@@ -14509,7 +14515,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B73" s="9"/>
       <c r="C73" s="61" t="s">
         <v>139</v>
@@ -14537,7 +14543,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" ht="30">
       <c r="B74" s="9"/>
       <c r="C74" s="61" t="s">
         <v>139</v>
@@ -14565,7 +14571,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" ht="18">
       <c r="B75" s="9" t="s">
         <v>139</v>
       </c>
@@ -14595,7 +14601,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" ht="18">
       <c r="B76" s="9" t="s">
         <v>139</v>
       </c>
@@ -14623,7 +14629,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" ht="30">
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
         <v>1318</v>
@@ -14651,7 +14657,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" ht="30">
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
         <v>1318</v>
@@ -14679,7 +14685,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" ht="18">
       <c r="B79" s="9"/>
       <c r="C79" s="61" t="s">
         <v>1318</v>
@@ -14707,7 +14713,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" ht="30">
       <c r="B80" s="9"/>
       <c r="C80" s="61" t="s">
         <v>1625</v>
@@ -14733,7 +14739,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:11" ht="30">
       <c r="B81" s="9"/>
       <c r="C81" s="61" t="s">
         <v>1625</v>
@@ -14759,7 +14765,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:11" ht="30">
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -14787,7 +14793,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:11" ht="45">
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -14815,7 +14821,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:11" ht="18">
       <c r="B84" s="25"/>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -14843,7 +14849,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:11" ht="30">
       <c r="B85" s="9"/>
       <c r="C85" s="66" t="s">
         <v>7</v>
@@ -14869,7 +14875,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:11" ht="30">
       <c r="B86" s="9"/>
       <c r="C86" s="61" t="s">
         <v>7</v>
@@ -14895,7 +14901,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:11" ht="18">
       <c r="B87" s="9"/>
       <c r="C87" s="61" t="s">
         <v>7</v>
@@ -14921,7 +14927,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:11" ht="30">
       <c r="B88" s="9"/>
       <c r="C88" s="61" t="s">
         <v>7</v>
@@ -14947,7 +14953,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:11" ht="30">
       <c r="B89" s="9" t="s">
         <v>60</v>
       </c>
@@ -14977,7 +14983,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:11" ht="30">
       <c r="B90" s="9"/>
       <c r="C90" s="61" t="s">
         <v>7</v>
@@ -15003,7 +15009,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="91" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:11" ht="30">
       <c r="B91" s="9"/>
       <c r="C91" s="61" t="s">
         <v>7</v>
@@ -15031,7 +15037,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="92" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:11" ht="30">
       <c r="B92" s="9"/>
       <c r="C92" s="61" t="s">
         <v>7</v>
@@ -15057,7 +15063,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:11" ht="18">
       <c r="B93" s="9"/>
       <c r="C93" s="61" t="s">
         <v>7</v>
@@ -15083,7 +15089,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:11" ht="18">
       <c r="B94" s="25"/>
       <c r="C94" s="9" t="s">
         <v>7</v>
@@ -15111,7 +15117,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="95" spans="2:11" ht="45" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:11" ht="45">
       <c r="B95" s="9"/>
       <c r="C95" s="61" t="s">
         <v>7</v>
@@ -15137,7 +15143,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="96" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:11" ht="18">
       <c r="B96" s="25" t="s">
         <v>712</v>
       </c>
@@ -15167,7 +15173,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:11" ht="18">
       <c r="B97" s="9" t="s">
         <v>148</v>
       </c>
@@ -15195,7 +15201,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:11" ht="30">
       <c r="B98" s="9" t="s">
         <v>19</v>
       </c>
@@ -15223,7 +15229,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:11" ht="18">
       <c r="B99" s="9" t="s">
         <v>712</v>
       </c>
@@ -15251,7 +15257,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:11" ht="18">
       <c r="B100" s="25"/>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -15279,7 +15285,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:11" ht="18">
       <c r="B101" s="25"/>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -15305,7 +15311,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:11" ht="30">
       <c r="B102" s="25"/>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -15331,7 +15337,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:11" ht="18">
       <c r="B103" s="25" t="s">
         <v>712</v>
       </c>
@@ -15361,7 +15367,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="104" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:11" ht="18">
       <c r="B104" s="25" t="s">
         <v>712</v>
       </c>
@@ -15389,7 +15395,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B105" s="9" t="s">
         <v>713</v>
       </c>
@@ -15419,7 +15425,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B106" s="9" t="s">
         <v>148</v>
       </c>
@@ -15445,7 +15451,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15473,7 +15479,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B108" s="9"/>
       <c r="C108" s="61" t="s">
         <v>7</v>
@@ -15497,7 +15503,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B109" s="9"/>
       <c r="C109" s="61" t="s">
         <v>7</v>
@@ -15521,7 +15527,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B110" s="9"/>
       <c r="C110" s="61" t="s">
         <v>7</v>
@@ -15545,7 +15551,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B111" s="9"/>
       <c r="C111" s="9" t="s">
         <v>1263</v>
@@ -15573,7 +15579,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
         <v>1263</v>
@@ -15601,7 +15607,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="113" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B113" s="25"/>
       <c r="C113" s="9" t="s">
         <v>1263</v>
@@ -15629,7 +15635,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B114" s="9"/>
       <c r="C114" s="61" t="s">
         <v>1554</v>
@@ -15655,7 +15661,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B115" s="9"/>
       <c r="C115" s="61" t="s">
         <v>1554</v>
@@ -15683,7 +15689,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B116" s="9"/>
       <c r="C116" s="61" t="s">
         <v>1554</v>
@@ -15709,7 +15715,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="117" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B117" s="9"/>
       <c r="C117" s="61" t="s">
         <v>1554</v>
@@ -15735,7 +15741,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="118" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B118" s="9"/>
       <c r="C118" s="61" t="s">
         <v>1554</v>
@@ -15761,7 +15767,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="119" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B119" s="9"/>
       <c r="C119" s="61" t="s">
         <v>1554</v>
@@ -15787,7 +15793,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B120" s="9"/>
       <c r="C120" s="61" t="s">
         <v>1554</v>
@@ -15813,7 +15819,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B121" s="9"/>
       <c r="C121" s="61" t="s">
         <v>1554</v>
@@ -15839,7 +15845,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="122" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B122" s="9"/>
       <c r="C122" s="61" t="s">
         <v>1554</v>
@@ -15865,7 +15871,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:11" s="1" customFormat="1" ht="60">
       <c r="B123" s="9"/>
       <c r="C123" s="61" t="s">
         <v>1554</v>
@@ -15891,7 +15897,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B124" s="9"/>
       <c r="C124" s="61" t="s">
         <v>1554</v>
@@ -15917,7 +15923,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="125" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B125" s="9"/>
       <c r="C125" s="61" t="s">
         <v>1554</v>
@@ -15943,7 +15949,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="126" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B126" s="9"/>
       <c r="C126" s="61" t="s">
         <v>1554</v>
@@ -15971,7 +15977,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="127" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B127" s="9"/>
       <c r="C127" s="61" t="s">
         <v>1554</v>
@@ -15999,7 +16005,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="128" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B128" s="9"/>
       <c r="C128" s="61" t="s">
         <v>1554</v>
@@ -16023,7 +16029,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B129" s="58"/>
       <c r="C129" s="61" t="s">
         <v>1554</v>
@@ -16049,7 +16055,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B130" s="9"/>
       <c r="C130" s="61" t="s">
         <v>1554</v>
@@ -16075,7 +16081,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B131" s="9"/>
       <c r="C131" s="61" t="s">
         <v>1554</v>
@@ -16101,7 +16107,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B132" s="9"/>
       <c r="C132" s="61" t="s">
         <v>1554</v>
@@ -16127,7 +16133,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B133" s="9"/>
       <c r="C133" s="61" t="s">
         <v>1554</v>
@@ -16153,7 +16159,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B134" s="9"/>
       <c r="C134" s="61" t="s">
         <v>1554</v>
@@ -16179,7 +16185,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B135" s="9"/>
       <c r="C135" s="61" t="s">
         <v>1554</v>
@@ -16205,7 +16211,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B136" s="9"/>
       <c r="C136" s="61" t="s">
         <v>1554</v>
@@ -16229,7 +16235,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B137" s="9"/>
       <c r="C137" s="61" t="s">
         <v>1554</v>
@@ -16257,7 +16263,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B138" s="9"/>
       <c r="C138" s="61" t="s">
         <v>1554</v>
@@ -16283,7 +16289,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="59" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:11" s="59" customFormat="1" ht="18">
       <c r="B139" s="9"/>
       <c r="C139" s="61" t="s">
         <v>1554</v>
@@ -16307,7 +16313,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B140" s="9"/>
       <c r="C140" s="61" t="s">
         <v>1554</v>
@@ -16331,7 +16337,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B141" s="8" t="s">
         <v>19</v>
       </c>
@@ -16359,7 +16365,7 @@
       </c>
       <c r="K141" s="85"/>
     </row>
-    <row r="142" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B142" s="8" t="s">
         <v>19</v>
       </c>
@@ -16389,7 +16395,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B143" s="8" t="s">
         <v>19</v>
       </c>
@@ -16419,7 +16425,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B144" s="8" t="s">
         <v>19</v>
       </c>
@@ -16449,7 +16455,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B145" s="8" t="s">
         <v>19</v>
       </c>
@@ -16479,7 +16485,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B146" s="9"/>
       <c r="C146" s="66" t="s">
         <v>60</v>
@@ -16507,7 +16513,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="147" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B147" s="9"/>
       <c r="C147" s="9" t="s">
         <v>60</v>
@@ -16535,7 +16541,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="148" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B148" s="9"/>
       <c r="C148" s="61" t="s">
         <v>60</v>
@@ -16563,7 +16569,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B149" s="9"/>
       <c r="C149" s="9" t="s">
         <v>60</v>
@@ -16591,7 +16597,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="150" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B150" s="9"/>
       <c r="C150" s="61" t="s">
         <v>60</v>
@@ -16617,7 +16623,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B151" s="9" t="s">
         <v>7</v>
       </c>
@@ -16647,7 +16653,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="152" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B152" s="9" t="s">
         <v>713</v>
       </c>
@@ -16675,7 +16681,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="153" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B153" s="9" t="s">
         <v>713</v>
       </c>
@@ -16703,7 +16709,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B154" s="9"/>
       <c r="C154" s="63" t="s">
         <v>60</v>
@@ -16729,7 +16735,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B155" s="9" t="s">
         <v>1389</v>
       </c>
@@ -16757,7 +16763,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="156" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B156" s="9"/>
       <c r="C156" s="66" t="s">
         <v>719</v>
@@ -16783,7 +16789,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B157" s="9"/>
       <c r="C157" s="61" t="s">
         <v>719</v>
@@ -16811,7 +16817,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="158" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B158" s="9"/>
       <c r="C158" s="61" t="s">
         <v>719</v>
@@ -16839,7 +16845,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="159" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B159" s="45"/>
       <c r="C159" s="61" t="s">
         <v>719</v>
@@ -16867,7 +16873,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B160" s="9"/>
       <c r="C160" s="9" t="s">
         <v>719</v>
@@ -16895,7 +16901,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
         <v>719</v>
@@ -16923,7 +16929,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B162" s="9"/>
       <c r="C162" s="61" t="s">
         <v>719</v>
@@ -16951,7 +16957,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B163" s="9"/>
       <c r="C163" s="61" t="s">
         <v>719</v>
@@ -16979,7 +16985,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B164" s="9" t="s">
         <v>717</v>
       </c>
@@ -17009,7 +17015,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B165" s="9" t="s">
         <v>717</v>
       </c>
@@ -17039,7 +17045,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B166" s="9" t="s">
         <v>717</v>
       </c>
@@ -17069,7 +17075,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B167" s="9"/>
       <c r="C167" s="9" t="s">
         <v>719</v>
@@ -17097,7 +17103,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B168" s="9"/>
       <c r="C168" s="61" t="s">
         <v>719</v>
@@ -17123,7 +17129,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B169" s="9"/>
       <c r="C169" s="66" t="s">
         <v>719</v>
@@ -17151,7 +17157,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B170" s="45"/>
       <c r="C170" s="61" t="s">
         <v>719</v>
@@ -17177,7 +17183,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B171" s="9"/>
       <c r="C171" s="66" t="s">
         <v>719</v>
@@ -17203,7 +17209,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B172" s="9"/>
       <c r="C172" s="9" t="s">
         <v>719</v>
@@ -17229,7 +17235,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B173" s="9" t="s">
         <v>719</v>
       </c>
@@ -17259,7 +17265,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B174" s="9" t="s">
         <v>719</v>
       </c>
@@ -17289,7 +17295,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B175" s="9"/>
       <c r="C175" s="61" t="s">
         <v>719</v>
@@ -17317,7 +17323,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B176" s="9"/>
       <c r="C176" s="61" t="s">
         <v>719</v>
@@ -17343,7 +17349,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B177" s="9"/>
       <c r="C177" s="66" t="s">
         <v>719</v>
@@ -17369,7 +17375,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="178" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B178" s="9"/>
       <c r="C178" s="61" t="s">
         <v>719</v>
@@ -17397,7 +17403,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B179" s="9"/>
       <c r="C179" s="61" t="s">
         <v>719</v>
@@ -17425,7 +17431,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B180" s="9"/>
       <c r="C180" s="61" t="s">
         <v>719</v>
@@ -17453,7 +17459,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B181" s="9"/>
       <c r="C181" s="61" t="s">
         <v>719</v>
@@ -17481,7 +17487,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B182" s="9"/>
       <c r="C182" s="61" t="s">
         <v>719</v>
@@ -17509,7 +17515,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="183" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B183" s="9"/>
       <c r="C183" s="61" t="s">
         <v>719</v>
@@ -17537,7 +17543,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="184" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B184" s="9"/>
       <c r="C184" s="61" t="s">
         <v>719</v>
@@ -17565,7 +17571,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B185" s="9"/>
       <c r="C185" s="9" t="s">
         <v>60</v>
@@ -17595,7 +17601,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B186" s="9" t="s">
         <v>7</v>
       </c>
@@ -17621,7 +17627,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17647,7 +17653,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="188" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B188" s="9" t="s">
         <v>148</v>
       </c>
@@ -17673,7 +17679,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="189" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B189" s="9" t="s">
         <v>148</v>
       </c>
@@ -17699,7 +17705,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B190" s="25"/>
       <c r="C190" s="9" t="s">
         <v>719</v>
@@ -17723,7 +17729,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B191" s="45"/>
       <c r="C191" s="9" t="s">
         <v>719</v>
@@ -17747,7 +17753,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B192" s="9"/>
       <c r="C192" s="9" t="s">
         <v>719</v>
@@ -17771,7 +17777,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="193" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B193" s="9"/>
       <c r="C193" s="9" t="s">
         <v>719</v>
@@ -17795,7 +17801,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>719</v>
@@ -17819,7 +17825,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="195" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B195" s="9"/>
       <c r="C195" s="61" t="s">
         <v>719</v>
@@ -17843,7 +17849,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B196" s="9"/>
       <c r="C196" s="61" t="s">
         <v>719</v>
@@ -17867,7 +17873,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="197" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B197" s="9"/>
       <c r="C197" s="61" t="s">
         <v>719</v>
@@ -17891,7 +17897,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="198" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B198" s="9"/>
       <c r="C198" s="61" t="s">
         <v>719</v>
@@ -17915,7 +17921,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="199" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B199" s="9" t="s">
         <v>7</v>
       </c>
@@ -17945,7 +17951,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="200" spans="2:11" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B200" s="9" t="s">
         <v>7</v>
       </c>
@@ -17975,7 +17981,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B201" s="9"/>
       <c r="C201" s="61" t="s">
         <v>1627</v>
@@ -17999,7 +18005,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B202" s="9"/>
       <c r="C202" s="61" t="s">
         <v>1627</v>
@@ -18023,7 +18029,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B203" s="9"/>
       <c r="C203" s="61" t="s">
         <v>1627</v>
@@ -18047,7 +18053,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B204" s="9"/>
       <c r="C204" s="61" t="s">
         <v>1627</v>
@@ -18071,7 +18077,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B205" s="9"/>
       <c r="C205" s="61" t="s">
         <v>1627</v>
@@ -18095,7 +18101,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B206" s="9"/>
       <c r="C206" s="61" t="s">
         <v>1627</v>
@@ -18119,7 +18125,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="207" spans="2:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:11" ht="18">
       <c r="B207" s="69"/>
       <c r="C207" s="84" t="s">
         <v>1627</v>
@@ -18143,7 +18149,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="208" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B208" s="9"/>
       <c r="C208" s="61" t="s">
         <v>1627</v>
@@ -18167,7 +18173,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="209" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B209" s="45"/>
       <c r="C209" s="45"/>
       <c r="D209" s="45"/>
@@ -18179,7 +18185,7 @@
       <c r="J209" s="45"/>
       <c r="K209" s="54"/>
     </row>
-    <row r="210" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B210" s="25"/>
       <c r="C210" s="25"/>
       <c r="D210" s="25"/>
@@ -18191,7 +18197,7 @@
       <c r="J210" s="25"/>
       <c r="K210" s="54"/>
     </row>
-    <row r="211" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B211" s="25"/>
       <c r="C211" s="25"/>
       <c r="D211" s="25"/>
@@ -18203,7 +18209,7 @@
       <c r="J211" s="25"/>
       <c r="K211" s="54"/>
     </row>
-    <row r="212" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B212" s="25"/>
       <c r="C212" s="25"/>
       <c r="D212" s="25"/>
@@ -18215,7 +18221,7 @@
       <c r="J212" s="25"/>
       <c r="K212" s="54"/>
     </row>
-    <row r="213" spans="2:11" s="24" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B213" s="25"/>
       <c r="C213" s="25"/>
       <c r="D213" s="25"/>
@@ -18227,7 +18233,7 @@
       <c r="J213" s="25"/>
       <c r="K213" s="54"/>
     </row>
-    <row r="214" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:11">
       <c r="B214" s="45"/>
       <c r="C214" s="45"/>
       <c r="D214" s="45"/>
@@ -18239,7 +18245,7 @@
       <c r="J214" s="45"/>
       <c r="K214" s="54"/>
     </row>
-    <row r="215" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:11">
       <c r="B215" s="45"/>
       <c r="C215" s="45"/>
       <c r="D215" s="45"/>
@@ -18251,7 +18257,7 @@
       <c r="J215" s="45"/>
       <c r="K215" s="54"/>
     </row>
-    <row r="216" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:11">
       <c r="B216" s="45"/>
       <c r="C216" s="45"/>
       <c r="D216" s="45"/>
@@ -18263,7 +18269,7 @@
       <c r="J216" s="45"/>
       <c r="K216" s="54"/>
     </row>
-    <row r="217" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:11">
       <c r="B217" s="45"/>
       <c r="C217" s="45"/>
       <c r="D217" s="45"/>
@@ -18275,7 +18281,7 @@
       <c r="J217" s="45"/>
       <c r="K217" s="54"/>
     </row>
-    <row r="218" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:11">
       <c r="B218" s="45"/>
       <c r="C218" s="45"/>
       <c r="D218" s="45"/>
@@ -18287,7 +18293,7 @@
       <c r="J218" s="45"/>
       <c r="K218" s="54"/>
     </row>
-    <row r="219" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:11">
       <c r="B219" s="45"/>
       <c r="C219" s="45"/>
       <c r="D219" s="45"/>
@@ -18299,7 +18305,7 @@
       <c r="J219" s="45"/>
       <c r="K219" s="54"/>
     </row>
-    <row r="220" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:11">
       <c r="B220" s="45"/>
       <c r="C220" s="45"/>
       <c r="D220" s="45"/>
@@ -18311,7 +18317,7 @@
       <c r="J220" s="45"/>
       <c r="K220" s="54"/>
     </row>
-    <row r="221" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:11">
       <c r="B221" s="45"/>
       <c r="C221" s="45"/>
       <c r="D221" s="45"/>
@@ -18323,7 +18329,7 @@
       <c r="J221" s="45"/>
       <c r="K221" s="54"/>
     </row>
-    <row r="222" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:11">
       <c r="B222" s="45"/>
       <c r="C222" s="45"/>
       <c r="D222" s="45"/>
@@ -18335,7 +18341,7 @@
       <c r="J222" s="45"/>
       <c r="K222" s="54"/>
     </row>
-    <row r="223" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:11">
       <c r="B223" s="45"/>
       <c r="C223" s="45"/>
       <c r="D223" s="45"/>
@@ -18347,7 +18353,7 @@
       <c r="J223" s="45"/>
       <c r="K223" s="54"/>
     </row>
-    <row r="224" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:11">
       <c r="B224" s="45"/>
       <c r="C224" s="45"/>
       <c r="D224" s="45"/>
@@ -18359,7 +18365,7 @@
       <c r="J224" s="45"/>
       <c r="K224" s="54"/>
     </row>
-    <row r="225" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:11">
       <c r="B225" s="45"/>
       <c r="C225" s="45"/>
       <c r="D225" s="45"/>
@@ -18371,7 +18377,7 @@
       <c r="J225" s="45"/>
       <c r="K225" s="54"/>
     </row>
-    <row r="226" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:11">
       <c r="B226" s="45"/>
       <c r="C226" s="45"/>
       <c r="D226" s="45"/>
@@ -18383,7 +18389,7 @@
       <c r="J226" s="45"/>
       <c r="K226" s="54"/>
     </row>
-    <row r="227" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:11">
       <c r="B227" s="45"/>
       <c r="C227" s="45"/>
       <c r="D227" s="45"/>
@@ -18395,7 +18401,7 @@
       <c r="J227" s="45"/>
       <c r="K227" s="54"/>
     </row>
-    <row r="228" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:11">
       <c r="B228" s="45"/>
       <c r="C228" s="45"/>
       <c r="D228" s="45"/>
@@ -18407,7 +18413,7 @@
       <c r="J228" s="45"/>
       <c r="K228" s="54"/>
     </row>
-    <row r="229" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:11">
       <c r="B229" s="45"/>
       <c r="C229" s="45"/>
       <c r="D229" s="45"/>
@@ -18419,7 +18425,7 @@
       <c r="J229" s="45"/>
       <c r="K229" s="54"/>
     </row>
-    <row r="230" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:11">
       <c r="B230" s="45"/>
       <c r="C230" s="45"/>
       <c r="D230" s="45"/>
@@ -18431,7 +18437,7 @@
       <c r="J230" s="45"/>
       <c r="K230" s="54"/>
     </row>
-    <row r="231" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:11">
       <c r="B231" s="45"/>
       <c r="C231" s="45"/>
       <c r="D231" s="45"/>
@@ -18443,7 +18449,7 @@
       <c r="J231" s="45"/>
       <c r="K231" s="54"/>
     </row>
-    <row r="232" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:11">
       <c r="B232" s="45"/>
       <c r="C232" s="45"/>
       <c r="D232" s="45"/>
@@ -18455,7 +18461,7 @@
       <c r="J232" s="45"/>
       <c r="K232" s="54"/>
     </row>
-    <row r="233" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:11">
       <c r="B233" s="45"/>
       <c r="C233" s="45"/>
       <c r="D233" s="45"/>
@@ -18467,7 +18473,7 @@
       <c r="J233" s="45"/>
       <c r="K233" s="54"/>
     </row>
-    <row r="234" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:11">
       <c r="B234" s="45"/>
       <c r="C234" s="45"/>
       <c r="D234" s="45"/>
@@ -18479,7 +18485,7 @@
       <c r="J234" s="45"/>
       <c r="K234" s="54"/>
     </row>
-    <row r="235" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:11">
       <c r="B235" s="45"/>
       <c r="C235" s="45"/>
       <c r="D235" s="45"/>
@@ -18491,7 +18497,7 @@
       <c r="J235" s="45"/>
       <c r="K235" s="54"/>
     </row>
-    <row r="236" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:11">
       <c r="B236" s="45"/>
       <c r="C236" s="45"/>
       <c r="D236" s="45"/>
@@ -18503,7 +18509,7 @@
       <c r="J236" s="45"/>
       <c r="K236" s="54"/>
     </row>
-    <row r="237" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:11">
       <c r="B237" s="45"/>
       <c r="C237" s="45"/>
       <c r="D237" s="45"/>
@@ -18515,7 +18521,7 @@
       <c r="J237" s="45"/>
       <c r="K237" s="54"/>
     </row>
-    <row r="238" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:11">
       <c r="B238" s="45"/>
       <c r="C238" s="45"/>
       <c r="D238" s="45"/>
@@ -18527,7 +18533,7 @@
       <c r="J238" s="45"/>
       <c r="K238" s="54"/>
     </row>
-    <row r="239" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:11">
       <c r="B239" s="45"/>
       <c r="C239" s="45"/>
       <c r="D239" s="45"/>
@@ -18539,7 +18545,7 @@
       <c r="J239" s="45"/>
       <c r="K239" s="54"/>
     </row>
-    <row r="240" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:11">
       <c r="B240" s="45"/>
       <c r="C240" s="45"/>
       <c r="D240" s="45"/>
@@ -18551,7 +18557,7 @@
       <c r="J240" s="45"/>
       <c r="K240" s="54"/>
     </row>
-    <row r="241" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:11">
       <c r="B241" s="45"/>
       <c r="C241" s="45"/>
       <c r="D241" s="45"/>
@@ -18563,7 +18569,7 @@
       <c r="J241" s="45"/>
       <c r="K241" s="54"/>
     </row>
-    <row r="242" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:11">
       <c r="B242" s="45"/>
       <c r="C242" s="45"/>
       <c r="D242" s="45"/>
@@ -18575,7 +18581,7 @@
       <c r="J242" s="45"/>
       <c r="K242" s="54"/>
     </row>
-    <row r="243" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:11">
       <c r="B243" s="45"/>
       <c r="C243" s="45"/>
       <c r="D243" s="45"/>
@@ -18587,7 +18593,7 @@
       <c r="J243" s="45"/>
       <c r="K243" s="54"/>
     </row>
-    <row r="244" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:11">
       <c r="B244" s="45"/>
       <c r="C244" s="45"/>
       <c r="D244" s="45"/>
@@ -18599,7 +18605,7 @@
       <c r="J244" s="45"/>
       <c r="K244" s="54"/>
     </row>
-    <row r="245" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:11">
       <c r="B245" s="45"/>
       <c r="C245" s="45"/>
       <c r="D245" s="45"/>
@@ -18611,7 +18617,7 @@
       <c r="J245" s="45"/>
       <c r="K245" s="54"/>
     </row>
-    <row r="246" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:11">
       <c r="B246" s="45"/>
       <c r="C246" s="45"/>
       <c r="D246" s="45"/>
@@ -18623,7 +18629,7 @@
       <c r="J246" s="45"/>
       <c r="K246" s="54"/>
     </row>
-    <row r="247" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:11">
       <c r="B247" s="45"/>
       <c r="C247" s="45"/>
       <c r="D247" s="45"/>
@@ -18635,7 +18641,7 @@
       <c r="J247" s="45"/>
       <c r="K247" s="54"/>
     </row>
-    <row r="248" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:11">
       <c r="B248" s="45"/>
       <c r="C248" s="45"/>
       <c r="D248" s="45"/>
@@ -18647,7 +18653,7 @@
       <c r="J248" s="45"/>
       <c r="K248" s="54"/>
     </row>
-    <row r="249" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:11">
       <c r="B249" s="45"/>
       <c r="C249" s="45"/>
       <c r="D249" s="45"/>
@@ -18659,7 +18665,7 @@
       <c r="J249" s="45"/>
       <c r="K249" s="54"/>
     </row>
-    <row r="250" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:11">
       <c r="B250" s="45"/>
       <c r="C250" s="45"/>
       <c r="D250" s="45"/>
@@ -18671,7 +18677,7 @@
       <c r="J250" s="45"/>
       <c r="K250" s="54"/>
     </row>
-    <row r="251" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:11">
       <c r="B251" s="45"/>
       <c r="C251" s="45"/>
       <c r="D251" s="45"/>
@@ -18683,7 +18689,7 @@
       <c r="J251" s="45"/>
       <c r="K251" s="54"/>
     </row>
-    <row r="252" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:11">
       <c r="B252" s="45"/>
       <c r="C252" s="45"/>
       <c r="D252" s="45"/>
@@ -18695,7 +18701,7 @@
       <c r="J252" s="45"/>
       <c r="K252" s="54"/>
     </row>
-    <row r="253" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:11">
       <c r="B253" s="45"/>
       <c r="C253" s="45"/>
       <c r="D253" s="45"/>
@@ -18707,7 +18713,7 @@
       <c r="J253" s="45"/>
       <c r="K253" s="54"/>
     </row>
-    <row r="254" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:11">
       <c r="B254" s="45"/>
       <c r="C254" s="45"/>
       <c r="D254" s="45"/>
@@ -18719,7 +18725,7 @@
       <c r="J254" s="45"/>
       <c r="K254" s="54"/>
     </row>
-    <row r="255" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:11">
       <c r="B255" s="45"/>
       <c r="C255" s="45"/>
       <c r="D255" s="45"/>
@@ -18731,7 +18737,7 @@
       <c r="J255" s="45"/>
       <c r="K255" s="54"/>
     </row>
-    <row r="256" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:11">
       <c r="B256" s="45"/>
       <c r="C256" s="45"/>
       <c r="D256" s="45"/>
@@ -18743,7 +18749,7 @@
       <c r="J256" s="45"/>
       <c r="K256" s="54"/>
     </row>
-    <row r="257" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:11">
       <c r="B257" s="45"/>
       <c r="C257" s="45"/>
       <c r="D257" s="45"/>
@@ -18755,7 +18761,7 @@
       <c r="J257" s="45"/>
       <c r="K257" s="54"/>
     </row>
-    <row r="258" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:11">
       <c r="B258" s="45"/>
       <c r="C258" s="45"/>
       <c r="D258" s="45"/>
@@ -18767,7 +18773,7 @@
       <c r="J258" s="45"/>
       <c r="K258" s="54"/>
     </row>
-    <row r="259" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:11">
       <c r="B259" s="45"/>
       <c r="C259" s="45"/>
       <c r="D259" s="45"/>
@@ -18779,7 +18785,7 @@
       <c r="J259" s="45"/>
       <c r="K259" s="54"/>
     </row>
-    <row r="260" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:11">
       <c r="B260" s="45"/>
       <c r="C260" s="45"/>
       <c r="D260" s="45"/>
@@ -18791,7 +18797,7 @@
       <c r="J260" s="45"/>
       <c r="K260" s="54"/>
     </row>
-    <row r="261" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:11">
       <c r="B261" s="45"/>
       <c r="C261" s="45"/>
       <c r="D261" s="45"/>
@@ -18803,7 +18809,7 @@
       <c r="J261" s="45"/>
       <c r="K261" s="54"/>
     </row>
-    <row r="262" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:11">
       <c r="B262" s="45"/>
       <c r="C262" s="45"/>
       <c r="D262" s="45"/>
@@ -18815,7 +18821,7 @@
       <c r="J262" s="45"/>
       <c r="K262" s="54"/>
     </row>
-    <row r="263" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:11">
       <c r="B263" s="45"/>
       <c r="C263" s="45"/>
       <c r="D263" s="45"/>
@@ -18827,7 +18833,7 @@
       <c r="J263" s="45"/>
       <c r="K263" s="54"/>
     </row>
-    <row r="264" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:11">
       <c r="B264" s="45"/>
       <c r="C264" s="45"/>
       <c r="D264" s="45"/>
@@ -18839,7 +18845,7 @@
       <c r="J264" s="45"/>
       <c r="K264" s="54"/>
     </row>
-    <row r="265" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:11">
       <c r="B265" s="45"/>
       <c r="C265" s="45"/>
       <c r="D265" s="45"/>
@@ -18851,7 +18857,7 @@
       <c r="J265" s="45"/>
       <c r="K265" s="54"/>
     </row>
-    <row r="266" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:11">
       <c r="B266" s="45"/>
       <c r="C266" s="45"/>
       <c r="D266" s="45"/>
@@ -18863,7 +18869,7 @@
       <c r="J266" s="45"/>
       <c r="K266" s="54"/>
     </row>
-    <row r="267" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:11">
       <c r="B267" s="45"/>
       <c r="C267" s="45"/>
       <c r="D267" s="45"/>
@@ -18875,7 +18881,7 @@
       <c r="J267" s="45"/>
       <c r="K267" s="54"/>
     </row>
-    <row r="268" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:11">
       <c r="B268" s="45"/>
       <c r="C268" s="45"/>
       <c r="D268" s="45"/>
@@ -18887,7 +18893,7 @@
       <c r="J268" s="45"/>
       <c r="K268" s="54"/>
     </row>
-    <row r="269" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:11">
       <c r="B269" s="45"/>
       <c r="C269" s="45"/>
       <c r="D269" s="45"/>

</xml_diff>

<commit_message>
Chamaka Ghanam and Jatai files 07/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -5220,74 +5220,6 @@
     <t>JD 22</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>+xªÉÉ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>(gm)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>+vÉ®úÉ xÉvÉ®úÉxÉxªÉÉ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>(gm)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>+xªÉÉ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>(gm)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="1"/>
-        <rFont val="DV2-TTVedic"/>
-        <family val="5"/>
-      </rPr>
-      <t>+vÉ®úÉxÉÂ *</t>
-    </r>
-  </si>
-  <si>
     <t>JD 35</t>
   </si>
   <si>
@@ -5346,13 +5278,16 @@
   </si>
   <si>
     <t>1.1.14.2</t>
+  </si>
+  <si>
+    <t>aqnyA(gm) adha#rAq nadha#rAnaqnyA(gm) aqnyA(gm) adha#rAn |</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5464,19 +5399,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="DV2-TTVedic"/>
-      <family val="5"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="DV2-TTVedic"/>
-      <family val="5"/>
     </font>
   </fonts>
   <fills count="10">
@@ -5702,7 +5624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5969,7 +5891,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6283,13 +6204,13 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K117" sqref="K117"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -6304,7 +6225,7 @@
     <col min="11" max="11" width="81.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.25">
+    <row r="1" spans="1:18" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6321,7 +6242,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="45.75">
+    <row r="3" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="18" t="s">
         <v>1</v>
@@ -6361,7 +6282,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75">
+    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>131</v>
@@ -6397,7 +6318,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>131</v>
@@ -6433,7 +6354,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>131</v>
@@ -6469,7 +6390,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
         <v>148</v>
@@ -6507,7 +6428,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>148</v>
@@ -6525,7 +6446,7 @@
         <v>1104</v>
       </c>
       <c r="G8" s="77" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
@@ -6535,7 +6456,7 @@
         <v>461</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -6545,7 +6466,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>148</v>
@@ -6583,7 +6504,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>148</v>
@@ -6619,7 +6540,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>148</v>
@@ -6657,7 +6578,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>148</v>
@@ -6697,7 +6618,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>148</v>
@@ -6735,7 +6656,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>148</v>
@@ -6773,7 +6694,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>148</v>
@@ -6799,7 +6720,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>148</v>
@@ -6835,7 +6756,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>148</v>
@@ -6871,7 +6792,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>148</v>
@@ -6907,7 +6828,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -6943,7 +6864,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="18">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>148</v>
@@ -6979,7 +6900,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="30.75">
+    <row r="21" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
         <v>148</v>
@@ -7015,7 +6936,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="18">
+    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
         <v>148</v>
@@ -7051,7 +6972,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="30.75">
+    <row r="23" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="s">
         <v>148</v>
@@ -7087,7 +7008,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="30.75">
+    <row r="24" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>148</v>
@@ -7123,7 +7044,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="60.75">
+    <row r="25" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>148</v>
@@ -7161,7 +7082,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="30.75">
+    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
         <v>148</v>
@@ -7199,7 +7120,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="30.75">
+    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
         <v>148</v>
@@ -7237,7 +7158,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="30.75">
+    <row r="28" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9" t="s">
         <v>148</v>
@@ -7275,7 +7196,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="45.75">
+    <row r="29" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9" t="s">
         <v>148</v>
@@ -7311,7 +7232,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="18">
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>148</v>
@@ -7347,7 +7268,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="18">
+    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9" t="s">
         <v>148</v>
@@ -7385,7 +7306,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="18">
+    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>148</v>
@@ -7423,7 +7344,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="45.75">
+    <row r="33" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
         <v>148</v>
@@ -7459,7 +7380,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="75.75">
+    <row r="34" spans="1:18" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="9" t="s">
         <v>148</v>
@@ -7495,7 +7416,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="18">
+    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="9" t="s">
         <v>148</v>
@@ -7533,7 +7454,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="30.75">
+    <row r="36" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
         <v>148</v>
@@ -7571,7 +7492,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="30.75">
+    <row r="37" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="9" t="s">
         <v>148</v>
@@ -7607,7 +7528,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="45.75">
+    <row r="38" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="9" t="s">
         <v>148</v>
@@ -7643,7 +7564,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="60.75">
+    <row r="39" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
         <v>148</v>
@@ -7681,7 +7602,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="45.75">
+    <row r="40" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
         <v>148</v>
@@ -7717,7 +7638,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="36">
+    <row r="41" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="9" t="s">
         <v>148</v>
@@ -7753,7 +7674,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="18">
+    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>148</v>
@@ -7789,7 +7710,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="30.75">
+    <row r="43" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
         <v>148</v>
@@ -7825,7 +7746,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="18">
+    <row r="44" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="9" t="s">
         <v>148</v>
@@ -7861,7 +7782,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="18">
+    <row r="45" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
         <v>148</v>
@@ -7897,7 +7818,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="18">
+    <row r="46" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="9" t="s">
         <v>148</v>
@@ -7931,7 +7852,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="18">
+    <row r="47" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="9" t="s">
         <v>148</v>
@@ -7969,7 +7890,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="30.75">
+    <row r="48" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
         <v>148</v>
@@ -8005,7 +7926,7 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" ht="18">
+    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="9" t="s">
         <v>148</v>
@@ -8041,7 +7962,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18" ht="30.75">
+    <row r="50" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="9" t="s">
         <v>148</v>
@@ -8077,7 +7998,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="18">
+    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
         <v>148</v>
@@ -8115,7 +8036,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="18">
+    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>148</v>
@@ -8153,7 +8074,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="60.75">
+    <row r="53" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
         <v>148</v>
@@ -8191,7 +8112,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" ht="36">
+    <row r="54" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
         <v>148</v>
@@ -8229,7 +8150,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" ht="18">
+    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
         <v>148</v>
@@ -8267,7 +8188,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="30.75">
+    <row r="56" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
         <v>791</v>
@@ -8305,7 +8226,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" ht="18">
+    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
         <v>791</v>
@@ -8339,7 +8260,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" ht="30.75">
+    <row r="58" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="9" t="s">
         <v>791</v>
@@ -8377,7 +8298,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" ht="18">
+    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
         <v>791</v>
@@ -8415,7 +8336,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="18">
+    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
         <v>791</v>
@@ -8453,7 +8374,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="18">
+    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="9" t="s">
         <v>791</v>
@@ -8491,7 +8412,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" ht="18">
+    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="8" t="s">
         <v>791</v>
@@ -8525,9 +8446,9 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" ht="18">
+    <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="137" t="s">
+      <c r="B63" s="136" t="s">
         <v>15</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -8547,7 +8468,7 @@
       <c r="I63" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J63" s="134" t="s">
+      <c r="J63" s="133" t="s">
         <v>347</v>
       </c>
       <c r="K63" s="34" t="s">
@@ -8561,9 +8482,9 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" ht="18">
+    <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="137" t="s">
+      <c r="B64" s="136" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -8583,7 +8504,7 @@
       <c r="I64" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J64" s="134" t="s">
+      <c r="J64" s="133" t="s">
         <v>348</v>
       </c>
       <c r="K64" s="34" t="s">
@@ -8597,9 +8518,9 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="18">
+    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="137" t="s">
+      <c r="B65" s="136" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -8619,7 +8540,7 @@
       <c r="I65" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J65" s="134" t="s">
+      <c r="J65" s="133" t="s">
         <v>346</v>
       </c>
       <c r="K65" s="34" t="s">
@@ -8633,9 +8554,9 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" ht="18">
+    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="137" t="s">
+      <c r="B66" s="136" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -8653,8 +8574,8 @@
       <c r="I66" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J66" s="134" t="s">
-        <v>1698</v>
+      <c r="J66" s="133" t="s">
+        <v>1697</v>
       </c>
       <c r="K66" s="34" t="s">
         <v>17</v>
@@ -8667,7 +8588,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" ht="30.75">
+    <row r="67" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
         <v>98</v>
@@ -8703,7 +8624,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="60.75">
+    <row r="68" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
         <v>98</v>
@@ -8722,7 +8643,7 @@
         <v>100</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>323</v>
@@ -8741,7 +8662,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="30.75">
+    <row r="69" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
         <v>98</v>
@@ -8760,7 +8681,7 @@
         <v>100</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="I69" s="21" t="s">
         <v>324</v>
@@ -8779,7 +8700,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" ht="30.75">
+    <row r="70" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="9" t="s">
         <v>98</v>
@@ -8798,7 +8719,7 @@
         <v>821</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>324</v>
@@ -8815,7 +8736,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="18">
+    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="9" t="s">
         <v>98</v>
@@ -8855,7 +8776,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" ht="18">
+    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
         <v>98</v>
@@ -8874,7 +8795,7 @@
         <v>1125</v>
       </c>
       <c r="H72" s="61" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="I72" s="21" t="s">
         <v>223</v>
@@ -8893,7 +8814,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="30.75">
+    <row r="73" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
         <v>98</v>
@@ -8912,7 +8833,7 @@
         <v>100</v>
       </c>
       <c r="H73" s="61" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="I73" s="21" t="s">
         <v>317</v>
@@ -8931,7 +8852,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" ht="27">
+    <row r="74" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
         <v>1339</v>
@@ -8958,8 +8879,8 @@
       <c r="J74" s="25" t="s">
         <v>1129</v>
       </c>
-      <c r="K74" s="132" t="s">
-        <v>1681</v>
+      <c r="K74" s="37" t="s">
+        <v>1701</v>
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -8969,7 +8890,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" ht="30.75">
+    <row r="75" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
         <v>1339</v>
@@ -9007,7 +8928,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" ht="18">
+    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
         <v>1339</v>
@@ -9043,7 +8964,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="30.75">
+    <row r="77" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
         <v>1339</v>
@@ -9081,7 +9002,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="30.75">
+    <row r="78" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
         <v>1339</v>
@@ -9119,7 +9040,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" ht="30.75">
+    <row r="79" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
         <v>139</v>
@@ -9138,7 +9059,7 @@
       </c>
       <c r="G79" s="45"/>
       <c r="H79" s="11" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="I79" s="21" t="s">
         <v>295</v>
@@ -9157,7 +9078,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="18">
+    <row r="80" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
         <v>139</v>
@@ -9176,7 +9097,7 @@
       </c>
       <c r="G80" s="45"/>
       <c r="H80" s="11" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="I80" s="21" t="s">
         <v>224</v>
@@ -9195,7 +9116,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" ht="18">
+    <row r="81" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
         <v>139</v>
@@ -9233,7 +9154,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" ht="30.75">
+    <row r="82" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
         <v>139</v>
@@ -9252,7 +9173,7 @@
         <v>1677</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="I82" s="21" t="s">
         <v>820</v>
@@ -9271,7 +9192,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" ht="18">
+    <row r="83" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="9" t="s">
         <v>1318</v>
@@ -9309,7 +9230,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="36">
+    <row r="84" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
         <v>1318</v>
@@ -9347,7 +9268,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="18">
+    <row r="85" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="9" t="s">
         <v>1318</v>
@@ -9387,7 +9308,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="30.75">
+    <row r="86" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="9" t="s">
         <v>1318</v>
@@ -9406,7 +9327,7 @@
         <v>1131</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="I86" s="21" t="s">
         <v>330</v>
@@ -9425,7 +9346,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="30.75">
+    <row r="87" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="9" t="s">
         <v>1318</v>
@@ -9461,7 +9382,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" ht="18">
+    <row r="88" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
         <v>1318</v>
@@ -9497,7 +9418,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="30.75">
+    <row r="89" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
         <v>7</v>
@@ -9533,7 +9454,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="30.75">
+    <row r="90" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="9" t="s">
         <v>7</v>
@@ -9569,7 +9490,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" ht="30.75">
+    <row r="91" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="9" t="s">
         <v>7</v>
@@ -9605,7 +9526,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" ht="30.75">
+    <row r="92" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="9" t="s">
         <v>7</v>
@@ -9641,7 +9562,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="18">
+    <row r="93" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
@@ -9677,7 +9598,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="18">
+    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="8" t="s">
         <v>7</v>
@@ -9715,7 +9636,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="18">
+    <row r="95" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="8" t="s">
         <v>7</v>
@@ -9751,7 +9672,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="30.75">
+    <row r="96" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="9" t="s">
         <v>7</v>
@@ -9789,7 +9710,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" ht="18">
+    <row r="97" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="9" t="s">
         <v>7</v>
@@ -9825,7 +9746,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="18">
+    <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9863,7 +9784,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="18">
+    <row r="99" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
         <v>7</v>
@@ -9901,7 +9822,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" ht="30.75">
+    <row r="100" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
@@ -9937,7 +9858,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="30.75">
+    <row r="101" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="9" t="s">
         <v>7</v>
@@ -9977,7 +9898,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="18">
+    <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="9" t="s">
         <v>7</v>
@@ -10015,7 +9936,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="30.75">
+    <row r="103" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="9" t="s">
         <v>7</v>
@@ -10053,7 +9974,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="45.75">
+    <row r="104" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
         <v>7</v>
@@ -10072,7 +9993,7 @@
       </c>
       <c r="G104" s="45"/>
       <c r="H104" s="96" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I104" s="76" t="s">
         <v>227</v>
@@ -10091,7 +10012,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="30.75">
+    <row r="105" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="9" t="s">
         <v>7</v>
@@ -10118,7 +10039,7 @@
       <c r="J105" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K105" s="143" t="s">
+      <c r="K105" s="142" t="s">
         <v>111</v>
       </c>
       <c r="L105" s="1"/>
@@ -10129,7 +10050,7 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" ht="36">
+    <row r="106" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="9" t="s">
         <v>7</v>
@@ -10148,7 +10069,7 @@
       </c>
       <c r="G106" s="45"/>
       <c r="H106" s="31" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="I106" s="21" t="s">
         <v>234</v>
@@ -10167,7 +10088,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="18">
+    <row r="107" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10186,7 +10107,7 @@
       </c>
       <c r="G107" s="45"/>
       <c r="H107" s="31" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="I107" s="21" t="s">
         <v>235</v>
@@ -10194,7 +10115,7 @@
       <c r="J107" s="25" t="s">
         <v>387</v>
       </c>
-      <c r="K107" s="138" t="s">
+      <c r="K107" s="137" t="s">
         <v>112</v>
       </c>
       <c r="L107" s="1"/>
@@ -10205,7 +10126,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" ht="18">
+    <row r="108" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>1169</v>
       </c>
@@ -10232,7 +10153,7 @@
       <c r="J108" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="K108" s="146" t="s">
+      <c r="K108" s="145" t="s">
         <v>114</v>
       </c>
       <c r="L108" s="1"/>
@@ -10243,7 +10164,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="18.75" thickBot="1">
+    <row r="109" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
         <v>7</v>
@@ -10268,7 +10189,7 @@
       <c r="J109" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="K109" s="145" t="s">
+      <c r="K109" s="144" t="s">
         <v>116</v>
       </c>
       <c r="L109" s="1"/>
@@ -10279,7 +10200,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="31.5" thickBot="1">
+    <row r="110" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
         <v>7</v>
@@ -10301,12 +10222,12 @@
         <v>237</v>
       </c>
       <c r="I110" s="21" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="J110" s="48" t="s">
         <v>1342</v>
       </c>
-      <c r="K110" s="144" t="s">
+      <c r="K110" s="143" t="s">
         <v>117</v>
       </c>
       <c r="L110" s="1"/>
@@ -10317,7 +10238,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="31.5" thickBot="1">
+    <row r="111" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
         <v>7</v>
@@ -10342,7 +10263,7 @@
       <c r="J111" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="K111" s="144" t="s">
+      <c r="K111" s="143" t="s">
         <v>118</v>
       </c>
       <c r="L111" s="1"/>
@@ -10353,7 +10274,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" ht="18.75" thickBot="1">
+    <row r="112" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
         <v>7</v>
@@ -10391,7 +10312,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" ht="18.75" thickBot="1">
+    <row r="113" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
         <v>7</v>
@@ -10408,7 +10329,7 @@
       <c r="F113" s="90" t="s">
         <v>1669</v>
       </c>
-      <c r="G113" s="133" t="s">
+      <c r="G113" s="132" t="s">
         <v>1674</v>
       </c>
       <c r="H113" s="11" t="s">
@@ -10420,7 +10341,7 @@
       <c r="J113" s="100" t="s">
         <v>393</v>
       </c>
-      <c r="K113" s="141" t="s">
+      <c r="K113" s="140" t="s">
         <v>121</v>
       </c>
       <c r="L113" s="1"/>
@@ -10431,7 +10352,7 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" ht="30.75">
+    <row r="114" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
         <v>7</v>
@@ -10448,7 +10369,7 @@
       <c r="F114" s="61" t="s">
         <v>1669</v>
       </c>
-      <c r="G114" s="133" t="s">
+      <c r="G114" s="132" t="s">
         <v>1674</v>
       </c>
       <c r="H114" s="11" t="s">
@@ -10460,7 +10381,7 @@
       <c r="J114" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="K114" s="142" t="s">
+      <c r="K114" s="141" t="s">
         <v>120</v>
       </c>
       <c r="L114" s="1"/>
@@ -10471,7 +10392,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="18">
+    <row r="115" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>7</v>
@@ -10498,7 +10419,7 @@
       <c r="J115" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="K115" s="143" t="s">
+      <c r="K115" s="142" t="s">
         <v>119</v>
       </c>
       <c r="L115" s="1"/>
@@ -10509,7 +10430,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" ht="18">
+    <row r="116" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
         <v>7</v>
@@ -10545,7 +10466,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="18">
+    <row r="117" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
         <v>7</v>
@@ -10581,7 +10502,7 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" ht="18">
+    <row r="118" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
         <v>19</v>
@@ -10621,7 +10542,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" ht="18">
+    <row r="119" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="63" t="s">
         <v>19</v>
@@ -10645,7 +10566,7 @@
       <c r="I119" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="J119" s="134" t="s">
+      <c r="J119" s="133" t="s">
         <v>349</v>
       </c>
       <c r="K119" s="36" t="s">
@@ -10659,7 +10580,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="18">
+    <row r="120" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="63" t="s">
         <v>19</v>
@@ -10681,7 +10602,7 @@
       <c r="I120" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J120" s="134" t="s">
+      <c r="J120" s="133" t="s">
         <v>350</v>
       </c>
       <c r="K120" s="31"/>
@@ -10693,7 +10614,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="18">
+    <row r="121" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="63" t="s">
         <v>19</v>
@@ -10715,7 +10636,7 @@
       <c r="I121" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J121" s="134" t="s">
+      <c r="J121" s="133" t="s">
         <v>351</v>
       </c>
       <c r="K121" s="31"/>
@@ -10727,7 +10648,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="18.75" thickBot="1">
+    <row r="122" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="63" t="s">
         <v>19</v>
@@ -10749,7 +10670,7 @@
       <c r="I122" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J122" s="134" t="s">
+      <c r="J122" s="133" t="s">
         <v>351</v>
       </c>
       <c r="K122" s="31"/>
@@ -10761,7 +10682,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="18.75" thickBot="1">
+    <row r="123" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="63" t="s">
         <v>19</v>
@@ -10783,7 +10704,7 @@
       <c r="I123" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J123" s="134" t="s">
+      <c r="J123" s="133" t="s">
         <v>563</v>
       </c>
       <c r="K123" s="109"/>
@@ -10795,7 +10716,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="18.75" thickBot="1">
+    <row r="124" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="63" t="s">
         <v>19</v>
@@ -10817,7 +10738,7 @@
       <c r="I124" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J124" s="134" t="s">
+      <c r="J124" s="133" t="s">
         <v>564</v>
       </c>
       <c r="K124" s="105"/>
@@ -10829,7 +10750,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" ht="31.5" thickBot="1">
+    <row r="125" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="63" t="s">
         <v>19</v>
@@ -10851,7 +10772,7 @@
       <c r="I125" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J125" s="134" t="s">
+      <c r="J125" s="133" t="s">
         <v>353</v>
       </c>
       <c r="K125" s="109"/>
@@ -10863,7 +10784,7 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" ht="31.5" thickBot="1">
+    <row r="126" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="63" t="s">
         <v>19</v>
@@ -10885,7 +10806,7 @@
       <c r="I126" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="J126" s="134" t="s">
+      <c r="J126" s="133" t="s">
         <v>355</v>
       </c>
       <c r="K126" s="105"/>
@@ -10897,7 +10818,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="18.75" thickBot="1">
+    <row r="127" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="63" t="s">
         <v>19</v>
@@ -10919,7 +10840,7 @@
       <c r="I127" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J127" s="134" t="s">
+      <c r="J127" s="133" t="s">
         <v>356</v>
       </c>
       <c r="K127" s="105"/>
@@ -10931,7 +10852,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="18.75" thickBot="1">
+    <row r="128" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="63" t="s">
         <v>19</v>
@@ -10953,7 +10874,7 @@
       <c r="I128" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="J128" s="134" t="s">
+      <c r="J128" s="133" t="s">
         <v>356</v>
       </c>
       <c r="K128" s="105"/>
@@ -10965,7 +10886,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="31.5" thickBot="1">
+    <row r="129" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="63" t="s">
         <v>19</v>
@@ -10999,7 +10920,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="30.75">
+    <row r="130" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="9" t="s">
         <v>19</v>
@@ -11035,7 +10956,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" ht="18">
+    <row r="131" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="9" t="s">
         <v>19</v>
@@ -11071,7 +10992,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="18">
+    <row r="132" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="9" t="s">
         <v>19</v>
@@ -11105,7 +11026,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="18">
+    <row r="133" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -11139,7 +11060,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="30.75">
+    <row r="134" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="9" t="s">
         <v>19</v>
@@ -11173,7 +11094,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" ht="18">
+    <row r="135" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
         <v>19</v>
@@ -11207,7 +11128,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" ht="18">
+    <row r="136" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
         <v>19</v>
@@ -11241,7 +11162,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" ht="18">
+    <row r="137" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
         <v>19</v>
@@ -11275,7 +11196,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="18">
+    <row r="138" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11309,7 +11230,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="18.75" thickBot="1">
+    <row r="139" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
         <v>19</v>
@@ -11343,7 +11264,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="18.75" thickBot="1">
+    <row r="140" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="9" t="s">
         <v>19</v>
@@ -11379,7 +11300,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="18">
+    <row r="141" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
         <v>19</v>
@@ -11415,7 +11336,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="18">
+    <row r="142" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
         <v>19</v>
@@ -11451,7 +11372,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="18">
+    <row r="143" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
         <v>19</v>
@@ -11487,7 +11408,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" ht="18">
+    <row r="144" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="9" t="s">
         <v>19</v>
@@ -11521,7 +11442,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" ht="18">
+    <row r="145" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="8" t="s">
         <v>60</v>
@@ -11559,7 +11480,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" ht="30.75">
+    <row r="146" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="8" t="s">
         <v>60</v>
@@ -11578,7 +11499,7 @@
       </c>
       <c r="G146" s="9"/>
       <c r="H146" s="31" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="I146" s="21" t="s">
         <v>245</v>
@@ -11597,7 +11518,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="30.75">
+    <row r="147" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="8" t="s">
         <v>60</v>
@@ -11635,7 +11556,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" ht="18.75" thickBot="1">
+    <row r="148" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="9" t="s">
         <v>60</v>
@@ -11654,7 +11575,7 @@
         <v>62</v>
       </c>
       <c r="H148" s="31" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="I148" s="86" t="s">
         <v>506</v>
@@ -11673,7 +11594,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" ht="31.5" thickBot="1">
+    <row r="149" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="9" t="s">
         <v>60</v>
@@ -11692,7 +11613,7 @@
       </c>
       <c r="G149" s="45"/>
       <c r="H149" s="31" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="I149" s="21" t="s">
         <v>312</v>
@@ -11710,7 +11631,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="18.75" thickBot="1">
+    <row r="150" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="9" t="s">
         <v>60</v>
@@ -11747,7 +11668,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" ht="30.75">
+    <row r="151" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="9" t="s">
         <v>60</v>
@@ -11764,7 +11685,7 @@
         <v>62</v>
       </c>
       <c r="H151" s="31" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="I151" s="21" t="s">
         <v>256</v>
@@ -11782,7 +11703,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="30.75">
+    <row r="152" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11813,7 +11734,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" ht="18">
+    <row r="153" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="8" t="s">
         <v>60</v>
@@ -11848,7 +11769,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" ht="18">
+    <row r="154" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="8" t="s">
         <v>60</v>
@@ -11883,7 +11804,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="30.75">
+    <row r="155" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
         <v>60</v>
@@ -11902,7 +11823,7 @@
       </c>
       <c r="G155" s="45"/>
       <c r="H155" s="31" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I155" s="21" t="s">
         <v>313</v>
@@ -11920,7 +11841,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="18">
+    <row r="156" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
         <v>60</v>
@@ -11939,7 +11860,7 @@
       </c>
       <c r="G156" s="45"/>
       <c r="H156" s="31" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="I156" s="21" t="s">
         <v>258</v>
@@ -11957,7 +11878,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="30.75">
+    <row r="157" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
         <v>719</v>
@@ -11992,7 +11913,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" customHeight="1">
+    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>719</v>
@@ -12027,7 +11948,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" ht="30.75">
+    <row r="159" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
         <v>719</v>
@@ -12062,7 +11983,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18.75" thickBot="1">
+    <row r="160" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>719</v>
@@ -12081,7 +12002,7 @@
       </c>
       <c r="G160" s="45"/>
       <c r="H160" s="11" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="I160" s="21" t="s">
         <v>231</v>
@@ -12099,7 +12020,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="36.75" thickBot="1">
+    <row r="161" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
         <v>719</v>
@@ -12136,7 +12057,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="46.5" thickBot="1">
+    <row r="162" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
         <v>719</v>
@@ -12171,7 +12092,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="18.75" thickBot="1">
+    <row r="163" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="8" t="s">
         <v>719</v>
@@ -12204,7 +12125,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="18.75" thickBot="1">
+    <row r="164" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="8" t="s">
         <v>719</v>
@@ -12237,7 +12158,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="18.75" thickBot="1">
+    <row r="165" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
         <v>719</v>
@@ -12270,7 +12191,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" ht="31.5" thickBot="1">
+    <row r="166" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
         <v>719</v>
@@ -12305,7 +12226,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" ht="31.5" thickBot="1">
+    <row r="167" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
         <v>719</v>
@@ -12334,7 +12255,7 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" ht="18.75" thickBot="1">
+    <row r="168" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
         <v>719</v>
@@ -12369,7 +12290,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="31.5" thickBot="1">
+    <row r="169" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
         <v>719</v>
@@ -12404,7 +12325,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" ht="18.75" thickBot="1">
+    <row r="170" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
       <c r="B170" s="9" t="s">
         <v>719</v>
@@ -12440,7 +12361,7 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" ht="46.5" thickBot="1">
+    <row r="171" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
       <c r="B171" s="9" t="s">
         <v>719</v>
@@ -12476,7 +12397,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="18">
+    <row r="172" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="9" t="s">
         <v>719</v>
@@ -12512,7 +12433,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" s="24" customFormat="1" ht="18">
+    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B173" s="70" t="s">
         <v>719</v>
       </c>
@@ -12540,7 +12461,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="174" spans="1:18" s="24" customFormat="1" ht="18">
+    <row r="174" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B174" s="70"/>
       <c r="C174" s="9"/>
       <c r="D174" s="69"/>
@@ -12552,7 +12473,7 @@
       <c r="J174" s="9"/>
       <c r="K174" s="11"/>
     </row>
-    <row r="175" spans="1:18" ht="18.75">
+    <row r="175" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B175" s="72"/>
       <c r="C175" s="72"/>
       <c r="D175" s="72"/>
@@ -12564,7 +12485,7 @@
       <c r="J175" s="72"/>
       <c r="K175" s="73"/>
     </row>
-    <row r="176" spans="1:18" ht="18.75">
+    <row r="176" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B176" s="72"/>
       <c r="C176" s="72"/>
       <c r="D176" s="72"/>
@@ -12596,10 +12517,10 @@
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -12612,7 +12533,7 @@
     <col min="11" max="11" width="77.85546875" style="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="20.25">
+    <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>775</v>
       </c>
@@ -12625,7 +12546,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="4" spans="2:11" ht="45.75">
+    <row r="4" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -12657,7 +12578,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="27" customHeight="1">
+    <row r="5" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="61" t="s">
         <v>131</v>
@@ -12683,7 +12604,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="26.25">
+    <row r="6" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="9"/>
       <c r="C6" s="61" t="s">
         <v>131</v>
@@ -12709,7 +12630,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="61" t="s">
         <v>131</v>
@@ -12737,7 +12658,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30">
+    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="61" t="s">
         <v>131</v>
@@ -12761,7 +12682,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30">
+    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
@@ -12791,7 +12712,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30">
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="61" t="s">
         <v>148</v>
@@ -12819,7 +12740,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30.75">
+    <row r="11" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="61" t="s">
         <v>148</v>
@@ -12847,7 +12768,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="18">
+    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="61" t="s">
         <v>148</v>
@@ -12875,7 +12796,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="45.75">
+    <row r="13" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="61" t="s">
         <v>148</v>
@@ -12905,7 +12826,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="20.45" customHeight="1">
+    <row r="14" spans="2:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>148</v>
       </c>
@@ -12935,7 +12856,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="30">
+    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>148</v>
       </c>
@@ -12965,7 +12886,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="26.25">
+    <row r="16" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -12993,7 +12914,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.75">
+    <row r="17" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="61" t="s">
         <v>148</v>
@@ -13021,7 +12942,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="18">
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -13049,7 +12970,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="30">
+    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>148</v>
       </c>
@@ -13079,7 +13000,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="26.25">
+    <row r="20" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="25"/>
       <c r="C20" s="66" t="s">
         <v>148</v>
@@ -13105,7 +13026,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="30">
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="61" t="s">
         <v>148</v>
@@ -13133,7 +13054,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="30">
+    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>148</v>
       </c>
@@ -13163,7 +13084,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30">
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="61" t="s">
         <v>148</v>
@@ -13191,7 +13112,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="18">
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
         <v>148</v>
@@ -13219,7 +13140,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30">
+    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>148</v>
       </c>
@@ -13249,7 +13170,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="30">
+    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
         <v>148</v>
@@ -13277,7 +13198,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30.75">
+    <row r="27" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="62" t="s">
         <v>148</v>
@@ -13307,7 +13228,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30.75">
+    <row r="28" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="62" t="s">
         <v>148</v>
@@ -13337,7 +13258,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="18">
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>148</v>
@@ -13361,7 +13282,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="30">
+    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="62" t="s">
         <v>1628</v>
@@ -13387,7 +13308,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="30">
+    <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="62" t="s">
         <v>1628</v>
@@ -13411,7 +13332,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="18">
+    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="61" t="s">
         <v>1628</v>
@@ -13439,7 +13360,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30">
+    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="C33" s="61" t="s">
         <v>1628</v>
@@ -13463,7 +13384,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="18">
+    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="61" t="s">
         <v>1628</v>
@@ -13487,7 +13408,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30">
+    <row r="35" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>791</v>
@@ -13515,7 +13436,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="30">
+    <row r="36" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>1465</v>
       </c>
@@ -13545,7 +13466,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="30">
+    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="61" t="s">
         <v>791</v>
@@ -13573,7 +13494,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="18">
+    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="66" t="s">
         <v>791</v>
@@ -13599,7 +13520,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="18">
+    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="66" t="s">
         <v>791</v>
@@ -13625,7 +13546,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="18">
+    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="61" t="s">
         <v>791</v>
@@ -13653,7 +13574,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="30">
+    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>791</v>
       </c>
@@ -13681,7 +13602,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="26.25">
+    <row r="42" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B42" s="9"/>
       <c r="C42" s="61" t="s">
         <v>791</v>
@@ -13705,7 +13626,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="26.25">
+    <row r="43" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B43" s="9"/>
       <c r="C43" s="61" t="s">
         <v>791</v>
@@ -13729,7 +13650,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="18">
+    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="61" t="s">
         <v>1385</v>
@@ -13755,7 +13676,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="18">
+    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="61" t="s">
         <v>1385</v>
@@ -13783,7 +13704,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="18">
+    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="61" t="s">
         <v>1385</v>
@@ -13811,7 +13732,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="30">
+    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="61" t="s">
         <v>1385</v>
@@ -13837,7 +13758,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="30">
+    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>15</v>
       </c>
@@ -13867,7 +13788,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>15</v>
       </c>
@@ -13897,7 +13818,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
@@ -13913,7 +13834,7 @@
       <c r="F50" s="63" t="s">
         <v>1489</v>
       </c>
-      <c r="G50" s="135" t="s">
+      <c r="G50" s="134" t="s">
         <v>1024</v>
       </c>
       <c r="H50" s="9"/>
@@ -13927,7 +13848,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75">
+    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>15</v>
       </c>
@@ -13943,7 +13864,7 @@
       <c r="F51" s="63" t="s">
         <v>1484</v>
       </c>
-      <c r="G51" s="135" t="s">
+      <c r="G51" s="134" t="s">
         <v>1024</v>
       </c>
       <c r="H51" s="17"/>
@@ -13957,7 +13878,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>15</v>
       </c>
@@ -13973,7 +13894,7 @@
       <c r="F52" s="63" t="s">
         <v>1485</v>
       </c>
-      <c r="G52" s="135" t="s">
+      <c r="G52" s="134" t="s">
         <v>1024</v>
       </c>
       <c r="H52" s="9"/>
@@ -13987,7 +13908,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>15</v>
       </c>
@@ -14003,7 +13924,7 @@
       <c r="F53" s="63" t="s">
         <v>1487</v>
       </c>
-      <c r="G53" s="135" t="s">
+      <c r="G53" s="134" t="s">
         <v>1071</v>
       </c>
       <c r="H53" s="9"/>
@@ -14017,7 +13938,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
         <v>15</v>
       </c>
@@ -14045,14 +13966,14 @@
         <v>827</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="136" t="s">
+      <c r="D55" s="135" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="61"/>
@@ -14073,7 +13994,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25">
+    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B56" s="9" t="s">
         <v>15</v>
       </c>
@@ -14101,7 +14022,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="61" t="s">
         <v>1135</v>
@@ -14125,7 +14046,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="61" t="s">
         <v>1135</v>
@@ -14149,7 +14070,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="61" t="s">
         <v>1135</v>
@@ -14173,7 +14094,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="61" t="s">
         <v>1135</v>
@@ -14197,7 +14118,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="61" t="s">
         <v>1135</v>
@@ -14221,7 +14142,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="61" t="s">
         <v>1135</v>
@@ -14247,7 +14168,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="61" t="s">
         <v>1135</v>
@@ -14273,7 +14194,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="61" t="s">
         <v>1135</v>
@@ -14297,7 +14218,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="30">
+    <row r="65" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="61" t="s">
         <v>1135</v>
@@ -14325,7 +14246,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="18">
+    <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="61" t="s">
         <v>1135</v>
@@ -14351,7 +14272,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="45">
+    <row r="67" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="61" t="s">
         <v>1384</v>
@@ -14379,7 +14300,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="68" spans="2:11" ht="45">
+    <row r="68" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="61" t="s">
         <v>1339</v>
@@ -14407,7 +14328,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="30">
+    <row r="69" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="25"/>
       <c r="C69" s="61" t="s">
         <v>1339</v>
@@ -14433,7 +14354,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="30">
+    <row r="70" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="25"/>
       <c r="C70" s="9" t="s">
         <v>1339</v>
@@ -14461,7 +14382,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="30">
+    <row r="71" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="61" t="s">
         <v>1339</v>
@@ -14487,7 +14408,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="30">
+    <row r="72" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="25"/>
       <c r="C72" s="60" t="s">
         <v>1339</v>
@@ -14515,7 +14436,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="24" customFormat="1" ht="30">
+    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
       <c r="C73" s="61" t="s">
         <v>139</v>
@@ -14543,7 +14464,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="30">
+    <row r="74" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
       <c r="C74" s="61" t="s">
         <v>139</v>
@@ -14571,7 +14492,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="18">
+    <row r="75" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>139</v>
       </c>
@@ -14601,7 +14522,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="18">
+    <row r="76" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>139</v>
       </c>
@@ -14629,7 +14550,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="30">
+    <row r="77" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
         <v>1318</v>
@@ -14657,7 +14578,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="30">
+    <row r="78" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
         <v>1318</v>
@@ -14685,7 +14606,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="18">
+    <row r="79" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="61" t="s">
         <v>1318</v>
@@ -14713,7 +14634,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="80" spans="2:11" ht="30">
+    <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="61" t="s">
         <v>1625</v>
@@ -14739,7 +14660,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="30">
+    <row r="81" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="61" t="s">
         <v>1625</v>
@@ -14765,7 +14686,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="30">
+    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -14793,7 +14714,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="45">
+    <row r="83" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -14821,7 +14742,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="18">
+    <row r="84" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B84" s="25"/>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -14849,7 +14770,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="30">
+    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="66" t="s">
         <v>7</v>
@@ -14875,7 +14796,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="30">
+    <row r="86" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="61" t="s">
         <v>7</v>
@@ -14901,7 +14822,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="18">
+    <row r="87" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="61" t="s">
         <v>7</v>
@@ -14927,7 +14848,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="30">
+    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="61" t="s">
         <v>7</v>
@@ -14953,7 +14874,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="30">
+    <row r="89" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="9" t="s">
         <v>60</v>
       </c>
@@ -14983,7 +14904,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="30">
+    <row r="90" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="61" t="s">
         <v>7</v>
@@ -15009,7 +14930,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="91" spans="2:11" ht="30">
+    <row r="91" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="61" t="s">
         <v>7</v>
@@ -15037,7 +14958,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="92" spans="2:11" ht="30">
+    <row r="92" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="61" t="s">
         <v>7</v>
@@ -15063,7 +14984,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="18">
+    <row r="93" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="61" t="s">
         <v>7</v>
@@ -15089,7 +15010,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="18">
+    <row r="94" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B94" s="25"/>
       <c r="C94" s="9" t="s">
         <v>7</v>
@@ -15117,7 +15038,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="95" spans="2:11" ht="45">
+    <row r="95" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="61" t="s">
         <v>7</v>
@@ -15143,7 +15064,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="96" spans="2:11" ht="18">
+    <row r="96" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B96" s="25" t="s">
         <v>712</v>
       </c>
@@ -15173,7 +15094,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="18">
+    <row r="97" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
         <v>148</v>
       </c>
@@ -15197,11 +15118,11 @@
       <c r="J97" s="25" t="s">
         <v>503</v>
       </c>
-      <c r="K97" s="139" t="s">
+      <c r="K97" s="138" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="30">
+    <row r="98" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
         <v>19</v>
       </c>
@@ -15229,7 +15150,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="18">
+    <row r="99" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>712</v>
       </c>
@@ -15253,11 +15174,11 @@
       <c r="J99" s="49" t="s">
         <v>1035</v>
       </c>
-      <c r="K99" s="140" t="s">
-        <v>1699</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" ht="18">
+      <c r="K99" s="139" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B100" s="25"/>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -15281,11 +15202,11 @@
       <c r="J100" s="25" t="s">
         <v>1520</v>
       </c>
-      <c r="K100" s="139" t="s">
+      <c r="K100" s="138" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="18">
+    <row r="101" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B101" s="25"/>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -15307,11 +15228,11 @@
       <c r="J101" s="25" t="s">
         <v>527</v>
       </c>
-      <c r="K101" s="139" t="s">
+      <c r="K101" s="138" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="30">
+    <row r="102" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="25"/>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -15337,7 +15258,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18">
+    <row r="103" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B103" s="25" t="s">
         <v>712</v>
       </c>
@@ -15363,11 +15284,11 @@
       <c r="J103" s="25" t="s">
         <v>531</v>
       </c>
-      <c r="K103" s="139" t="s">
+      <c r="K103" s="138" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="104" spans="2:11" ht="18">
+    <row r="104" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B104" s="25" t="s">
         <v>712</v>
       </c>
@@ -15391,11 +15312,11 @@
       <c r="J104" s="25" t="s">
         <v>534</v>
       </c>
-      <c r="K104" s="139" t="s">
+      <c r="K104" s="138" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="105" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="9" t="s">
         <v>713</v>
       </c>
@@ -15425,7 +15346,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B106" s="9" t="s">
         <v>148</v>
       </c>
@@ -15451,7 +15372,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15479,7 +15400,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="9"/>
       <c r="C108" s="61" t="s">
         <v>7</v>
@@ -15503,7 +15424,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B109" s="9"/>
       <c r="C109" s="61" t="s">
         <v>7</v>
@@ -15527,7 +15448,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="9"/>
       <c r="C110" s="61" t="s">
         <v>7</v>
@@ -15551,7 +15472,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="9" t="s">
         <v>1263</v>
@@ -15575,11 +15496,11 @@
       <c r="J111" s="25" t="s">
         <v>716</v>
       </c>
-      <c r="K111" s="139" t="s">
+      <c r="K111" s="138" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
         <v>1263</v>
@@ -15603,11 +15524,11 @@
       <c r="J112" s="25" t="s">
         <v>545</v>
       </c>
-      <c r="K112" s="139" t="s">
+      <c r="K112" s="138" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="113" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="113" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B113" s="25"/>
       <c r="C113" s="9" t="s">
         <v>1263</v>
@@ -15631,11 +15552,11 @@
       <c r="J113" s="25" t="s">
         <v>774</v>
       </c>
-      <c r="K113" s="140" t="s">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11" s="1" customFormat="1" ht="45">
+      <c r="K113" s="139" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="61" t="s">
         <v>1554</v>
@@ -15661,7 +15582,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="115" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="61" t="s">
         <v>1554</v>
@@ -15689,7 +15610,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="116" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="61" t="s">
         <v>1554</v>
@@ -15715,7 +15636,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="117" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="117" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="61" t="s">
         <v>1554</v>
@@ -15741,7 +15662,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="118" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="118" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="61" t="s">
         <v>1554</v>
@@ -15767,7 +15688,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="119" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="119" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="61" t="s">
         <v>1554</v>
@@ -15793,7 +15714,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="120" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="61" t="s">
         <v>1554</v>
@@ -15819,7 +15740,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="121" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="61" t="s">
         <v>1554</v>
@@ -15845,7 +15766,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B122" s="9"/>
       <c r="C122" s="61" t="s">
         <v>1554</v>
@@ -15871,7 +15792,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="123" spans="2:11" s="1" customFormat="1" ht="60">
+    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
       <c r="C123" s="61" t="s">
         <v>1554</v>
@@ -15897,7 +15818,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="124" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="9"/>
       <c r="C124" s="61" t="s">
         <v>1554</v>
@@ -15923,7 +15844,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="125" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="125" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B125" s="9"/>
       <c r="C125" s="61" t="s">
         <v>1554</v>
@@ -15949,7 +15870,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="126" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="126" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B126" s="9"/>
       <c r="C126" s="61" t="s">
         <v>1554</v>
@@ -15977,7 +15898,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="127" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="127" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B127" s="9"/>
       <c r="C127" s="61" t="s">
         <v>1554</v>
@@ -16005,7 +15926,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="128" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="128" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="61" t="s">
         <v>1554</v>
@@ -16029,7 +15950,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B129" s="58"/>
       <c r="C129" s="61" t="s">
         <v>1554</v>
@@ -16055,7 +15976,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B130" s="9"/>
       <c r="C130" s="61" t="s">
         <v>1554</v>
@@ -16081,7 +16002,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="61" t="s">
         <v>1554</v>
@@ -16107,7 +16028,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="61" t="s">
         <v>1554</v>
@@ -16133,7 +16054,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B133" s="9"/>
       <c r="C133" s="61" t="s">
         <v>1554</v>
@@ -16159,7 +16080,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="61" t="s">
         <v>1554</v>
@@ -16185,7 +16106,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B135" s="9"/>
       <c r="C135" s="61" t="s">
         <v>1554</v>
@@ -16211,7 +16132,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B136" s="9"/>
       <c r="C136" s="61" t="s">
         <v>1554</v>
@@ -16235,7 +16156,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="9"/>
       <c r="C137" s="61" t="s">
         <v>1554</v>
@@ -16263,7 +16184,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="9"/>
       <c r="C138" s="61" t="s">
         <v>1554</v>
@@ -16289,7 +16210,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="59" customFormat="1" ht="18">
+    <row r="139" spans="2:11" s="59" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="61" t="s">
         <v>1554</v>
@@ -16313,7 +16234,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="61" t="s">
         <v>1554</v>
@@ -16337,7 +16258,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="s">
         <v>19</v>
       </c>
@@ -16365,7 +16286,7 @@
       </c>
       <c r="K141" s="85"/>
     </row>
-    <row r="142" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B142" s="8" t="s">
         <v>19</v>
       </c>
@@ -16395,7 +16316,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B143" s="8" t="s">
         <v>19</v>
       </c>
@@ -16425,7 +16346,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">
         <v>19</v>
       </c>
@@ -16455,7 +16376,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75">
+    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
         <v>19</v>
       </c>
@@ -16485,7 +16406,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75">
+    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
       <c r="C146" s="66" t="s">
         <v>60</v>
@@ -16513,7 +16434,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="147" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B147" s="9"/>
       <c r="C147" s="9" t="s">
         <v>60</v>
@@ -16541,7 +16462,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="148" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B148" s="9"/>
       <c r="C148" s="61" t="s">
         <v>60</v>
@@ -16569,7 +16490,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="149" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="9"/>
       <c r="C149" s="9" t="s">
         <v>60</v>
@@ -16597,7 +16518,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="150" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B150" s="9"/>
       <c r="C150" s="61" t="s">
         <v>60</v>
@@ -16623,7 +16544,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="151" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B151" s="9" t="s">
         <v>7</v>
       </c>
@@ -16653,7 +16574,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="152" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B152" s="9" t="s">
         <v>713</v>
       </c>
@@ -16681,7 +16602,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="153" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B153" s="9" t="s">
         <v>713</v>
       </c>
@@ -16709,7 +16630,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="154" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="63" t="s">
         <v>60</v>
@@ -16735,7 +16656,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="155" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B155" s="9" t="s">
         <v>1389</v>
       </c>
@@ -16763,7 +16684,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B156" s="9"/>
       <c r="C156" s="66" t="s">
         <v>719</v>
@@ -16789,7 +16710,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="157" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="9"/>
       <c r="C157" s="61" t="s">
         <v>719</v>
@@ -16817,7 +16738,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="158" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B158" s="9"/>
       <c r="C158" s="61" t="s">
         <v>719</v>
@@ -16845,7 +16766,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="159" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B159" s="45"/>
       <c r="C159" s="61" t="s">
         <v>719</v>
@@ -16873,7 +16794,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="160" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9" t="s">
         <v>719</v>
@@ -16901,7 +16822,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
         <v>719</v>
@@ -16929,7 +16850,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="61" t="s">
         <v>719</v>
@@ -16957,7 +16878,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="61" t="s">
         <v>719</v>
@@ -16985,7 +16906,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>717</v>
       </c>
@@ -17015,7 +16936,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>717</v>
       </c>
@@ -17045,7 +16966,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B166" s="9" t="s">
         <v>717</v>
       </c>
@@ -17075,7 +16996,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9" t="s">
         <v>719</v>
@@ -17103,7 +17024,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="61" t="s">
         <v>719</v>
@@ -17129,7 +17050,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
       <c r="C169" s="66" t="s">
         <v>719</v>
@@ -17157,7 +17078,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B170" s="45"/>
       <c r="C170" s="61" t="s">
         <v>719</v>
@@ -17183,7 +17104,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B171" s="9"/>
       <c r="C171" s="66" t="s">
         <v>719</v>
@@ -17209,7 +17130,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="1" customFormat="1" ht="45">
+    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B172" s="9"/>
       <c r="C172" s="9" t="s">
         <v>719</v>
@@ -17235,7 +17156,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>719</v>
       </c>
@@ -17265,7 +17186,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>719</v>
       </c>
@@ -17295,7 +17216,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B175" s="9"/>
       <c r="C175" s="61" t="s">
         <v>719</v>
@@ -17323,7 +17244,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="61" t="s">
         <v>719</v>
@@ -17349,7 +17270,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B177" s="9"/>
       <c r="C177" s="66" t="s">
         <v>719</v>
@@ -17375,7 +17296,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="178" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B178" s="9"/>
       <c r="C178" s="61" t="s">
         <v>719</v>
@@ -17403,7 +17324,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B179" s="9"/>
       <c r="C179" s="61" t="s">
         <v>719</v>
@@ -17431,7 +17352,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B180" s="9"/>
       <c r="C180" s="61" t="s">
         <v>719</v>
@@ -17459,7 +17380,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B181" s="9"/>
       <c r="C181" s="61" t="s">
         <v>719</v>
@@ -17487,7 +17408,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B182" s="9"/>
       <c r="C182" s="61" t="s">
         <v>719</v>
@@ -17515,7 +17436,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="183" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="183" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B183" s="9"/>
       <c r="C183" s="61" t="s">
         <v>719</v>
@@ -17543,7 +17464,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B184" s="9"/>
       <c r="C184" s="61" t="s">
         <v>719</v>
@@ -17571,7 +17492,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25">
+    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B185" s="9"/>
       <c r="C185" s="9" t="s">
         <v>60</v>
@@ -17601,7 +17522,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B186" s="9" t="s">
         <v>7</v>
       </c>
@@ -17627,7 +17548,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17653,7 +17574,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="188" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B188" s="9" t="s">
         <v>148</v>
       </c>
@@ -17679,7 +17600,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="189" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
         <v>148</v>
       </c>
@@ -17705,7 +17626,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B190" s="25"/>
       <c r="C190" s="9" t="s">
         <v>719</v>
@@ -17729,7 +17650,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B191" s="45"/>
       <c r="C191" s="9" t="s">
         <v>719</v>
@@ -17753,7 +17674,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
       <c r="C192" s="9" t="s">
         <v>719</v>
@@ -17777,7 +17698,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="193" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B193" s="9"/>
       <c r="C193" s="9" t="s">
         <v>719</v>
@@ -17801,7 +17722,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="194" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>719</v>
@@ -17825,7 +17746,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="195" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B195" s="9"/>
       <c r="C195" s="61" t="s">
         <v>719</v>
@@ -17849,7 +17770,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="196" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B196" s="9"/>
       <c r="C196" s="61" t="s">
         <v>719</v>
@@ -17873,7 +17794,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="197" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B197" s="9"/>
       <c r="C197" s="61" t="s">
         <v>719</v>
@@ -17897,7 +17818,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="198" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B198" s="9"/>
       <c r="C198" s="61" t="s">
         <v>719</v>
@@ -17921,7 +17842,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="199" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B199" s="9" t="s">
         <v>7</v>
       </c>
@@ -17951,7 +17872,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="200" spans="2:11" s="1" customFormat="1" ht="18">
+    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B200" s="9" t="s">
         <v>7</v>
       </c>
@@ -17981,7 +17902,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="201" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="61" t="s">
         <v>1627</v>
@@ -18005,7 +17926,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="202" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="61" t="s">
         <v>1627</v>
@@ -18029,7 +17950,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="203" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B203" s="9"/>
       <c r="C203" s="61" t="s">
         <v>1627</v>
@@ -18053,7 +17974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="204" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B204" s="9"/>
       <c r="C204" s="61" t="s">
         <v>1627</v>
@@ -18077,7 +17998,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="205" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B205" s="9"/>
       <c r="C205" s="61" t="s">
         <v>1627</v>
@@ -18101,7 +18022,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="206" spans="2:11" s="1" customFormat="1" ht="30">
+    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B206" s="9"/>
       <c r="C206" s="61" t="s">
         <v>1627</v>
@@ -18125,7 +18046,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="207" spans="2:11" ht="18">
+    <row r="207" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B207" s="69"/>
       <c r="C207" s="84" t="s">
         <v>1627</v>
@@ -18149,7 +18070,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="208" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="208" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B208" s="9"/>
       <c r="C208" s="61" t="s">
         <v>1627</v>
@@ -18173,7 +18094,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="209" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="209" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B209" s="45"/>
       <c r="C209" s="45"/>
       <c r="D209" s="45"/>
@@ -18185,7 +18106,7 @@
       <c r="J209" s="45"/>
       <c r="K209" s="54"/>
     </row>
-    <row r="210" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="210" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B210" s="25"/>
       <c r="C210" s="25"/>
       <c r="D210" s="25"/>
@@ -18197,7 +18118,7 @@
       <c r="J210" s="25"/>
       <c r="K210" s="54"/>
     </row>
-    <row r="211" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="211" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B211" s="25"/>
       <c r="C211" s="25"/>
       <c r="D211" s="25"/>
@@ -18209,7 +18130,7 @@
       <c r="J211" s="25"/>
       <c r="K211" s="54"/>
     </row>
-    <row r="212" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="212" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B212" s="25"/>
       <c r="C212" s="25"/>
       <c r="D212" s="25"/>
@@ -18221,7 +18142,7 @@
       <c r="J212" s="25"/>
       <c r="K212" s="54"/>
     </row>
-    <row r="213" spans="2:11" s="24" customFormat="1" ht="18">
+    <row r="213" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B213" s="25"/>
       <c r="C213" s="25"/>
       <c r="D213" s="25"/>
@@ -18233,7 +18154,7 @@
       <c r="J213" s="25"/>
       <c r="K213" s="54"/>
     </row>
-    <row r="214" spans="2:11">
+    <row r="214" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B214" s="45"/>
       <c r="C214" s="45"/>
       <c r="D214" s="45"/>
@@ -18245,7 +18166,7 @@
       <c r="J214" s="45"/>
       <c r="K214" s="54"/>
     </row>
-    <row r="215" spans="2:11">
+    <row r="215" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B215" s="45"/>
       <c r="C215" s="45"/>
       <c r="D215" s="45"/>
@@ -18257,7 +18178,7 @@
       <c r="J215" s="45"/>
       <c r="K215" s="54"/>
     </row>
-    <row r="216" spans="2:11">
+    <row r="216" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B216" s="45"/>
       <c r="C216" s="45"/>
       <c r="D216" s="45"/>
@@ -18269,7 +18190,7 @@
       <c r="J216" s="45"/>
       <c r="K216" s="54"/>
     </row>
-    <row r="217" spans="2:11">
+    <row r="217" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B217" s="45"/>
       <c r="C217" s="45"/>
       <c r="D217" s="45"/>
@@ -18281,7 +18202,7 @@
       <c r="J217" s="45"/>
       <c r="K217" s="54"/>
     </row>
-    <row r="218" spans="2:11">
+    <row r="218" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B218" s="45"/>
       <c r="C218" s="45"/>
       <c r="D218" s="45"/>
@@ -18293,7 +18214,7 @@
       <c r="J218" s="45"/>
       <c r="K218" s="54"/>
     </row>
-    <row r="219" spans="2:11">
+    <row r="219" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B219" s="45"/>
       <c r="C219" s="45"/>
       <c r="D219" s="45"/>
@@ -18305,7 +18226,7 @@
       <c r="J219" s="45"/>
       <c r="K219" s="54"/>
     </row>
-    <row r="220" spans="2:11">
+    <row r="220" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B220" s="45"/>
       <c r="C220" s="45"/>
       <c r="D220" s="45"/>
@@ -18317,7 +18238,7 @@
       <c r="J220" s="45"/>
       <c r="K220" s="54"/>
     </row>
-    <row r="221" spans="2:11">
+    <row r="221" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B221" s="45"/>
       <c r="C221" s="45"/>
       <c r="D221" s="45"/>
@@ -18329,7 +18250,7 @@
       <c r="J221" s="45"/>
       <c r="K221" s="54"/>
     </row>
-    <row r="222" spans="2:11">
+    <row r="222" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B222" s="45"/>
       <c r="C222" s="45"/>
       <c r="D222" s="45"/>
@@ -18341,7 +18262,7 @@
       <c r="J222" s="45"/>
       <c r="K222" s="54"/>
     </row>
-    <row r="223" spans="2:11">
+    <row r="223" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B223" s="45"/>
       <c r="C223" s="45"/>
       <c r="D223" s="45"/>
@@ -18353,7 +18274,7 @@
       <c r="J223" s="45"/>
       <c r="K223" s="54"/>
     </row>
-    <row r="224" spans="2:11">
+    <row r="224" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B224" s="45"/>
       <c r="C224" s="45"/>
       <c r="D224" s="45"/>
@@ -18365,7 +18286,7 @@
       <c r="J224" s="45"/>
       <c r="K224" s="54"/>
     </row>
-    <row r="225" spans="2:11">
+    <row r="225" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B225" s="45"/>
       <c r="C225" s="45"/>
       <c r="D225" s="45"/>
@@ -18377,7 +18298,7 @@
       <c r="J225" s="45"/>
       <c r="K225" s="54"/>
     </row>
-    <row r="226" spans="2:11">
+    <row r="226" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B226" s="45"/>
       <c r="C226" s="45"/>
       <c r="D226" s="45"/>
@@ -18389,7 +18310,7 @@
       <c r="J226" s="45"/>
       <c r="K226" s="54"/>
     </row>
-    <row r="227" spans="2:11">
+    <row r="227" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B227" s="45"/>
       <c r="C227" s="45"/>
       <c r="D227" s="45"/>
@@ -18401,7 +18322,7 @@
       <c r="J227" s="45"/>
       <c r="K227" s="54"/>
     </row>
-    <row r="228" spans="2:11">
+    <row r="228" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B228" s="45"/>
       <c r="C228" s="45"/>
       <c r="D228" s="45"/>
@@ -18413,7 +18334,7 @@
       <c r="J228" s="45"/>
       <c r="K228" s="54"/>
     </row>
-    <row r="229" spans="2:11">
+    <row r="229" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B229" s="45"/>
       <c r="C229" s="45"/>
       <c r="D229" s="45"/>
@@ -18425,7 +18346,7 @@
       <c r="J229" s="45"/>
       <c r="K229" s="54"/>
     </row>
-    <row r="230" spans="2:11">
+    <row r="230" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B230" s="45"/>
       <c r="C230" s="45"/>
       <c r="D230" s="45"/>
@@ -18437,7 +18358,7 @@
       <c r="J230" s="45"/>
       <c r="K230" s="54"/>
     </row>
-    <row r="231" spans="2:11">
+    <row r="231" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B231" s="45"/>
       <c r="C231" s="45"/>
       <c r="D231" s="45"/>
@@ -18449,7 +18370,7 @@
       <c r="J231" s="45"/>
       <c r="K231" s="54"/>
     </row>
-    <row r="232" spans="2:11">
+    <row r="232" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B232" s="45"/>
       <c r="C232" s="45"/>
       <c r="D232" s="45"/>
@@ -18461,7 +18382,7 @@
       <c r="J232" s="45"/>
       <c r="K232" s="54"/>
     </row>
-    <row r="233" spans="2:11">
+    <row r="233" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B233" s="45"/>
       <c r="C233" s="45"/>
       <c r="D233" s="45"/>
@@ -18473,7 +18394,7 @@
       <c r="J233" s="45"/>
       <c r="K233" s="54"/>
     </row>
-    <row r="234" spans="2:11">
+    <row r="234" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B234" s="45"/>
       <c r="C234" s="45"/>
       <c r="D234" s="45"/>
@@ -18485,7 +18406,7 @@
       <c r="J234" s="45"/>
       <c r="K234" s="54"/>
     </row>
-    <row r="235" spans="2:11">
+    <row r="235" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B235" s="45"/>
       <c r="C235" s="45"/>
       <c r="D235" s="45"/>
@@ -18497,7 +18418,7 @@
       <c r="J235" s="45"/>
       <c r="K235" s="54"/>
     </row>
-    <row r="236" spans="2:11">
+    <row r="236" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B236" s="45"/>
       <c r="C236" s="45"/>
       <c r="D236" s="45"/>
@@ -18509,7 +18430,7 @@
       <c r="J236" s="45"/>
       <c r="K236" s="54"/>
     </row>
-    <row r="237" spans="2:11">
+    <row r="237" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B237" s="45"/>
       <c r="C237" s="45"/>
       <c r="D237" s="45"/>
@@ -18521,7 +18442,7 @@
       <c r="J237" s="45"/>
       <c r="K237" s="54"/>
     </row>
-    <row r="238" spans="2:11">
+    <row r="238" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B238" s="45"/>
       <c r="C238" s="45"/>
       <c r="D238" s="45"/>
@@ -18533,7 +18454,7 @@
       <c r="J238" s="45"/>
       <c r="K238" s="54"/>
     </row>
-    <row r="239" spans="2:11">
+    <row r="239" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B239" s="45"/>
       <c r="C239" s="45"/>
       <c r="D239" s="45"/>
@@ -18545,7 +18466,7 @@
       <c r="J239" s="45"/>
       <c r="K239" s="54"/>
     </row>
-    <row r="240" spans="2:11">
+    <row r="240" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B240" s="45"/>
       <c r="C240" s="45"/>
       <c r="D240" s="45"/>
@@ -18557,7 +18478,7 @@
       <c r="J240" s="45"/>
       <c r="K240" s="54"/>
     </row>
-    <row r="241" spans="2:11">
+    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B241" s="45"/>
       <c r="C241" s="45"/>
       <c r="D241" s="45"/>
@@ -18569,7 +18490,7 @@
       <c r="J241" s="45"/>
       <c r="K241" s="54"/>
     </row>
-    <row r="242" spans="2:11">
+    <row r="242" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B242" s="45"/>
       <c r="C242" s="45"/>
       <c r="D242" s="45"/>
@@ -18581,7 +18502,7 @@
       <c r="J242" s="45"/>
       <c r="K242" s="54"/>
     </row>
-    <row r="243" spans="2:11">
+    <row r="243" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B243" s="45"/>
       <c r="C243" s="45"/>
       <c r="D243" s="45"/>
@@ -18593,7 +18514,7 @@
       <c r="J243" s="45"/>
       <c r="K243" s="54"/>
     </row>
-    <row r="244" spans="2:11">
+    <row r="244" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B244" s="45"/>
       <c r="C244" s="45"/>
       <c r="D244" s="45"/>
@@ -18605,7 +18526,7 @@
       <c r="J244" s="45"/>
       <c r="K244" s="54"/>
     </row>
-    <row r="245" spans="2:11">
+    <row r="245" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B245" s="45"/>
       <c r="C245" s="45"/>
       <c r="D245" s="45"/>
@@ -18617,7 +18538,7 @@
       <c r="J245" s="45"/>
       <c r="K245" s="54"/>
     </row>
-    <row r="246" spans="2:11">
+    <row r="246" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B246" s="45"/>
       <c r="C246" s="45"/>
       <c r="D246" s="45"/>
@@ -18629,7 +18550,7 @@
       <c r="J246" s="45"/>
       <c r="K246" s="54"/>
     </row>
-    <row r="247" spans="2:11">
+    <row r="247" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B247" s="45"/>
       <c r="C247" s="45"/>
       <c r="D247" s="45"/>
@@ -18641,7 +18562,7 @@
       <c r="J247" s="45"/>
       <c r="K247" s="54"/>
     </row>
-    <row r="248" spans="2:11">
+    <row r="248" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B248" s="45"/>
       <c r="C248" s="45"/>
       <c r="D248" s="45"/>
@@ -18653,7 +18574,7 @@
       <c r="J248" s="45"/>
       <c r="K248" s="54"/>
     </row>
-    <row r="249" spans="2:11">
+    <row r="249" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B249" s="45"/>
       <c r="C249" s="45"/>
       <c r="D249" s="45"/>
@@ -18665,7 +18586,7 @@
       <c r="J249" s="45"/>
       <c r="K249" s="54"/>
     </row>
-    <row r="250" spans="2:11">
+    <row r="250" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B250" s="45"/>
       <c r="C250" s="45"/>
       <c r="D250" s="45"/>
@@ -18677,7 +18598,7 @@
       <c r="J250" s="45"/>
       <c r="K250" s="54"/>
     </row>
-    <row r="251" spans="2:11">
+    <row r="251" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B251" s="45"/>
       <c r="C251" s="45"/>
       <c r="D251" s="45"/>
@@ -18689,7 +18610,7 @@
       <c r="J251" s="45"/>
       <c r="K251" s="54"/>
     </row>
-    <row r="252" spans="2:11">
+    <row r="252" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B252" s="45"/>
       <c r="C252" s="45"/>
       <c r="D252" s="45"/>
@@ -18701,7 +18622,7 @@
       <c r="J252" s="45"/>
       <c r="K252" s="54"/>
     </row>
-    <row r="253" spans="2:11">
+    <row r="253" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B253" s="45"/>
       <c r="C253" s="45"/>
       <c r="D253" s="45"/>
@@ -18713,7 +18634,7 @@
       <c r="J253" s="45"/>
       <c r="K253" s="54"/>
     </row>
-    <row r="254" spans="2:11">
+    <row r="254" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B254" s="45"/>
       <c r="C254" s="45"/>
       <c r="D254" s="45"/>
@@ -18725,7 +18646,7 @@
       <c r="J254" s="45"/>
       <c r="K254" s="54"/>
     </row>
-    <row r="255" spans="2:11">
+    <row r="255" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B255" s="45"/>
       <c r="C255" s="45"/>
       <c r="D255" s="45"/>
@@ -18737,7 +18658,7 @@
       <c r="J255" s="45"/>
       <c r="K255" s="54"/>
     </row>
-    <row r="256" spans="2:11">
+    <row r="256" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B256" s="45"/>
       <c r="C256" s="45"/>
       <c r="D256" s="45"/>
@@ -18749,7 +18670,7 @@
       <c r="J256" s="45"/>
       <c r="K256" s="54"/>
     </row>
-    <row r="257" spans="2:11">
+    <row r="257" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B257" s="45"/>
       <c r="C257" s="45"/>
       <c r="D257" s="45"/>
@@ -18761,7 +18682,7 @@
       <c r="J257" s="45"/>
       <c r="K257" s="54"/>
     </row>
-    <row r="258" spans="2:11">
+    <row r="258" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B258" s="45"/>
       <c r="C258" s="45"/>
       <c r="D258" s="45"/>
@@ -18773,7 +18694,7 @@
       <c r="J258" s="45"/>
       <c r="K258" s="54"/>
     </row>
-    <row r="259" spans="2:11">
+    <row r="259" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B259" s="45"/>
       <c r="C259" s="45"/>
       <c r="D259" s="45"/>
@@ -18785,7 +18706,7 @@
       <c r="J259" s="45"/>
       <c r="K259" s="54"/>
     </row>
-    <row r="260" spans="2:11">
+    <row r="260" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B260" s="45"/>
       <c r="C260" s="45"/>
       <c r="D260" s="45"/>
@@ -18797,7 +18718,7 @@
       <c r="J260" s="45"/>
       <c r="K260" s="54"/>
     </row>
-    <row r="261" spans="2:11">
+    <row r="261" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B261" s="45"/>
       <c r="C261" s="45"/>
       <c r="D261" s="45"/>
@@ -18809,7 +18730,7 @@
       <c r="J261" s="45"/>
       <c r="K261" s="54"/>
     </row>
-    <row r="262" spans="2:11">
+    <row r="262" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B262" s="45"/>
       <c r="C262" s="45"/>
       <c r="D262" s="45"/>
@@ -18821,7 +18742,7 @@
       <c r="J262" s="45"/>
       <c r="K262" s="54"/>
     </row>
-    <row r="263" spans="2:11">
+    <row r="263" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B263" s="45"/>
       <c r="C263" s="45"/>
       <c r="D263" s="45"/>
@@ -18833,7 +18754,7 @@
       <c r="J263" s="45"/>
       <c r="K263" s="54"/>
     </row>
-    <row r="264" spans="2:11">
+    <row r="264" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B264" s="45"/>
       <c r="C264" s="45"/>
       <c r="D264" s="45"/>
@@ -18845,7 +18766,7 @@
       <c r="J264" s="45"/>
       <c r="K264" s="54"/>
     </row>
-    <row r="265" spans="2:11">
+    <row r="265" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B265" s="45"/>
       <c r="C265" s="45"/>
       <c r="D265" s="45"/>
@@ -18857,7 +18778,7 @@
       <c r="J265" s="45"/>
       <c r="K265" s="54"/>
     </row>
-    <row r="266" spans="2:11">
+    <row r="266" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B266" s="45"/>
       <c r="C266" s="45"/>
       <c r="D266" s="45"/>
@@ -18869,7 +18790,7 @@
       <c r="J266" s="45"/>
       <c r="K266" s="54"/>
     </row>
-    <row r="267" spans="2:11">
+    <row r="267" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B267" s="45"/>
       <c r="C267" s="45"/>
       <c r="D267" s="45"/>
@@ -18881,7 +18802,7 @@
       <c r="J267" s="45"/>
       <c r="K267" s="54"/>
     </row>
-    <row r="268" spans="2:11">
+    <row r="268" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B268" s="45"/>
       <c r="C268" s="45"/>
       <c r="D268" s="45"/>
@@ -18893,7 +18814,7 @@
       <c r="J268" s="45"/>
       <c r="K268" s="54"/>
     </row>
-    <row r="269" spans="2:11">
+    <row r="269" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B269" s="45"/>
       <c r="C269" s="45"/>
       <c r="D269" s="45"/>

</xml_diff>

<commit_message>
Chamaka Ghanam and Template 1.1&4.7 12/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -6204,10 +6204,10 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12517,7 +12517,7 @@
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1 MA vrikshi and Jatai files 15/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,11 +6203,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F52" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K54" sqref="K54"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12512,8 +12512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>

</xml_diff>

<commit_message>
TS Jatai working as on 16/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,11 +6203,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12512,12 +12512,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS Jatai Working Updates 23/08/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,7 +6203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -12512,12 +12512,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jatai Working files+Chamaka Jatai Tamil 01/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -12513,11 +12513,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I96" sqref="I96"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jatai working files,template changes
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,11 +6203,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12512,12 +12512,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jatai Changes Raja/Venkat 20/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,11 +6203,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F160" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I108" sqref="I108"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12512,12 +12512,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes as on 21/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6203,8 +6203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F160" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
@@ -12512,8 +12512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="K143" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>

</xml_diff>

<commit_message>
TS Pada, Krama, Template input changes 28/112020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -5287,13 +5287,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -5624,303 +5630,304 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6204,10 +6211,10 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K103" sqref="K103"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12513,11 +12520,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12733,7 +12740,7 @@
       <c r="I10" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="146" t="s">
         <v>733</v>
       </c>
       <c r="K10" s="53" t="s">

</xml_diff>

<commit_message>
Padam Template and GS 10/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -5287,13 +5287,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -5632,302 +5638,302 @@
   </cellStyleXfs>
   <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6211,10 +6217,10 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomRight" activeCell="I161" sqref="I161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Padam Template Edits 16/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -5637,7 +5637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5825,7 +5825,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5936,6 +5935,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6218,11 +6226,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I174" sqref="I174"/>
+      <selection pane="bottomRight" activeCell="J129" sqref="J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,7 +6552,7 @@
       <c r="J10" s="48" t="s">
         <v>442</v>
       </c>
-      <c r="K10" s="112" t="s">
+      <c r="K10" s="111" t="s">
         <v>190</v>
       </c>
       <c r="L10" s="1"/>
@@ -6759,7 +6767,7 @@
       <c r="I16" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="J16" s="101" t="s">
+      <c r="J16" s="150" t="s">
         <v>424</v>
       </c>
       <c r="K16" s="11"/>
@@ -6793,7 +6801,7 @@
       <c r="I17" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="59" t="s">
         <v>425</v>
       </c>
       <c r="K17" s="37" t="s">
@@ -6829,10 +6837,10 @@
       <c r="I18" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="59" t="s">
         <v>427</v>
       </c>
-      <c r="K18" s="116" t="s">
+      <c r="K18" s="115" t="s">
         <v>164</v>
       </c>
       <c r="L18" s="1"/>
@@ -6940,7 +6948,7 @@
       <c r="J21" s="25" t="s">
         <v>430</v>
       </c>
-      <c r="K21" s="109" t="s">
+      <c r="K21" s="108" t="s">
         <v>167</v>
       </c>
       <c r="L21" s="1"/>
@@ -7045,7 +7053,7 @@
       <c r="I24" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="59" t="s">
         <v>426</v>
       </c>
       <c r="K24" s="37" t="s">
@@ -7159,10 +7167,10 @@
       <c r="I27" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="59" t="s">
         <v>423</v>
       </c>
-      <c r="K27" s="120" t="s">
+      <c r="K27" s="119" t="s">
         <v>161</v>
       </c>
       <c r="L27" s="1"/>
@@ -7414,7 +7422,7 @@
         <v>160</v>
       </c>
       <c r="H34" s="11"/>
-      <c r="I34" s="11" t="s">
+      <c r="I34" s="74" t="s">
         <v>287</v>
       </c>
       <c r="J34" s="25" t="s">
@@ -7568,7 +7576,7 @@
       <c r="J38" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="K38" s="109" t="s">
+      <c r="K38" s="108" t="s">
         <v>200</v>
       </c>
       <c r="L38" s="1"/>
@@ -7822,7 +7830,7 @@
       <c r="J45" s="25" t="s">
         <v>1355</v>
       </c>
-      <c r="K45" s="103" t="s">
+      <c r="K45" s="102" t="s">
         <v>211</v>
       </c>
       <c r="L45" s="1"/>
@@ -8002,7 +8010,7 @@
       <c r="J50" s="25" t="s">
         <v>454</v>
       </c>
-      <c r="K50" s="109" t="s">
+      <c r="K50" s="108" t="s">
         <v>202</v>
       </c>
       <c r="L50" s="1"/>
@@ -8040,7 +8048,7 @@
       <c r="J51" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="K51" s="106" t="s">
+      <c r="K51" s="105" t="s">
         <v>216</v>
       </c>
       <c r="L51" s="1"/>
@@ -8113,7 +8121,7 @@
       <c r="I53" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="J53" s="25" t="s">
+      <c r="J53" s="59" t="s">
         <v>453</v>
       </c>
       <c r="K53" s="37" t="s">
@@ -8230,7 +8238,7 @@
       <c r="J56" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="K56" s="121" t="s">
+      <c r="K56" s="120" t="s">
         <v>156</v>
       </c>
       <c r="L56" s="1"/>
@@ -8463,7 +8471,7 @@
     </row>
     <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="135" t="s">
+      <c r="B63" s="134" t="s">
         <v>15</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -8483,7 +8491,7 @@
       <c r="I63" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J63" s="132" t="s">
+      <c r="J63" s="131" t="s">
         <v>346</v>
       </c>
       <c r="K63" s="34" t="s">
@@ -8499,7 +8507,7 @@
     </row>
     <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="135" t="s">
+      <c r="B64" s="134" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -8519,7 +8527,7 @@
       <c r="I64" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J64" s="132" t="s">
+      <c r="J64" s="131" t="s">
         <v>347</v>
       </c>
       <c r="K64" s="34" t="s">
@@ -8535,7 +8543,7 @@
     </row>
     <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="135" t="s">
+      <c r="B65" s="134" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -8555,7 +8563,7 @@
       <c r="I65" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J65" s="132" t="s">
+      <c r="J65" s="131" t="s">
         <v>345</v>
       </c>
       <c r="K65" s="34" t="s">
@@ -8571,7 +8579,7 @@
     </row>
     <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="135" t="s">
+      <c r="B66" s="134" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -8589,7 +8597,7 @@
       <c r="I66" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J66" s="132" t="s">
+      <c r="J66" s="131" t="s">
         <v>1696</v>
       </c>
       <c r="K66" s="34" t="s">
@@ -8704,7 +8712,7 @@
       <c r="J69" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="K69" s="114" t="s">
+      <c r="K69" s="113" t="s">
         <v>105</v>
       </c>
       <c r="L69" s="1"/>
@@ -8742,7 +8750,7 @@
       <c r="J70" s="25" t="s">
         <v>813</v>
       </c>
-      <c r="K70" s="115"/>
+      <c r="K70" s="114"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -9120,7 +9128,7 @@
       <c r="J80" s="25" t="s">
         <v>412</v>
       </c>
-      <c r="K80" s="107" t="s">
+      <c r="K80" s="106" t="s">
         <v>140</v>
       </c>
       <c r="L80" s="1"/>
@@ -9136,7 +9144,7 @@
       <c r="B81" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C81" s="122" t="s">
+      <c r="C81" s="121" t="s">
         <v>1401</v>
       </c>
       <c r="D81" s="9" t="s">
@@ -9312,7 +9320,7 @@
       <c r="J85" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="K85" s="103" t="s">
+      <c r="K85" s="102" t="s">
         <v>189</v>
       </c>
       <c r="L85" s="1"/>
@@ -9350,7 +9358,7 @@
       <c r="J86" s="25" t="s">
         <v>440</v>
       </c>
-      <c r="K86" s="103" t="s">
+      <c r="K86" s="102" t="s">
         <v>188</v>
       </c>
       <c r="L86" s="1"/>
@@ -9520,11 +9528,11 @@
       <c r="F91" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="G91" s="91"/>
-      <c r="H91" s="11" t="s">
+      <c r="G91" s="147"/>
+      <c r="H91" s="148" t="s">
         <v>90</v>
       </c>
-      <c r="I91" s="21" t="s">
+      <c r="I91" s="149" t="s">
         <v>267</v>
       </c>
       <c r="J91" s="100" t="s">
@@ -9714,7 +9722,7 @@
       <c r="J96" s="25" t="s">
         <v>411</v>
       </c>
-      <c r="K96" s="103" t="s">
+      <c r="K96" s="102" t="s">
         <v>260</v>
       </c>
       <c r="L96" s="1"/>
@@ -9937,7 +9945,7 @@
       <c r="I102" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="J102" s="25" t="s">
+      <c r="J102" s="59" t="s">
         <v>393</v>
       </c>
       <c r="K102" s="35" t="s">
@@ -9978,7 +9986,7 @@
       <c r="J103" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="K103" s="145" t="s">
+      <c r="K103" s="144" t="s">
         <v>115</v>
       </c>
       <c r="L103" s="1"/>
@@ -10054,7 +10062,7 @@
       <c r="J105" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="K105" s="141" t="s">
+      <c r="K105" s="140" t="s">
         <v>111</v>
       </c>
       <c r="L105" s="1"/>
@@ -10130,7 +10138,7 @@
       <c r="J107" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="K107" s="136" t="s">
+      <c r="K107" s="135" t="s">
         <v>112</v>
       </c>
       <c r="L107" s="1"/>
@@ -10168,7 +10176,7 @@
       <c r="J108" s="25" t="s">
         <v>387</v>
       </c>
-      <c r="K108" s="144" t="s">
+      <c r="K108" s="143" t="s">
         <v>114</v>
       </c>
       <c r="L108" s="1"/>
@@ -10204,7 +10212,7 @@
       <c r="J109" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="K109" s="143" t="s">
+      <c r="K109" s="142" t="s">
         <v>116</v>
       </c>
       <c r="L109" s="1"/>
@@ -10242,7 +10250,7 @@
       <c r="J110" s="47" t="s">
         <v>1341</v>
       </c>
-      <c r="K110" s="142" t="s">
+      <c r="K110" s="141" t="s">
         <v>117</v>
       </c>
       <c r="L110" s="1"/>
@@ -10278,7 +10286,7 @@
       <c r="J111" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="K111" s="142" t="s">
+      <c r="K111" s="141" t="s">
         <v>118</v>
       </c>
       <c r="L111" s="1"/>
@@ -10316,7 +10324,7 @@
       <c r="J112" s="25" t="s">
         <v>397</v>
       </c>
-      <c r="K112" s="110" t="s">
+      <c r="K112" s="109" t="s">
         <v>130</v>
       </c>
       <c r="L112" s="1"/>
@@ -10344,7 +10352,7 @@
       <c r="F113" s="89" t="s">
         <v>1668</v>
       </c>
-      <c r="G113" s="131" t="s">
+      <c r="G113" s="130" t="s">
         <v>1673</v>
       </c>
       <c r="H113" s="11" t="s">
@@ -10356,7 +10364,7 @@
       <c r="J113" s="99" t="s">
         <v>392</v>
       </c>
-      <c r="K113" s="139" t="s">
+      <c r="K113" s="138" t="s">
         <v>121</v>
       </c>
       <c r="L113" s="1"/>
@@ -10384,7 +10392,7 @@
       <c r="F114" s="60" t="s">
         <v>1668</v>
       </c>
-      <c r="G114" s="131" t="s">
+      <c r="G114" s="130" t="s">
         <v>1673</v>
       </c>
       <c r="H114" s="11" t="s">
@@ -10396,7 +10404,7 @@
       <c r="J114" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="K114" s="140" t="s">
+      <c r="K114" s="139" t="s">
         <v>120</v>
       </c>
       <c r="L114" s="1"/>
@@ -10434,7 +10442,7 @@
       <c r="J115" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="K115" s="141" t="s">
+      <c r="K115" s="140" t="s">
         <v>119</v>
       </c>
       <c r="L115" s="1"/>
@@ -10470,7 +10478,7 @@
       <c r="J116" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="K116" s="111" t="s">
+      <c r="K116" s="110" t="s">
         <v>129</v>
       </c>
       <c r="L116" s="1"/>
@@ -10581,7 +10589,7 @@
       <c r="I119" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J119" s="132" t="s">
+      <c r="J119" s="131" t="s">
         <v>348</v>
       </c>
       <c r="K119" s="36" t="s">
@@ -10617,7 +10625,7 @@
       <c r="I120" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J120" s="132" t="s">
+      <c r="J120" s="131" t="s">
         <v>349</v>
       </c>
       <c r="K120" s="31"/>
@@ -10651,7 +10659,7 @@
       <c r="I121" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J121" s="132" t="s">
+      <c r="J121" s="131" t="s">
         <v>350</v>
       </c>
       <c r="K121" s="31"/>
@@ -10685,7 +10693,7 @@
       <c r="I122" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J122" s="132" t="s">
+      <c r="J122" s="131" t="s">
         <v>350</v>
       </c>
       <c r="K122" s="31"/>
@@ -10719,10 +10727,10 @@
       <c r="I123" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J123" s="132" t="s">
+      <c r="J123" s="131" t="s">
         <v>562</v>
       </c>
-      <c r="K123" s="108"/>
+      <c r="K123" s="107"/>
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
@@ -10753,10 +10761,10 @@
       <c r="I124" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J124" s="132" t="s">
+      <c r="J124" s="131" t="s">
         <v>563</v>
       </c>
-      <c r="K124" s="104"/>
+      <c r="K124" s="103"/>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
@@ -10787,10 +10795,10 @@
       <c r="I125" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J125" s="132" t="s">
+      <c r="J125" s="131" t="s">
         <v>352</v>
       </c>
-      <c r="K125" s="108"/>
+      <c r="K125" s="107"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
@@ -10821,10 +10829,10 @@
       <c r="I126" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="J126" s="132" t="s">
+      <c r="J126" s="131" t="s">
         <v>354</v>
       </c>
-      <c r="K126" s="104"/>
+      <c r="K126" s="103"/>
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
@@ -10855,10 +10863,10 @@
       <c r="I127" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J127" s="132" t="s">
+      <c r="J127" s="131" t="s">
         <v>355</v>
       </c>
-      <c r="K127" s="104"/>
+      <c r="K127" s="103"/>
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
@@ -10889,10 +10897,10 @@
       <c r="I128" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="J128" s="132" t="s">
+      <c r="J128" s="131" t="s">
         <v>355</v>
       </c>
-      <c r="K128" s="104"/>
+      <c r="K128" s="103"/>
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
@@ -10923,10 +10931,10 @@
       <c r="I129" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J129" s="25" t="s">
+      <c r="J129" s="59" t="s">
         <v>356</v>
       </c>
-      <c r="K129" s="108"/>
+      <c r="K129" s="107"/>
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
@@ -10962,7 +10970,7 @@
       <c r="J130" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="K130" s="113"/>
+      <c r="K130" s="112"/>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
@@ -11100,7 +11108,7 @@
       <c r="J134" s="25" t="s">
         <v>361</v>
       </c>
-      <c r="K134" s="115"/>
+      <c r="K134" s="114"/>
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
@@ -11131,7 +11139,7 @@
       <c r="I135" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J135" s="25" t="s">
+      <c r="J135" s="59" t="s">
         <v>366</v>
       </c>
       <c r="K135" s="31"/>
@@ -11270,7 +11278,7 @@
       <c r="J139" s="25" t="s">
         <v>365</v>
       </c>
-      <c r="K139" s="104"/>
+      <c r="K139" s="103"/>
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
@@ -11304,7 +11312,7 @@
       <c r="J140" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="K140" s="104" t="s">
+      <c r="K140" s="103" t="s">
         <v>817</v>
       </c>
       <c r="L140" s="1"/>
@@ -11342,7 +11350,7 @@
       <c r="J141" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="K141" s="113"/>
+      <c r="K141" s="112"/>
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
@@ -11445,7 +11453,7 @@
       <c r="I144" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J144" s="97" t="s">
+      <c r="J144" s="151" t="s">
         <v>815</v>
       </c>
       <c r="K144" s="11"/>
@@ -11636,7 +11644,7 @@
       <c r="J149" s="25" t="s">
         <v>368</v>
       </c>
-      <c r="K149" s="119" t="s">
+      <c r="K149" s="118" t="s">
         <v>64</v>
       </c>
       <c r="M149" s="1"/>
@@ -11673,7 +11681,7 @@
       <c r="J150" s="25" t="s">
         <v>370</v>
       </c>
-      <c r="K150" s="105" t="s">
+      <c r="K150" s="104" t="s">
         <v>66</v>
       </c>
       <c r="M150" s="1"/>
@@ -11708,7 +11716,7 @@
       <c r="J151" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="K151" s="118" t="s">
+      <c r="K151" s="117" t="s">
         <v>63</v>
       </c>
       <c r="M151" s="1"/>
@@ -11880,7 +11888,7 @@
       <c r="I156" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="J156" s="25" t="s">
+      <c r="J156" s="59" t="s">
         <v>374</v>
       </c>
       <c r="K156" s="19" t="s">
@@ -12025,7 +12033,7 @@
       <c r="J160" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="K160" s="109" t="s">
+      <c r="K160" s="108" t="s">
         <v>179</v>
       </c>
       <c r="M160" s="1"/>
@@ -12062,7 +12070,7 @@
       <c r="J161" s="25" t="s">
         <v>564</v>
       </c>
-      <c r="K161" s="119" t="s">
+      <c r="K161" s="118" t="s">
         <v>145</v>
       </c>
       <c r="M161" s="1"/>
@@ -12097,7 +12105,7 @@
       <c r="J162" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="K162" s="110" t="s">
+      <c r="K162" s="109" t="s">
         <v>76</v>
       </c>
       <c r="M162" s="1"/>
@@ -12130,7 +12138,7 @@
       <c r="J163" s="25" t="s">
         <v>338</v>
       </c>
-      <c r="K163" s="102" t="s">
+      <c r="K163" s="101" t="s">
         <v>792</v>
       </c>
       <c r="M163" s="1"/>
@@ -12163,7 +12171,7 @@
       <c r="J164" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="K164" s="117" t="s">
+      <c r="K164" s="116" t="s">
         <v>11</v>
       </c>
       <c r="M164" s="1"/>
@@ -12196,7 +12204,7 @@
       <c r="J165" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="K165" s="110" t="s">
+      <c r="K165" s="109" t="s">
         <v>108</v>
       </c>
       <c r="M165" s="1"/>
@@ -12231,7 +12239,7 @@
       <c r="J166" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="K166" s="110" t="s">
+      <c r="K166" s="109" t="s">
         <v>109</v>
       </c>
       <c r="M166" s="1"/>
@@ -12262,7 +12270,7 @@
       <c r="J167" s="25" t="s">
         <v>656</v>
       </c>
-      <c r="K167" s="110"/>
+      <c r="K167" s="109"/>
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
       <c r="O167" s="1"/>
@@ -12295,7 +12303,7 @@
       <c r="J168" s="25" t="s">
         <v>1478</v>
       </c>
-      <c r="K168" s="110" t="s">
+      <c r="K168" s="109" t="s">
         <v>92</v>
       </c>
       <c r="M168" s="1"/>
@@ -12330,7 +12338,7 @@
       <c r="J169" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="K169" s="110" t="s">
+      <c r="K169" s="109" t="s">
         <v>93</v>
       </c>
       <c r="M169" s="1"/>
@@ -12365,7 +12373,7 @@
       <c r="J170" s="25" t="s">
         <v>798</v>
       </c>
-      <c r="K170" s="119" t="s">
+      <c r="K170" s="118" t="s">
         <v>94</v>
       </c>
       <c r="L170" s="1"/>
@@ -12401,7 +12409,7 @@
       <c r="J171" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="K171" s="110" t="s">
+      <c r="K171" s="109" t="s">
         <v>95</v>
       </c>
       <c r="L171" s="1"/>
@@ -12437,7 +12445,7 @@
       <c r="J172" s="25" t="s">
         <v>1479</v>
       </c>
-      <c r="K172" s="107" t="s">
+      <c r="K172" s="106" t="s">
         <v>96</v>
       </c>
       <c r="L172" s="1"/>
@@ -12527,12 +12535,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="J139" sqref="J139"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12545,7 +12553,7 @@
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="77.85546875" style="129" customWidth="1"/>
+    <col min="11" max="11" width="77.85546875" style="128" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
@@ -12748,7 +12756,7 @@
       <c r="I10" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="J10" s="146" t="s">
+      <c r="J10" s="145" t="s">
         <v>732</v>
       </c>
       <c r="K10" s="53" t="s">
@@ -12794,7 +12802,7 @@
       <c r="E12" s="60" t="s">
         <v>1301</v>
       </c>
-      <c r="F12" s="128" t="s">
+      <c r="F12" s="127" t="s">
         <v>1631</v>
       </c>
       <c r="G12" s="60" t="s">
@@ -12919,7 +12927,7 @@
         <v>1048</v>
       </c>
       <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="60" t="s">
         <v>542</v>
       </c>
       <c r="J16" s="97" t="s">
@@ -12975,7 +12983,7 @@
         <v>1054</v>
       </c>
       <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="60" t="s">
         <v>582</v>
       </c>
       <c r="J18" s="25" t="s">
@@ -13230,7 +13238,7 @@
       <c r="G27" s="60" t="s">
         <v>1056</v>
       </c>
-      <c r="H27" s="124" t="s">
+      <c r="H27" s="123" t="s">
         <v>1568</v>
       </c>
       <c r="I27" s="9" t="s">
@@ -13260,7 +13268,7 @@
       <c r="G28" s="60" t="s">
         <v>1056</v>
       </c>
-      <c r="H28" s="124" t="s">
+      <c r="H28" s="123" t="s">
         <v>1568</v>
       </c>
       <c r="I28" s="9" t="s">
@@ -13313,7 +13321,7 @@
         <v>1092</v>
       </c>
       <c r="H30" s="9"/>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="60" t="s">
         <v>542</v>
       </c>
       <c r="J30" s="25" t="s">
@@ -13365,7 +13373,7 @@
         <v>1092</v>
       </c>
       <c r="H32" s="9"/>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="60" t="s">
         <v>233</v>
       </c>
       <c r="J32" s="25" t="s">
@@ -13655,7 +13663,7 @@
         <v>1585</v>
       </c>
       <c r="H43" s="9"/>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="60" t="s">
         <v>1595</v>
       </c>
       <c r="J43" s="24" t="s">
@@ -13849,7 +13857,7 @@
       <c r="F50" s="62" t="s">
         <v>1488</v>
       </c>
-      <c r="G50" s="133" t="s">
+      <c r="G50" s="132" t="s">
         <v>1023</v>
       </c>
       <c r="H50" s="9"/>
@@ -13879,7 +13887,7 @@
       <c r="F51" s="62" t="s">
         <v>1483</v>
       </c>
-      <c r="G51" s="133" t="s">
+      <c r="G51" s="132" t="s">
         <v>1023</v>
       </c>
       <c r="H51" s="17"/>
@@ -13909,7 +13917,7 @@
       <c r="F52" s="62" t="s">
         <v>1484</v>
       </c>
-      <c r="G52" s="133" t="s">
+      <c r="G52" s="132" t="s">
         <v>1023</v>
       </c>
       <c r="H52" s="9"/>
@@ -13939,7 +13947,7 @@
       <c r="F53" s="62" t="s">
         <v>1486</v>
       </c>
-      <c r="G53" s="133" t="s">
+      <c r="G53" s="132" t="s">
         <v>1070</v>
       </c>
       <c r="H53" s="9"/>
@@ -13971,7 +13979,7 @@
         <v>1021</v>
       </c>
       <c r="H54" s="9"/>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="60" t="s">
         <v>18</v>
       </c>
       <c r="J54" s="48" t="s">
@@ -13988,7 +13996,7 @@
       <c r="C55" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="134" t="s">
+      <c r="D55" s="133" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="60"/>
@@ -14051,7 +14059,7 @@
         <v>1074</v>
       </c>
       <c r="H57" s="9"/>
-      <c r="I57" s="9" t="s">
+      <c r="I57" s="60" t="s">
         <v>32</v>
       </c>
       <c r="J57" s="25" t="s">
@@ -14393,7 +14401,7 @@
       <c r="J70" s="25" t="s">
         <v>524</v>
       </c>
-      <c r="K70" s="127" t="s">
+      <c r="K70" s="126" t="s">
         <v>867</v>
       </c>
     </row>
@@ -14725,7 +14733,7 @@
       <c r="J82" s="97" t="s">
         <v>514</v>
       </c>
-      <c r="K82" s="127" t="s">
+      <c r="K82" s="126" t="s">
         <v>860</v>
       </c>
     </row>
@@ -15127,13 +15135,13 @@
         <v>1033</v>
       </c>
       <c r="H97" s="9"/>
-      <c r="I97" s="9" t="s">
+      <c r="I97" s="60" t="s">
         <v>233</v>
       </c>
       <c r="J97" s="25" t="s">
         <v>502</v>
       </c>
-      <c r="K97" s="137" t="s">
+      <c r="K97" s="136" t="s">
         <v>849</v>
       </c>
     </row>
@@ -15189,7 +15197,7 @@
       <c r="J99" s="48" t="s">
         <v>1034</v>
       </c>
-      <c r="K99" s="138" t="s">
+      <c r="K99" s="137" t="s">
         <v>1697</v>
       </c>
     </row>
@@ -15217,7 +15225,7 @@
       <c r="J100" s="25" t="s">
         <v>1519</v>
       </c>
-      <c r="K100" s="137" t="s">
+      <c r="K100" s="136" t="s">
         <v>875</v>
       </c>
     </row>
@@ -15243,7 +15251,7 @@
       <c r="J101" s="25" t="s">
         <v>526</v>
       </c>
-      <c r="K101" s="137" t="s">
+      <c r="K101" s="136" t="s">
         <v>869</v>
       </c>
     </row>
@@ -15299,7 +15307,7 @@
       <c r="J103" s="25" t="s">
         <v>530</v>
       </c>
-      <c r="K103" s="137" t="s">
+      <c r="K103" s="136" t="s">
         <v>871</v>
       </c>
     </row>
@@ -15327,7 +15335,7 @@
       <c r="J104" s="25" t="s">
         <v>533</v>
       </c>
-      <c r="K104" s="137" t="s">
+      <c r="K104" s="136" t="s">
         <v>874</v>
       </c>
     </row>
@@ -15511,7 +15519,7 @@
       <c r="J111" s="25" t="s">
         <v>715</v>
       </c>
-      <c r="K111" s="137" t="s">
+      <c r="K111" s="136" t="s">
         <v>881</v>
       </c>
     </row>
@@ -15539,7 +15547,7 @@
       <c r="J112" s="25" t="s">
         <v>544</v>
       </c>
-      <c r="K112" s="137" t="s">
+      <c r="K112" s="136" t="s">
         <v>882</v>
       </c>
     </row>
@@ -15567,7 +15575,7 @@
       <c r="J113" s="25" t="s">
         <v>773</v>
       </c>
-      <c r="K113" s="138" t="s">
+      <c r="K113" s="137" t="s">
         <v>1698</v>
       </c>
     </row>
@@ -15984,10 +15992,10 @@
       <c r="I129" s="57" t="s">
         <v>623</v>
       </c>
-      <c r="J129" s="126" t="s">
+      <c r="J129" s="125" t="s">
         <v>743</v>
       </c>
-      <c r="K129" s="130" t="s">
+      <c r="K129" s="129" t="s">
         <v>945</v>
       </c>
     </row>
@@ -16085,7 +16093,7 @@
         <v>1069</v>
       </c>
       <c r="H133" s="9"/>
-      <c r="I133" s="9" t="s">
+      <c r="I133" s="60" t="s">
         <v>233</v>
       </c>
       <c r="J133" s="25" t="s">
@@ -16381,7 +16389,7 @@
         <v>1025</v>
       </c>
       <c r="H144" s="9"/>
-      <c r="I144" s="9" t="s">
+      <c r="I144" s="60" t="s">
         <v>32</v>
       </c>
       <c r="J144" s="25" t="s">
@@ -16432,7 +16440,7 @@
       <c r="E146" s="9" t="s">
         <v>1416</v>
       </c>
-      <c r="F146" s="125" t="s">
+      <c r="F146" s="124" t="s">
         <v>1581</v>
       </c>
       <c r="G146" s="60" t="s">
@@ -16792,7 +16800,7 @@
       <c r="E159" s="60" t="s">
         <v>1539</v>
       </c>
-      <c r="F159" s="123" t="s">
+      <c r="F159" s="122" t="s">
         <v>1540</v>
       </c>
       <c r="G159" s="60" t="s">
@@ -17019,7 +17027,7 @@
       <c r="D167" s="9" t="s">
         <v>1407</v>
       </c>
-      <c r="E167" s="123" t="s">
+      <c r="E167" s="122" t="s">
         <v>1537</v>
       </c>
       <c r="F167" s="60" t="s">
@@ -17605,7 +17613,7 @@
         <v>1032</v>
       </c>
       <c r="H188" s="9"/>
-      <c r="I188" s="147" t="s">
+      <c r="I188" s="146" t="s">
         <v>235</v>
       </c>
       <c r="J188" s="25" t="s">
@@ -17703,7 +17711,7 @@
         <v>1047</v>
       </c>
       <c r="H192" s="9"/>
-      <c r="I192" s="9" t="s">
+      <c r="I192" s="60" t="s">
         <v>537</v>
       </c>
       <c r="J192" s="25" t="s">
@@ -18081,7 +18089,7 @@
       <c r="J207" s="97" t="s">
         <v>757</v>
       </c>
-      <c r="K207" s="127" t="s">
+      <c r="K207" s="126" t="s">
         <v>1002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest in Ghanam etc 24/02/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA0E39-79AD-4579-B42E-63A5E59D1D50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5205"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -5287,7 +5288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6229,11 +6230,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -6312,7 +6312,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>131</v>
@@ -6348,7 +6348,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>131</v>
@@ -6384,7 +6384,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>131</v>
@@ -6420,7 +6420,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
         <v>148</v>
@@ -6458,7 +6458,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>148</v>
@@ -6496,7 +6496,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>148</v>
@@ -6534,7 +6534,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>148</v>
@@ -6570,7 +6570,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>148</v>
@@ -6608,7 +6608,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>148</v>
@@ -6648,7 +6648,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>148</v>
@@ -6686,7 +6686,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>148</v>
@@ -6724,7 +6724,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>148</v>
@@ -6750,7 +6750,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>148</v>
@@ -6786,7 +6786,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>148</v>
@@ -6822,7 +6822,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>148</v>
@@ -6858,7 +6858,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -6894,7 +6894,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>148</v>
@@ -6930,7 +6930,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
         <v>148</v>
@@ -6966,7 +6966,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
         <v>148</v>
@@ -7002,7 +7002,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="s">
         <v>148</v>
@@ -7038,7 +7038,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>148</v>
@@ -7074,7 +7074,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>148</v>
@@ -7112,7 +7112,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
         <v>148</v>
@@ -7150,7 +7150,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
         <v>148</v>
@@ -7188,7 +7188,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9" t="s">
         <v>148</v>
@@ -7262,7 +7262,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>148</v>
@@ -7298,7 +7298,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9" t="s">
         <v>148</v>
@@ -7336,7 +7336,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>148</v>
@@ -7374,7 +7374,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
         <v>148</v>
@@ -7410,7 +7410,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="75.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="9" t="s">
         <v>148</v>
@@ -7446,7 +7446,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="9" t="s">
         <v>148</v>
@@ -7484,7 +7484,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
         <v>148</v>
@@ -7522,7 +7522,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="9" t="s">
         <v>148</v>
@@ -7558,7 +7558,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="9" t="s">
         <v>148</v>
@@ -7594,7 +7594,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
         <v>148</v>
@@ -7632,7 +7632,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
         <v>148</v>
@@ -7704,7 +7704,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>148</v>
@@ -7740,7 +7740,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
         <v>148</v>
@@ -7776,7 +7776,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="9" t="s">
         <v>148</v>
@@ -7812,7 +7812,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
         <v>148</v>
@@ -7848,7 +7848,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="9" t="s">
         <v>148</v>
@@ -7882,7 +7882,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="9" t="s">
         <v>148</v>
@@ -7920,7 +7920,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
         <v>148</v>
@@ -7956,7 +7956,7 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="9" t="s">
         <v>148</v>
@@ -8028,7 +8028,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
         <v>148</v>
@@ -8066,7 +8066,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>148</v>
@@ -8104,7 +8104,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
         <v>148</v>
@@ -8142,7 +8142,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
         <v>148</v>
@@ -8180,7 +8180,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
         <v>148</v>
@@ -8218,7 +8218,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
         <v>789</v>
@@ -8256,7 +8256,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
         <v>789</v>
@@ -8290,7 +8290,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="9" t="s">
         <v>789</v>
@@ -8328,7 +8328,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
         <v>789</v>
@@ -8366,7 +8366,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
         <v>789</v>
@@ -8404,7 +8404,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="9" t="s">
         <v>789</v>
@@ -8442,7 +8442,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="8" t="s">
         <v>789</v>
@@ -8476,7 +8476,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="132" t="s">
         <v>15</v>
@@ -8512,7 +8512,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="132" t="s">
         <v>15</v>
@@ -8548,7 +8548,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="132" t="s">
         <v>15</v>
@@ -8584,7 +8584,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="132" t="s">
         <v>15</v>
@@ -8618,7 +8618,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
         <v>98</v>
@@ -8654,7 +8654,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
         <v>98</v>
@@ -8692,7 +8692,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
         <v>98</v>
@@ -8730,7 +8730,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="9" t="s">
         <v>98</v>
@@ -8766,7 +8766,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="9" t="s">
         <v>98</v>
@@ -8806,7 +8806,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
         <v>98</v>
@@ -8844,7 +8844,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
         <v>98</v>
@@ -8882,7 +8882,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
         <v>1337</v>
@@ -8920,7 +8920,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
         <v>1337</v>
@@ -8958,7 +8958,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
         <v>1337</v>
@@ -8994,7 +8994,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
         <v>1337</v>
@@ -9032,7 +9032,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
         <v>1337</v>
@@ -9070,7 +9070,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
         <v>139</v>
@@ -9108,7 +9108,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
         <v>139</v>
@@ -9146,7 +9146,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
         <v>139</v>
@@ -9184,7 +9184,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
         <v>139</v>
@@ -9222,7 +9222,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="9" t="s">
         <v>1316</v>
@@ -9260,7 +9260,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
         <v>1316</v>
@@ -9298,7 +9298,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="9" t="s">
         <v>1316</v>
@@ -9338,7 +9338,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="9" t="s">
         <v>1316</v>
@@ -9376,7 +9376,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="9" t="s">
         <v>1316</v>
@@ -9412,7 +9412,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
         <v>1316</v>
@@ -9448,7 +9448,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
         <v>7</v>
@@ -9484,7 +9484,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="9" t="s">
         <v>7</v>
@@ -9520,7 +9520,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="9" t="s">
         <v>7</v>
@@ -9556,7 +9556,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="9" t="s">
         <v>7</v>
@@ -9592,7 +9592,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
@@ -9628,7 +9628,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="8" t="s">
         <v>7</v>
@@ -9666,7 +9666,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="8" t="s">
         <v>7</v>
@@ -9702,7 +9702,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="9" t="s">
         <v>7</v>
@@ -9740,7 +9740,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="9" t="s">
         <v>7</v>
@@ -9776,7 +9776,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9814,7 +9814,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
         <v>7</v>
@@ -9852,7 +9852,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
@@ -9888,7 +9888,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="9" t="s">
         <v>7</v>
@@ -9928,7 +9928,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="9" t="s">
         <v>7</v>
@@ -9966,7 +9966,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="9" t="s">
         <v>7</v>
@@ -10004,7 +10004,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
         <v>7</v>
@@ -10042,7 +10042,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="9" t="s">
         <v>7</v>
@@ -10080,7 +10080,7 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="9" t="s">
         <v>7</v>
@@ -10118,7 +10118,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10156,7 +10156,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>1167</v>
       </c>
@@ -10194,7 +10194,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
         <v>7</v>
@@ -10230,7 +10230,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
         <v>7</v>
@@ -10268,7 +10268,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
         <v>7</v>
@@ -10304,7 +10304,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
         <v>7</v>
@@ -10342,7 +10342,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
         <v>7</v>
@@ -10382,7 +10382,7 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
         <v>7</v>
@@ -10422,7 +10422,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>7</v>
@@ -10460,7 +10460,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
         <v>7</v>
@@ -10496,7 +10496,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
         <v>7</v>
@@ -10532,7 +10532,7 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
         <v>19</v>
@@ -10572,7 +10572,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="61" t="s">
         <v>19</v>
@@ -10610,7 +10610,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="61" t="s">
         <v>19</v>
@@ -10644,7 +10644,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="61" t="s">
         <v>19</v>
@@ -10678,7 +10678,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="61" t="s">
         <v>19</v>
@@ -10712,7 +10712,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="61" t="s">
         <v>19</v>
@@ -10746,7 +10746,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="61" t="s">
         <v>19</v>
@@ -10780,7 +10780,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="61" t="s">
         <v>19</v>
@@ -10814,7 +10814,7 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="61" t="s">
         <v>19</v>
@@ -10848,7 +10848,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="61" t="s">
         <v>19</v>
@@ -10882,7 +10882,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="61" t="s">
         <v>19</v>
@@ -10916,7 +10916,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="61" t="s">
         <v>19</v>
@@ -10950,7 +10950,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="9" t="s">
         <v>19</v>
@@ -10986,7 +10986,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="9" t="s">
         <v>19</v>
@@ -11022,7 +11022,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="9" t="s">
         <v>19</v>
@@ -11056,7 +11056,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -11090,7 +11090,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="9" t="s">
         <v>19</v>
@@ -11124,7 +11124,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
         <v>19</v>
@@ -11158,7 +11158,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
         <v>19</v>
@@ -11192,7 +11192,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
         <v>19</v>
@@ -11226,7 +11226,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11260,7 +11260,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
         <v>19</v>
@@ -11294,7 +11294,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="9" t="s">
         <v>19</v>
@@ -11330,7 +11330,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
         <v>19</v>
@@ -11366,7 +11366,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
         <v>19</v>
@@ -11402,7 +11402,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
         <v>19</v>
@@ -11438,7 +11438,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="9" t="s">
         <v>19</v>
@@ -11472,7 +11472,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="8" t="s">
         <v>60</v>
@@ -11510,7 +11510,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="8" t="s">
         <v>60</v>
@@ -11548,7 +11548,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="8" t="s">
         <v>60</v>
@@ -11586,7 +11586,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="9" t="s">
         <v>60</v>
@@ -11624,7 +11624,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="9" t="s">
         <v>60</v>
@@ -11661,7 +11661,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="9" t="s">
         <v>60</v>
@@ -11698,7 +11698,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="9" t="s">
         <v>60</v>
@@ -11733,7 +11733,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11764,7 +11764,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="8" t="s">
         <v>60</v>
@@ -11799,7 +11799,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="8" t="s">
         <v>60</v>
@@ -11834,7 +11834,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
         <v>60</v>
@@ -11871,7 +11871,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
         <v>60</v>
@@ -11908,7 +11908,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
         <v>717</v>
@@ -11943,7 +11943,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>717</v>
@@ -11978,7 +11978,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
         <v>717</v>
@@ -12013,7 +12013,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>717</v>
@@ -12050,7 +12050,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="36.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
         <v>717</v>
@@ -12087,7 +12087,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="46.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
         <v>717</v>
@@ -12122,7 +12122,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="8" t="s">
         <v>717</v>
@@ -12155,7 +12155,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="8" t="s">
         <v>717</v>
@@ -12188,7 +12188,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
         <v>717</v>
@@ -12221,7 +12221,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
         <v>717</v>
@@ -12256,7 +12256,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
         <v>717</v>
@@ -12285,7 +12285,7 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
         <v>717</v>
@@ -12320,7 +12320,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
         <v>717</v>
@@ -12355,7 +12355,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
       <c r="B170" s="9" t="s">
         <v>717</v>
@@ -12391,7 +12391,7 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" ht="46.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
       <c r="B171" s="9" t="s">
         <v>717</v>
@@ -12427,7 +12427,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="9" t="s">
         <v>717</v>
@@ -12463,7 +12463,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B173" s="68" t="s">
         <v>717</v>
       </c>
@@ -12528,16 +12528,7 @@
       <c r="K176" s="71"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:K173">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="4.7.10.2"/>
-        <filter val="4.7.11.2"/>
-        <filter val="4.7.13.4 5.7.7.3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="B4:K175">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:K175">
     <sortCondition ref="B4:B175"/>
     <sortCondition ref="C4:C175"/>
     <sortCondition ref="D4:D175"/>
@@ -12548,16 +12539,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="J150" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I208" sqref="I208"/>
+      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12644,7 +12634,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B6" s="9"/>
       <c r="C6" s="59" t="s">
         <v>131</v>
@@ -12670,7 +12660,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="59" t="s">
         <v>131</v>
@@ -12698,7 +12688,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="59" t="s">
         <v>131</v>
@@ -12722,7 +12712,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
@@ -12752,7 +12742,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="59" t="s">
         <v>148</v>
@@ -12780,7 +12770,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="59" t="s">
         <v>148</v>
@@ -12836,7 +12826,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="59" t="s">
         <v>148</v>
@@ -12866,7 +12856,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="20.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>148</v>
       </c>
@@ -12896,7 +12886,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>148</v>
       </c>
@@ -12926,7 +12916,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -12954,7 +12944,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="59" t="s">
         <v>148</v>
@@ -12982,7 +12972,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -13010,7 +13000,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>148</v>
       </c>
@@ -13040,7 +13030,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="25"/>
       <c r="C20" s="64" t="s">
         <v>148</v>
@@ -13094,7 +13084,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>148</v>
       </c>
@@ -13124,7 +13114,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="59" t="s">
         <v>148</v>
@@ -13180,7 +13170,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>148</v>
       </c>
@@ -13210,7 +13200,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
         <v>148</v>
@@ -13238,7 +13228,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="60" t="s">
         <v>148</v>
@@ -13268,7 +13258,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="60" t="s">
         <v>148</v>
@@ -13298,7 +13288,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>148</v>
@@ -13322,7 +13312,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="60" t="s">
         <v>1626</v>
@@ -13348,7 +13338,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="60" t="s">
         <v>1626</v>
@@ -13372,7 +13362,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="59" t="s">
         <v>1626</v>
@@ -13400,7 +13390,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="C33" s="59" t="s">
         <v>1626</v>
@@ -13424,7 +13414,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="59" t="s">
         <v>1626</v>
@@ -13448,7 +13438,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>789</v>
@@ -13476,7 +13466,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>1463</v>
       </c>
@@ -13506,7 +13496,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="59" t="s">
         <v>789</v>
@@ -13534,7 +13524,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="64" t="s">
         <v>789</v>
@@ -13560,7 +13550,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="64" t="s">
         <v>789</v>
@@ -13586,7 +13576,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="59" t="s">
         <v>789</v>
@@ -13614,7 +13604,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>789</v>
       </c>
@@ -13642,7 +13632,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B42" s="9"/>
       <c r="C42" s="59" t="s">
         <v>789</v>
@@ -13666,7 +13656,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B43" s="9"/>
       <c r="C43" s="59" t="s">
         <v>789</v>
@@ -13690,7 +13680,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="59" t="s">
         <v>1383</v>
@@ -13716,7 +13706,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="59" t="s">
         <v>1383</v>
@@ -13744,7 +13734,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="59" t="s">
         <v>1383</v>
@@ -13772,7 +13762,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="59" t="s">
         <v>1383</v>
@@ -13828,7 +13818,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>15</v>
       </c>
@@ -13858,7 +13848,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
@@ -13888,7 +13878,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>15</v>
       </c>
@@ -13918,7 +13908,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>15</v>
       </c>
@@ -13948,7 +13938,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>15</v>
       </c>
@@ -13978,7 +13968,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
         <v>15</v>
       </c>
@@ -14006,7 +13996,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
@@ -14034,7 +14024,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B56" s="9" t="s">
         <v>15</v>
       </c>
@@ -14062,7 +14052,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="59" t="s">
         <v>1133</v>
@@ -14086,7 +14076,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="59" t="s">
         <v>1133</v>
@@ -14110,7 +14100,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="59" t="s">
         <v>1133</v>
@@ -14134,7 +14124,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="59" t="s">
         <v>1133</v>
@@ -14158,7 +14148,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="59" t="s">
         <v>1133</v>
@@ -14182,7 +14172,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="59" t="s">
         <v>1133</v>
@@ -14208,7 +14198,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="59" t="s">
         <v>1133</v>
@@ -14234,7 +14224,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="59" t="s">
         <v>1133</v>
@@ -14258,7 +14248,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="59" t="s">
         <v>1133</v>
@@ -14286,7 +14276,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="59" t="s">
         <v>1133</v>
@@ -14312,7 +14302,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="59" t="s">
         <v>1382</v>
@@ -14340,7 +14330,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="68" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="59" t="s">
         <v>1337</v>
@@ -14368,7 +14358,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="25"/>
       <c r="C69" s="59" t="s">
         <v>1337</v>
@@ -14394,7 +14384,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="25"/>
       <c r="C70" s="9" t="s">
         <v>1337</v>
@@ -14422,7 +14412,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="59" t="s">
         <v>1337</v>
@@ -14448,7 +14438,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="25"/>
       <c r="C72" s="58" t="s">
         <v>1337</v>
@@ -14476,7 +14466,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
       <c r="C73" s="59" t="s">
         <v>139</v>
@@ -14504,7 +14494,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
       <c r="C74" s="59" t="s">
         <v>139</v>
@@ -14532,7 +14522,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>139</v>
       </c>
@@ -14562,7 +14552,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>139</v>
       </c>
@@ -14590,7 +14580,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
         <v>1316</v>
@@ -14618,7 +14608,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
         <v>1316</v>
@@ -14646,7 +14636,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="59" t="s">
         <v>1316</v>
@@ -14674,7 +14664,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="80" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="59" t="s">
         <v>1623</v>
@@ -14700,7 +14690,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="59" t="s">
         <v>1623</v>
@@ -14726,7 +14716,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -14754,7 +14744,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -14782,7 +14772,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B84" s="25"/>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -14810,7 +14800,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="64" t="s">
         <v>7</v>
@@ -14836,7 +14826,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="59" t="s">
         <v>7</v>
@@ -14862,7 +14852,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="59" t="s">
         <v>7</v>
@@ -14888,7 +14878,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="59" t="s">
         <v>7</v>
@@ -14914,7 +14904,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="9" t="s">
         <v>60</v>
       </c>
@@ -14944,7 +14934,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="59" t="s">
         <v>7</v>
@@ -14970,7 +14960,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="91" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="59" t="s">
         <v>7</v>
@@ -14998,7 +14988,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="92" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="59" t="s">
         <v>7</v>
@@ -15024,7 +15014,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="59" t="s">
         <v>7</v>
@@ -15050,7 +15040,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B94" s="25"/>
       <c r="C94" s="9" t="s">
         <v>7</v>
@@ -15078,7 +15068,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="95" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="59" t="s">
         <v>7</v>
@@ -15104,7 +15094,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="96" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B96" s="25" t="s">
         <v>710</v>
       </c>
@@ -15134,7 +15124,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
         <v>148</v>
       </c>
@@ -15190,7 +15180,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>710</v>
       </c>
@@ -15218,7 +15208,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B100" s="25"/>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -15246,7 +15236,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B101" s="25"/>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -15272,7 +15262,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="25"/>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -15298,7 +15288,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B103" s="25" t="s">
         <v>710</v>
       </c>
@@ -15386,7 +15376,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B106" s="9" t="s">
         <v>148</v>
       </c>
@@ -15412,7 +15402,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15440,7 +15430,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="9"/>
       <c r="C108" s="59" t="s">
         <v>7</v>
@@ -15464,7 +15454,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B109" s="9"/>
       <c r="C109" s="59" t="s">
         <v>7</v>
@@ -15488,7 +15478,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="9"/>
       <c r="C110" s="59" t="s">
         <v>7</v>
@@ -15512,7 +15502,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="9" t="s">
         <v>1261</v>
@@ -15540,7 +15530,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
         <v>1261</v>
@@ -15568,7 +15558,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="113" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B113" s="25"/>
       <c r="C113" s="9" t="s">
         <v>1261</v>
@@ -15596,7 +15586,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="59" t="s">
         <v>1552</v>
@@ -15622,7 +15612,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="59" t="s">
         <v>1552</v>
@@ -15650,7 +15640,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="59" t="s">
         <v>1552</v>
@@ -15676,7 +15666,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="117" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="59" t="s">
         <v>1552</v>
@@ -15702,7 +15692,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="118" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="59" t="s">
         <v>1552</v>
@@ -15728,7 +15718,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="119" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="59" t="s">
         <v>1552</v>
@@ -15754,7 +15744,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="59" t="s">
         <v>1552</v>
@@ -15780,7 +15770,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="59" t="s">
         <v>1552</v>
@@ -15806,7 +15796,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B122" s="9"/>
       <c r="C122" s="59" t="s">
         <v>1552</v>
@@ -15832,7 +15822,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
       <c r="C123" s="59" t="s">
         <v>1552</v>
@@ -15858,7 +15848,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="9"/>
       <c r="C124" s="59" t="s">
         <v>1552</v>
@@ -15884,7 +15874,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="125" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B125" s="9"/>
       <c r="C125" s="59" t="s">
         <v>1552</v>
@@ -15910,7 +15900,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="126" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B126" s="9"/>
       <c r="C126" s="59" t="s">
         <v>1552</v>
@@ -15938,7 +15928,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="127" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B127" s="9"/>
       <c r="C127" s="59" t="s">
         <v>1552</v>
@@ -15966,7 +15956,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="128" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="59" t="s">
         <v>1552</v>
@@ -15990,7 +15980,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B129" s="56"/>
       <c r="C129" s="59" t="s">
         <v>1552</v>
@@ -16016,7 +16006,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B130" s="9"/>
       <c r="C130" s="59" t="s">
         <v>1552</v>
@@ -16042,7 +16032,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="59" t="s">
         <v>1552</v>
@@ -16068,7 +16058,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="59" t="s">
         <v>1552</v>
@@ -16094,7 +16084,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B133" s="9"/>
       <c r="C133" s="59" t="s">
         <v>1552</v>
@@ -16120,7 +16110,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="59" t="s">
         <v>1552</v>
@@ -16146,7 +16136,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B135" s="9"/>
       <c r="C135" s="59" t="s">
         <v>1552</v>
@@ -16172,7 +16162,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B136" s="9"/>
       <c r="C136" s="59" t="s">
         <v>1552</v>
@@ -16196,7 +16186,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="9"/>
       <c r="C137" s="59" t="s">
         <v>1552</v>
@@ -16224,7 +16214,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B138" s="9"/>
       <c r="C138" s="59" t="s">
         <v>1552</v>
@@ -16250,7 +16240,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="57" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="59" t="s">
         <v>1552</v>
@@ -16274,7 +16264,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="59" t="s">
         <v>1552</v>
@@ -16298,7 +16288,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="s">
         <v>19</v>
       </c>
@@ -16326,7 +16316,7 @@
       </c>
       <c r="K141" s="83"/>
     </row>
-    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B142" s="8" t="s">
         <v>19</v>
       </c>
@@ -16356,7 +16346,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B143" s="8" t="s">
         <v>19</v>
       </c>
@@ -16386,7 +16376,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">
         <v>19</v>
       </c>
@@ -16416,7 +16406,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
         <v>19</v>
       </c>
@@ -16446,7 +16436,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
       <c r="C146" s="64" t="s">
         <v>60</v>
@@ -16474,7 +16464,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B147" s="9"/>
       <c r="C147" s="9" t="s">
         <v>60</v>
@@ -16502,7 +16492,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B148" s="9"/>
       <c r="C148" s="59" t="s">
         <v>60</v>
@@ -16530,7 +16520,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="9"/>
       <c r="C149" s="9" t="s">
         <v>60</v>
@@ -16558,7 +16548,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B150" s="9"/>
       <c r="C150" s="59" t="s">
         <v>60</v>
@@ -16584,7 +16574,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B151" s="9" t="s">
         <v>7</v>
       </c>
@@ -16614,7 +16604,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B152" s="9" t="s">
         <v>711</v>
       </c>
@@ -16642,7 +16632,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B153" s="9" t="s">
         <v>711</v>
       </c>
@@ -16670,7 +16660,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="61" t="s">
         <v>60</v>
@@ -16696,7 +16686,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B155" s="9" t="s">
         <v>1387</v>
       </c>
@@ -16724,7 +16714,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B156" s="9"/>
       <c r="C156" s="64" t="s">
         <v>717</v>
@@ -16750,7 +16740,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="9"/>
       <c r="C157" s="59" t="s">
         <v>717</v>
@@ -16778,7 +16768,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B158" s="9"/>
       <c r="C158" s="59" t="s">
         <v>717</v>
@@ -16806,7 +16796,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B159" s="44"/>
       <c r="C159" s="59" t="s">
         <v>717</v>
@@ -16834,7 +16824,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9" t="s">
         <v>717</v>
@@ -16862,7 +16852,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
         <v>717</v>
@@ -16890,7 +16880,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="59" t="s">
         <v>717</v>
@@ -16918,7 +16908,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="59" t="s">
         <v>717</v>
@@ -16946,7 +16936,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>715</v>
       </c>
@@ -16976,7 +16966,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>715</v>
       </c>
@@ -17006,7 +16996,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B166" s="9" t="s">
         <v>715</v>
       </c>
@@ -17036,7 +17026,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9" t="s">
         <v>717</v>
@@ -17064,7 +17054,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="59" t="s">
         <v>717</v>
@@ -17090,7 +17080,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
       <c r="C169" s="64" t="s">
         <v>717</v>
@@ -17118,7 +17108,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B170" s="44"/>
       <c r="C170" s="59" t="s">
         <v>717</v>
@@ -17144,7 +17134,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B171" s="9"/>
       <c r="C171" s="64" t="s">
         <v>717</v>
@@ -17170,7 +17160,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B172" s="9"/>
       <c r="C172" s="9" t="s">
         <v>717</v>
@@ -17196,7 +17186,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>717</v>
       </c>
@@ -17226,7 +17216,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>717</v>
       </c>
@@ -17256,7 +17246,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B175" s="9"/>
       <c r="C175" s="59" t="s">
         <v>717</v>
@@ -17284,7 +17274,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="59" t="s">
         <v>717</v>
@@ -17310,7 +17300,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B177" s="9"/>
       <c r="C177" s="64" t="s">
         <v>717</v>
@@ -17336,7 +17326,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B178" s="9"/>
       <c r="C178" s="59" t="s">
         <v>717</v>
@@ -17364,7 +17354,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B179" s="9"/>
       <c r="C179" s="59" t="s">
         <v>717</v>
@@ -17392,7 +17382,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B180" s="9"/>
       <c r="C180" s="59" t="s">
         <v>717</v>
@@ -17420,7 +17410,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B181" s="9"/>
       <c r="C181" s="59" t="s">
         <v>717</v>
@@ -17448,7 +17438,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B182" s="9"/>
       <c r="C182" s="59" t="s">
         <v>717</v>
@@ -17532,7 +17522,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B185" s="9"/>
       <c r="C185" s="9" t="s">
         <v>60</v>
@@ -17562,7 +17552,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B186" s="9" t="s">
         <v>7</v>
       </c>
@@ -17588,7 +17578,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17614,7 +17604,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B188" s="9" t="s">
         <v>148</v>
       </c>
@@ -17640,7 +17630,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
         <v>148</v>
       </c>
@@ -17666,7 +17656,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B190" s="25"/>
       <c r="C190" s="9" t="s">
         <v>717</v>
@@ -17690,7 +17680,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B191" s="44"/>
       <c r="C191" s="9" t="s">
         <v>717</v>
@@ -17714,7 +17704,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
       <c r="C192" s="9" t="s">
         <v>717</v>
@@ -17738,7 +17728,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B193" s="9"/>
       <c r="C193" s="9" t="s">
         <v>717</v>
@@ -17762,7 +17752,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>717</v>
@@ -17786,7 +17776,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B195" s="9"/>
       <c r="C195" s="59" t="s">
         <v>717</v>
@@ -17810,7 +17800,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B196" s="9"/>
       <c r="C196" s="59" t="s">
         <v>717</v>
@@ -17834,7 +17824,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B197" s="9"/>
       <c r="C197" s="59" t="s">
         <v>717</v>
@@ -17858,7 +17848,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B198" s="9"/>
       <c r="C198" s="59" t="s">
         <v>717</v>
@@ -17882,7 +17872,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B199" s="9" t="s">
         <v>7</v>
       </c>
@@ -17912,7 +17902,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B200" s="9" t="s">
         <v>7</v>
       </c>
@@ -17942,7 +17932,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="59" t="s">
         <v>1625</v>
@@ -17966,7 +17956,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="59" t="s">
         <v>1625</v>
@@ -17990,7 +17980,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B203" s="9"/>
       <c r="C203" s="59" t="s">
         <v>1625</v>
@@ -18014,7 +18004,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B204" s="9"/>
       <c r="C204" s="59" t="s">
         <v>1625</v>
@@ -18038,7 +18028,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B205" s="9"/>
       <c r="C205" s="59" t="s">
         <v>1625</v>
@@ -18062,7 +18052,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B206" s="9"/>
       <c r="C206" s="59" t="s">
         <v>1625</v>
@@ -18086,7 +18076,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="207" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B207" s="67"/>
       <c r="C207" s="82" t="s">
         <v>1625</v>
@@ -18867,22 +18857,7 @@
       <c r="K269" s="52"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:K208">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="4.6.1.3"/>
-        <filter val="4.6.2.2"/>
-        <filter val="4.6.2.4"/>
-        <filter val="4.6.2.5"/>
-        <filter val="4.6.5.2"/>
-        <filter val="4.6.5.6"/>
-        <filter val="4.6.6.1"/>
-        <filter val="4.6.6.5"/>
-        <filter val="4.6.7.3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="B5:K210">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:K210">
     <sortCondition ref="C5:C210"/>
     <sortCondition ref="E5:E210"/>
   </sortState>

</xml_diff>

<commit_message>
GS 5, TS 5 and 6 Padam Input Templates -01/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA0E39-79AD-4579-B42E-63A5E59D1D50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325A14DF-687D-4B6F-B008-F43AEB741DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5770,7 +5770,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5951,6 +5950,7 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6237,7 +6237,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I178" sqref="I178"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,10 +6434,10 @@
       <c r="E7" s="9" t="s">
         <v>1335</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="74" t="s">
         <v>1101</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="74" t="s">
         <v>1117</v>
       </c>
       <c r="H7" s="11"/>
@@ -6472,14 +6472,14 @@
       <c r="E8" s="59" t="s">
         <v>1495</v>
       </c>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="74" t="s">
         <v>1102</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="74" t="s">
         <v>1679</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="72" t="s">
         <v>305</v>
       </c>
       <c r="J8" s="25" t="s">
@@ -6510,14 +6510,14 @@
       <c r="E9" s="59" t="s">
         <v>1495</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="74" t="s">
         <v>1102</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="74" t="s">
         <v>1652</v>
       </c>
       <c r="H9" s="11"/>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="72" t="s">
         <v>305</v>
       </c>
       <c r="J9" s="25" t="s">
@@ -6559,7 +6559,7 @@
       <c r="J10" s="47" t="s">
         <v>441</v>
       </c>
-      <c r="K10" s="150" t="s">
+      <c r="K10" s="149" t="s">
         <v>1701</v>
       </c>
       <c r="L10" s="1"/>
@@ -6735,12 +6735,12 @@
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="89" t="s">
+      <c r="G15" s="88" t="s">
         <v>150</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="67"/>
+      <c r="J15" s="66"/>
       <c r="K15" s="11"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -6774,7 +6774,7 @@
       <c r="I16" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="J16" s="148" t="s">
+      <c r="J16" s="147" t="s">
         <v>423</v>
       </c>
       <c r="K16" s="11"/>
@@ -6839,7 +6839,7 @@
       <c r="F18" s="60" t="s">
         <v>1101</v>
       </c>
-      <c r="G18" s="92"/>
+      <c r="G18" s="91"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
         <v>285</v>
@@ -6847,7 +6847,7 @@
       <c r="J18" s="58" t="s">
         <v>426</v>
       </c>
-      <c r="K18" s="113" t="s">
+      <c r="K18" s="112" t="s">
         <v>164</v>
       </c>
       <c r="L18" s="1"/>
@@ -6875,9 +6875,9 @@
       <c r="F19" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="G19" s="92"/>
+      <c r="G19" s="91"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="72" t="s">
         <v>303</v>
       </c>
       <c r="J19" s="25" t="s">
@@ -6911,9 +6911,9 @@
       <c r="F20" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="G20" s="92"/>
+      <c r="G20" s="91"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="72" t="s">
         <v>303</v>
       </c>
       <c r="J20" s="25" t="s">
@@ -6955,7 +6955,7 @@
       <c r="J21" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="K21" s="107" t="s">
+      <c r="K21" s="106" t="s">
         <v>167</v>
       </c>
       <c r="L21" s="1"/>
@@ -7021,7 +7021,7 @@
         <v>1130</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="73" t="s">
+      <c r="I23" s="72" t="s">
         <v>327</v>
       </c>
       <c r="J23" s="25" t="s">
@@ -7177,7 +7177,7 @@
       <c r="J27" s="58" t="s">
         <v>422</v>
       </c>
-      <c r="K27" s="117" t="s">
+      <c r="K27" s="116" t="s">
         <v>161</v>
       </c>
       <c r="L27" s="1"/>
@@ -7209,7 +7209,7 @@
       <c r="H28" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="72" t="s">
         <v>236</v>
       </c>
       <c r="J28" s="25" t="s">
@@ -7319,10 +7319,10 @@
         <v>173</v>
       </c>
       <c r="H31" s="50"/>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="72" t="s">
         <v>494</v>
       </c>
-      <c r="J31" s="85" t="s">
+      <c r="J31" s="84" t="s">
         <v>1470</v>
       </c>
       <c r="K31" s="32" t="s">
@@ -7429,7 +7429,7 @@
         <v>160</v>
       </c>
       <c r="H34" s="11"/>
-      <c r="I34" s="73" t="s">
+      <c r="I34" s="72" t="s">
         <v>286</v>
       </c>
       <c r="J34" s="25" t="s">
@@ -7501,7 +7501,7 @@
       <c r="F36" s="59" t="s">
         <v>1115</v>
       </c>
-      <c r="G36" s="75" t="s">
+      <c r="G36" s="74" t="s">
         <v>1652</v>
       </c>
       <c r="H36" s="11"/>
@@ -7536,7 +7536,7 @@
       <c r="E37" s="9" t="s">
         <v>1210</v>
       </c>
-      <c r="F37" s="75" t="s">
+      <c r="F37" s="74" t="s">
         <v>176</v>
       </c>
       <c r="G37" s="44"/>
@@ -7573,7 +7573,7 @@
         <v>1311</v>
       </c>
       <c r="F38" s="9"/>
-      <c r="G38" s="75" t="s">
+      <c r="G38" s="74" t="s">
         <v>1117</v>
       </c>
       <c r="H38" s="11"/>
@@ -7583,7 +7583,7 @@
       <c r="J38" s="25" t="s">
         <v>451</v>
       </c>
-      <c r="K38" s="107" t="s">
+      <c r="K38" s="106" t="s">
         <v>199</v>
       </c>
       <c r="L38" s="1"/>
@@ -7608,10 +7608,10 @@
       <c r="E39" s="9" t="s">
         <v>1314</v>
       </c>
-      <c r="F39" s="75" t="s">
+      <c r="F39" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="75" t="s">
+      <c r="G39" s="74" t="s">
         <v>1117</v>
       </c>
       <c r="H39" s="11"/>
@@ -7646,12 +7646,12 @@
       <c r="E40" s="9" t="s">
         <v>1315</v>
       </c>
-      <c r="F40" s="75" t="s">
+      <c r="F40" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="G40" s="44"/>
       <c r="H40" s="11"/>
-      <c r="I40" s="73" t="s">
+      <c r="I40" s="72" t="s">
         <v>297</v>
       </c>
       <c r="J40" s="25" t="s">
@@ -7682,7 +7682,7 @@
       <c r="E41" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="F41" s="75" t="s">
+      <c r="F41" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="G41" s="44"/>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="G42" s="44"/>
       <c r="H42" s="11"/>
-      <c r="I42" s="73" t="s">
+      <c r="I42" s="72" t="s">
         <v>283</v>
       </c>
       <c r="J42" s="25" t="s">
@@ -7754,7 +7754,7 @@
       <c r="E43" s="9" t="s">
         <v>1352</v>
       </c>
-      <c r="F43" s="75" t="s">
+      <c r="F43" s="74" t="s">
         <v>176</v>
       </c>
       <c r="G43" s="44"/>
@@ -7791,11 +7791,11 @@
       <c r="F44" s="59" t="s">
         <v>1115</v>
       </c>
-      <c r="G44" s="75" t="s">
+      <c r="G44" s="74" t="s">
         <v>173</v>
       </c>
       <c r="H44" s="11"/>
-      <c r="I44" s="11" t="s">
+      <c r="I44" s="72" t="s">
         <v>306</v>
       </c>
       <c r="J44" s="25" t="s">
@@ -7837,7 +7837,7 @@
       <c r="J45" s="25" t="s">
         <v>1354</v>
       </c>
-      <c r="K45" s="101" t="s">
+      <c r="K45" s="100" t="s">
         <v>210</v>
       </c>
       <c r="L45" s="1"/>
@@ -7862,7 +7862,7 @@
       <c r="E46" s="9" t="s">
         <v>1308</v>
       </c>
-      <c r="F46" s="81" t="s">
+      <c r="F46" s="80" t="s">
         <v>1101</v>
       </c>
       <c r="G46" s="44"/>
@@ -7870,7 +7870,7 @@
       <c r="I46" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="J46" s="96" t="s">
+      <c r="J46" s="95" t="s">
         <v>447</v>
       </c>
       <c r="K46" s="13"/>
@@ -7896,7 +7896,7 @@
       <c r="E47" s="9" t="s">
         <v>1308</v>
       </c>
-      <c r="F47" s="75" t="s">
+      <c r="F47" s="74" t="s">
         <v>61</v>
       </c>
       <c r="G47" s="44"/>
@@ -7906,7 +7906,7 @@
       <c r="I47" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="J47" s="96" t="s">
+      <c r="J47" s="95" t="s">
         <v>446</v>
       </c>
       <c r="K47" s="13" t="s">
@@ -7934,12 +7934,12 @@
       <c r="E48" s="9" t="s">
         <v>1349</v>
       </c>
-      <c r="F48" s="75" t="s">
+      <c r="F48" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="G48" s="44"/>
       <c r="H48" s="11"/>
-      <c r="I48" s="73" t="s">
+      <c r="I48" s="72" t="s">
         <v>304</v>
       </c>
       <c r="J48" s="25" t="s">
@@ -7975,7 +7975,7 @@
       </c>
       <c r="G49" s="27"/>
       <c r="H49" s="11"/>
-      <c r="I49" s="73" t="s">
+      <c r="I49" s="72" t="s">
         <v>308</v>
       </c>
       <c r="J49" s="25" t="s">
@@ -8006,7 +8006,7 @@
       <c r="E50" s="9" t="s">
         <v>1313</v>
       </c>
-      <c r="F50" s="75" t="s">
+      <c r="F50" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="G50" s="44"/>
@@ -8017,7 +8017,7 @@
       <c r="J50" s="25" t="s">
         <v>453</v>
       </c>
-      <c r="K50" s="107" t="s">
+      <c r="K50" s="106" t="s">
         <v>201</v>
       </c>
       <c r="L50" s="1"/>
@@ -8055,7 +8055,7 @@
       <c r="J51" s="25" t="s">
         <v>409</v>
       </c>
-      <c r="K51" s="104" t="s">
+      <c r="K51" s="103" t="s">
         <v>215</v>
       </c>
       <c r="L51" s="1"/>
@@ -8080,7 +8080,7 @@
       <c r="E52" s="9" t="s">
         <v>1310</v>
       </c>
-      <c r="F52" s="75" t="s">
+      <c r="F52" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="G52" s="44"/>
@@ -8118,14 +8118,14 @@
       <c r="E53" s="9" t="s">
         <v>1312</v>
       </c>
-      <c r="F53" s="75" t="s">
+      <c r="F53" s="74" t="s">
         <v>1101</v>
       </c>
-      <c r="G53" s="75" t="s">
+      <c r="G53" s="74" t="s">
         <v>1117</v>
       </c>
       <c r="H53" s="11"/>
-      <c r="I53" s="73" t="s">
+      <c r="I53" s="72" t="s">
         <v>287</v>
       </c>
       <c r="J53" s="58" t="s">
@@ -8163,7 +8163,7 @@
       <c r="H54" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="I54" s="73" t="s">
+      <c r="I54" s="72" t="s">
         <v>251</v>
       </c>
       <c r="J54" s="45" t="s">
@@ -8245,7 +8245,7 @@
       <c r="J56" s="25" t="s">
         <v>400</v>
       </c>
-      <c r="K56" s="118" t="s">
+      <c r="K56" s="117" t="s">
         <v>156</v>
       </c>
       <c r="L56" s="1"/>
@@ -8273,7 +8273,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="11"/>
-      <c r="I57" s="151" t="s">
+      <c r="I57" s="150" t="s">
         <v>817</v>
       </c>
       <c r="J57" s="45" t="s">
@@ -8308,7 +8308,7 @@
         <v>1665</v>
       </c>
       <c r="G58" s="44"/>
-      <c r="H58" s="79" t="s">
+      <c r="H58" s="78" t="s">
         <v>83</v>
       </c>
       <c r="I58" s="11" t="s">
@@ -8346,7 +8346,7 @@
         <v>1665</v>
       </c>
       <c r="G59" s="44"/>
-      <c r="H59" s="79" t="s">
+      <c r="H59" s="78" t="s">
         <v>83</v>
       </c>
       <c r="I59" s="11" t="s">
@@ -8387,7 +8387,7 @@
         <v>1139</v>
       </c>
       <c r="H60" s="11"/>
-      <c r="I60" s="73" t="s">
+      <c r="I60" s="72" t="s">
         <v>318</v>
       </c>
       <c r="J60" s="25" t="s">
@@ -8459,7 +8459,7 @@
         <v>1678</v>
       </c>
       <c r="H62" s="11"/>
-      <c r="I62" s="74" t="s">
+      <c r="I62" s="73" t="s">
         <v>26</v>
       </c>
       <c r="J62" s="25" t="s">
@@ -8478,7 +8478,7 @@
     </row>
     <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="132" t="s">
+      <c r="B63" s="131" t="s">
         <v>15</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -8488,17 +8488,17 @@
       <c r="E63" s="9" t="s">
         <v>1183</v>
       </c>
-      <c r="F63" s="72" t="s">
+      <c r="F63" s="71" t="s">
         <v>1656</v>
       </c>
-      <c r="G63" s="72" t="s">
+      <c r="G63" s="71" t="s">
         <v>1108</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J63" s="129" t="s">
+      <c r="J63" s="128" t="s">
         <v>345</v>
       </c>
       <c r="K63" s="34" t="s">
@@ -8514,7 +8514,7 @@
     </row>
     <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="132" t="s">
+      <c r="B64" s="131" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -8524,17 +8524,17 @@
       <c r="E64" s="9" t="s">
         <v>1184</v>
       </c>
-      <c r="F64" s="72" t="s">
+      <c r="F64" s="71" t="s">
         <v>1656</v>
       </c>
-      <c r="G64" s="72" t="s">
+      <c r="G64" s="71" t="s">
         <v>1108</v>
       </c>
       <c r="H64" s="17"/>
       <c r="I64" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J64" s="129" t="s">
+      <c r="J64" s="128" t="s">
         <v>346</v>
       </c>
       <c r="K64" s="34" t="s">
@@ -8550,7 +8550,7 @@
     </row>
     <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="132" t="s">
+      <c r="B65" s="131" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -8562,15 +8562,15 @@
       <c r="E65" s="9" t="s">
         <v>1473</v>
       </c>
-      <c r="F65" s="72" t="s">
+      <c r="F65" s="71" t="s">
         <v>1656</v>
       </c>
       <c r="G65" s="10"/>
       <c r="H65" s="17"/>
-      <c r="I65" s="74" t="s">
+      <c r="I65" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="J65" s="129" t="s">
+      <c r="J65" s="128" t="s">
         <v>344</v>
       </c>
       <c r="K65" s="34" t="s">
@@ -8586,7 +8586,7 @@
     </row>
     <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="132" t="s">
+      <c r="B66" s="131" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -8596,7 +8596,7 @@
       <c r="E66" s="9" t="s">
         <v>1181</v>
       </c>
-      <c r="F66" s="72" t="s">
+      <c r="F66" s="71" t="s">
         <v>1657</v>
       </c>
       <c r="G66" s="10"/>
@@ -8604,7 +8604,7 @@
       <c r="I66" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J66" s="129" t="s">
+      <c r="J66" s="128" t="s">
         <v>1695</v>
       </c>
       <c r="K66" s="34" t="s">
@@ -8713,13 +8713,13 @@
       <c r="H69" s="11" t="s">
         <v>1682</v>
       </c>
-      <c r="I69" s="74" t="s">
+      <c r="I69" s="73" t="s">
         <v>322</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="K69" s="111" t="s">
+      <c r="K69" s="110" t="s">
         <v>105</v>
       </c>
       <c r="L69" s="1"/>
@@ -8751,13 +8751,13 @@
       <c r="H70" s="11" t="s">
         <v>1682</v>
       </c>
-      <c r="I70" s="73" t="s">
+      <c r="I70" s="72" t="s">
         <v>322</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>812</v>
       </c>
-      <c r="K70" s="112"/>
+      <c r="K70" s="111"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -8821,7 +8821,7 @@
         <v>1273</v>
       </c>
       <c r="F72" s="9"/>
-      <c r="G72" s="72" t="s">
+      <c r="G72" s="71" t="s">
         <v>1123</v>
       </c>
       <c r="H72" s="59" t="s">
@@ -8928,7 +8928,7 @@
       <c r="C75" s="26" t="s">
         <v>1357</v>
       </c>
-      <c r="D75" s="87" t="s">
+      <c r="D75" s="86" t="s">
         <v>1361</v>
       </c>
       <c r="E75" s="26" t="s">
@@ -8979,7 +8979,7 @@
       <c r="H76" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="I76" s="80" t="s">
+      <c r="I76" s="79" t="s">
         <v>322</v>
       </c>
       <c r="J76" s="25" t="s">
@@ -9129,13 +9129,13 @@
       <c r="H80" s="11" t="s">
         <v>1684</v>
       </c>
-      <c r="I80" s="74" t="s">
+      <c r="I80" s="73" t="s">
         <v>222</v>
       </c>
       <c r="J80" s="25" t="s">
         <v>411</v>
       </c>
-      <c r="K80" s="105" t="s">
+      <c r="K80" s="104" t="s">
         <v>140</v>
       </c>
       <c r="L80" s="1"/>
@@ -9151,7 +9151,7 @@
       <c r="B81" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C81" s="119" t="s">
+      <c r="C81" s="118" t="s">
         <v>1400</v>
       </c>
       <c r="D81" s="9" t="s">
@@ -9327,7 +9327,7 @@
       <c r="J85" s="25" t="s">
         <v>440</v>
       </c>
-      <c r="K85" s="101" t="s">
+      <c r="K85" s="100" t="s">
         <v>189</v>
       </c>
       <c r="L85" s="1"/>
@@ -9365,7 +9365,7 @@
       <c r="J86" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="K86" s="101" t="s">
+      <c r="K86" s="100" t="s">
         <v>188</v>
       </c>
       <c r="L86" s="1"/>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="G88" s="44"/>
       <c r="H88" s="11"/>
-      <c r="I88" s="74" t="s">
+      <c r="I88" s="73" t="s">
         <v>253</v>
       </c>
       <c r="J88" s="25" t="s">
@@ -9496,10 +9496,10 @@
       <c r="E90" s="28" t="s">
         <v>1213</v>
       </c>
-      <c r="F90" s="80" t="s">
+      <c r="F90" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="G90" s="91"/>
+      <c r="G90" s="90"/>
       <c r="H90" s="11" t="s">
         <v>90</v>
       </c>
@@ -9528,21 +9528,21 @@
       <c r="C91" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D91" s="67"/>
-      <c r="E91" s="67" t="s">
+      <c r="D91" s="66"/>
+      <c r="E91" s="66" t="s">
         <v>1214</v>
       </c>
-      <c r="F91" s="82" t="s">
+      <c r="F91" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="G91" s="145"/>
-      <c r="H91" s="146" t="s">
+      <c r="G91" s="144"/>
+      <c r="H91" s="145" t="s">
         <v>90</v>
       </c>
-      <c r="I91" s="147" t="s">
+      <c r="I91" s="146" t="s">
         <v>266</v>
       </c>
-      <c r="J91" s="99" t="s">
+      <c r="J91" s="98" t="s">
         <v>85</v>
       </c>
       <c r="K91" s="19" t="s">
@@ -9611,7 +9611,7 @@
       <c r="H93" s="11" t="s">
         <v>795</v>
       </c>
-      <c r="I93" s="21" t="s">
+      <c r="I93" s="73" t="s">
         <v>217</v>
       </c>
       <c r="J93" s="25" t="s">
@@ -9685,7 +9685,7 @@
       <c r="H95" s="11" t="s">
         <v>794</v>
       </c>
-      <c r="I95" s="21" t="s">
+      <c r="I95" s="73" t="s">
         <v>245</v>
       </c>
       <c r="J95" s="25" t="s">
@@ -9729,7 +9729,7 @@
       <c r="J96" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="K96" s="101" t="s">
+      <c r="K96" s="100" t="s">
         <v>259</v>
       </c>
       <c r="L96" s="1"/>
@@ -9759,7 +9759,7 @@
       </c>
       <c r="G97" s="44"/>
       <c r="H97" s="11"/>
-      <c r="I97" s="80" t="s">
+      <c r="I97" s="79" t="s">
         <v>219</v>
       </c>
       <c r="J97" s="25" t="s">
@@ -9794,7 +9794,7 @@
         <v>67</v>
       </c>
       <c r="G98" s="44"/>
-      <c r="H98" s="79" t="s">
+      <c r="H98" s="78" t="s">
         <v>69</v>
       </c>
       <c r="I98" s="21" t="s">
@@ -9832,7 +9832,7 @@
         <v>70</v>
       </c>
       <c r="G99" s="44"/>
-      <c r="H99" s="79" t="s">
+      <c r="H99" s="78" t="s">
         <v>69</v>
       </c>
       <c r="I99" s="21" t="s">
@@ -9905,10 +9905,10 @@
       <c r="F101" s="59" t="s">
         <v>1110</v>
       </c>
-      <c r="G101" s="72" t="s">
+      <c r="G101" s="71" t="s">
         <v>1676</v>
       </c>
-      <c r="H101" s="79" t="s">
+      <c r="H101" s="78" t="s">
         <v>75</v>
       </c>
       <c r="I101" s="21" t="s">
@@ -9946,7 +9946,7 @@
         <v>125</v>
       </c>
       <c r="G102" s="44"/>
-      <c r="H102" s="73" t="s">
+      <c r="H102" s="72" t="s">
         <v>799</v>
       </c>
       <c r="I102" s="28" t="s">
@@ -9993,7 +9993,7 @@
       <c r="J103" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="K103" s="142" t="s">
+      <c r="K103" s="141" t="s">
         <v>115</v>
       </c>
       <c r="L103" s="1"/>
@@ -10022,10 +10022,10 @@
         <v>125</v>
       </c>
       <c r="G104" s="44"/>
-      <c r="H104" s="94" t="s">
+      <c r="H104" s="93" t="s">
         <v>1687</v>
       </c>
-      <c r="I104" s="74" t="s">
+      <c r="I104" s="73" t="s">
         <v>225</v>
       </c>
       <c r="J104" s="25" t="s">
@@ -10069,7 +10069,7 @@
       <c r="J105" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="K105" s="138" t="s">
+      <c r="K105" s="137" t="s">
         <v>111</v>
       </c>
       <c r="L105" s="1"/>
@@ -10094,7 +10094,7 @@
       <c r="E106" s="9" t="s">
         <v>1263</v>
       </c>
-      <c r="F106" s="76" t="s">
+      <c r="F106" s="75" t="s">
         <v>113</v>
       </c>
       <c r="G106" s="44"/>
@@ -10145,7 +10145,7 @@
       <c r="J107" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K107" s="133" t="s">
+      <c r="K107" s="132" t="s">
         <v>112</v>
       </c>
       <c r="L107" s="1"/>
@@ -10183,7 +10183,7 @@
       <c r="J108" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="K108" s="141" t="s">
+      <c r="K108" s="140" t="s">
         <v>114</v>
       </c>
       <c r="L108" s="1"/>
@@ -10213,13 +10213,13 @@
         <v>1672</v>
       </c>
       <c r="H109" s="11"/>
-      <c r="I109" s="74" t="s">
+      <c r="I109" s="73" t="s">
         <v>231</v>
       </c>
       <c r="J109" s="25" t="s">
         <v>387</v>
       </c>
-      <c r="K109" s="140" t="s">
+      <c r="K109" s="139" t="s">
         <v>116</v>
       </c>
       <c r="L109" s="1"/>
@@ -10244,20 +10244,20 @@
       <c r="E110" s="9" t="s">
         <v>1268</v>
       </c>
-      <c r="F110" s="76" t="s">
+      <c r="F110" s="75" t="s">
         <v>1667</v>
       </c>
       <c r="G110" s="44"/>
       <c r="H110" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="I110" s="74" t="s">
+      <c r="I110" s="73" t="s">
         <v>1698</v>
       </c>
       <c r="J110" s="46" t="s">
         <v>1340</v>
       </c>
-      <c r="K110" s="139" t="s">
+      <c r="K110" s="138" t="s">
         <v>117</v>
       </c>
       <c r="L110" s="1"/>
@@ -10287,13 +10287,13 @@
       </c>
       <c r="G111" s="44"/>
       <c r="H111" s="11"/>
-      <c r="I111" s="74" t="s">
+      <c r="I111" s="73" t="s">
         <v>236</v>
       </c>
       <c r="J111" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="K111" s="139" t="s">
+      <c r="K111" s="138" t="s">
         <v>118</v>
       </c>
       <c r="L111" s="1"/>
@@ -10331,7 +10331,7 @@
       <c r="J112" s="25" t="s">
         <v>396</v>
       </c>
-      <c r="K112" s="108" t="s">
+      <c r="K112" s="107" t="s">
         <v>130</v>
       </c>
       <c r="L112" s="1"/>
@@ -10350,16 +10350,16 @@
       <c r="C113" s="9" t="s">
         <v>1270</v>
       </c>
-      <c r="D113" s="67" t="s">
+      <c r="D113" s="66" t="s">
         <v>1224</v>
       </c>
-      <c r="E113" s="67" t="s">
+      <c r="E113" s="66" t="s">
         <v>1671</v>
       </c>
-      <c r="F113" s="88" t="s">
+      <c r="F113" s="87" t="s">
         <v>1667</v>
       </c>
-      <c r="G113" s="128" t="s">
+      <c r="G113" s="127" t="s">
         <v>1672</v>
       </c>
       <c r="H113" s="11" t="s">
@@ -10368,10 +10368,10 @@
       <c r="I113" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J113" s="98" t="s">
+      <c r="J113" s="97" t="s">
         <v>391</v>
       </c>
-      <c r="K113" s="136" t="s">
+      <c r="K113" s="135" t="s">
         <v>121</v>
       </c>
       <c r="L113" s="1"/>
@@ -10399,7 +10399,7 @@
       <c r="F114" s="59" t="s">
         <v>1667</v>
       </c>
-      <c r="G114" s="128" t="s">
+      <c r="G114" s="127" t="s">
         <v>1672</v>
       </c>
       <c r="H114" s="11" t="s">
@@ -10411,7 +10411,7 @@
       <c r="J114" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="K114" s="137" t="s">
+      <c r="K114" s="136" t="s">
         <v>120</v>
       </c>
       <c r="L114" s="1"/>
@@ -10449,7 +10449,7 @@
       <c r="J115" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="K115" s="138" t="s">
+      <c r="K115" s="137" t="s">
         <v>119</v>
       </c>
       <c r="L115" s="1"/>
@@ -10485,7 +10485,7 @@
       <c r="J116" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="K116" s="109" t="s">
+      <c r="K116" s="108" t="s">
         <v>129</v>
       </c>
       <c r="L116" s="1"/>
@@ -10552,7 +10552,7 @@
       <c r="G118" s="59" t="s">
         <v>1109</v>
       </c>
-      <c r="H118" s="73" t="s">
+      <c r="H118" s="72" t="s">
         <v>796</v>
       </c>
       <c r="I118" s="21" t="s">
@@ -10593,10 +10593,10 @@
         <v>1109</v>
       </c>
       <c r="H119" s="11"/>
-      <c r="I119" s="74" t="s">
+      <c r="I119" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="J119" s="129" t="s">
+      <c r="J119" s="128" t="s">
         <v>347</v>
       </c>
       <c r="K119" s="36" t="s">
@@ -10632,7 +10632,7 @@
       <c r="I120" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J120" s="129" t="s">
+      <c r="J120" s="128" t="s">
         <v>348</v>
       </c>
       <c r="K120" s="31"/>
@@ -10666,7 +10666,7 @@
       <c r="I121" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J121" s="129" t="s">
+      <c r="J121" s="128" t="s">
         <v>349</v>
       </c>
       <c r="K121" s="31"/>
@@ -10700,7 +10700,7 @@
       <c r="I122" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J122" s="129" t="s">
+      <c r="J122" s="128" t="s">
         <v>349</v>
       </c>
       <c r="K122" s="31"/>
@@ -10734,10 +10734,10 @@
       <c r="I123" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J123" s="129" t="s">
+      <c r="J123" s="128" t="s">
         <v>561</v>
       </c>
-      <c r="K123" s="106"/>
+      <c r="K123" s="105"/>
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
@@ -10768,10 +10768,10 @@
       <c r="I124" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J124" s="129" t="s">
+      <c r="J124" s="128" t="s">
         <v>562</v>
       </c>
-      <c r="K124" s="102"/>
+      <c r="K124" s="101"/>
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
@@ -10795,17 +10795,17 @@
         <v>1188</v>
       </c>
       <c r="F125" s="9"/>
-      <c r="G125" s="82" t="s">
+      <c r="G125" s="81" t="s">
         <v>1109</v>
       </c>
       <c r="H125" s="11"/>
       <c r="I125" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J125" s="129" t="s">
+      <c r="J125" s="128" t="s">
         <v>351</v>
       </c>
-      <c r="K125" s="106"/>
+      <c r="K125" s="105"/>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
@@ -10833,13 +10833,13 @@
         <v>1109</v>
       </c>
       <c r="H126" s="11"/>
-      <c r="I126" s="74" t="s">
+      <c r="I126" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="J126" s="129" t="s">
+      <c r="J126" s="128" t="s">
         <v>353</v>
       </c>
-      <c r="K126" s="102"/>
+      <c r="K126" s="101"/>
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
@@ -10856,7 +10856,7 @@
       <c r="C127" s="9" t="s">
         <v>1147</v>
       </c>
-      <c r="D127" s="86" t="s">
+      <c r="D127" s="85" t="s">
         <v>1250</v>
       </c>
       <c r="E127" s="9" t="s">
@@ -10870,10 +10870,10 @@
       <c r="I127" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J127" s="129" t="s">
+      <c r="J127" s="128" t="s">
         <v>354</v>
       </c>
-      <c r="K127" s="102"/>
+      <c r="K127" s="101"/>
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
@@ -10890,7 +10890,7 @@
       <c r="C128" s="9" t="s">
         <v>1147</v>
       </c>
-      <c r="D128" s="86" t="s">
+      <c r="D128" s="85" t="s">
         <v>1250</v>
       </c>
       <c r="E128" s="9" t="s">
@@ -10904,10 +10904,10 @@
       <c r="I128" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="J128" s="129" t="s">
+      <c r="J128" s="128" t="s">
         <v>354</v>
       </c>
-      <c r="K128" s="102"/>
+      <c r="K128" s="101"/>
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
@@ -10924,7 +10924,7 @@
       <c r="C129" s="9" t="s">
         <v>1147</v>
       </c>
-      <c r="D129" s="86" t="s">
+      <c r="D129" s="85" t="s">
         <v>1250</v>
       </c>
       <c r="E129" s="9" t="s">
@@ -10941,7 +10941,7 @@
       <c r="J129" s="58" t="s">
         <v>355</v>
       </c>
-      <c r="K129" s="106"/>
+      <c r="K129" s="105"/>
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
@@ -10977,7 +10977,7 @@
       <c r="J130" s="25" t="s">
         <v>356</v>
       </c>
-      <c r="K130" s="110"/>
+      <c r="K130" s="109"/>
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
@@ -11000,7 +11000,7 @@
       <c r="E131" s="9" t="s">
         <v>1194</v>
       </c>
-      <c r="F131" s="72" t="s">
+      <c r="F131" s="71" t="s">
         <v>1658</v>
       </c>
       <c r="G131" s="44"/>
@@ -11115,7 +11115,7 @@
       <c r="J134" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="K134" s="112"/>
+      <c r="K134" s="111"/>
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
@@ -11177,7 +11177,7 @@
       </c>
       <c r="G136" s="44"/>
       <c r="H136" s="11"/>
-      <c r="I136" s="21" t="s">
+      <c r="I136" s="73" t="s">
         <v>42</v>
       </c>
       <c r="J136" s="25" t="s">
@@ -11243,7 +11243,7 @@
       <c r="F138" s="59" t="s">
         <v>1096</v>
       </c>
-      <c r="G138" s="90"/>
+      <c r="G138" s="89"/>
       <c r="H138" s="11"/>
       <c r="I138" s="21" t="s">
         <v>44</v>
@@ -11285,7 +11285,7 @@
       <c r="J139" s="25" t="s">
         <v>364</v>
       </c>
-      <c r="K139" s="102"/>
+      <c r="K139" s="101"/>
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
@@ -11319,7 +11319,7 @@
       <c r="J140" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="K140" s="102" t="s">
+      <c r="K140" s="101" t="s">
         <v>816</v>
       </c>
       <c r="L140" s="1"/>
@@ -11348,16 +11348,16 @@
       <c r="G141" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="H141" s="73" t="s">
+      <c r="H141" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="I141" s="74" t="s">
+      <c r="I141" s="73" t="s">
         <v>29</v>
       </c>
       <c r="J141" s="33" t="s">
         <v>352</v>
       </c>
-      <c r="K141" s="110"/>
+      <c r="K141" s="109"/>
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
@@ -11384,13 +11384,13 @@
       <c r="G142" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="H142" s="94" t="s">
+      <c r="H142" s="93" t="s">
         <v>796</v>
       </c>
-      <c r="I142" s="73" t="s">
+      <c r="I142" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="J142" s="97" t="s">
+      <c r="J142" s="96" t="s">
         <v>352</v>
       </c>
       <c r="K142" s="11"/>
@@ -11423,10 +11423,10 @@
       <c r="H143" s="31" t="s">
         <v>796</v>
       </c>
-      <c r="I143" s="21" t="s">
+      <c r="I143" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J143" s="97" t="s">
+      <c r="J143" s="96" t="s">
         <v>352</v>
       </c>
       <c r="K143" s="11"/>
@@ -11460,7 +11460,7 @@
       <c r="I144" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J144" s="149" t="s">
+      <c r="J144" s="148" t="s">
         <v>814</v>
       </c>
       <c r="K144" s="11"/>
@@ -11531,7 +11531,7 @@
       <c r="H146" s="31" t="s">
         <v>1691</v>
       </c>
-      <c r="I146" s="21" t="s">
+      <c r="I146" s="73" t="s">
         <v>243</v>
       </c>
       <c r="J146" s="25" t="s">
@@ -11572,7 +11572,7 @@
       <c r="I147" s="21" t="s">
         <v>804</v>
       </c>
-      <c r="J147" s="99" t="s">
+      <c r="J147" s="98" t="s">
         <v>805</v>
       </c>
       <c r="K147" s="35" t="s">
@@ -11607,7 +11607,7 @@
       <c r="H148" s="31" t="s">
         <v>1689</v>
       </c>
-      <c r="I148" s="84" t="s">
+      <c r="I148" s="83" t="s">
         <v>504</v>
       </c>
       <c r="J148" s="45" t="s">
@@ -11651,7 +11651,7 @@
       <c r="J149" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="K149" s="116" t="s">
+      <c r="K149" s="115" t="s">
         <v>64</v>
       </c>
       <c r="M149" s="1"/>
@@ -11688,7 +11688,7 @@
       <c r="J150" s="25" t="s">
         <v>369</v>
       </c>
-      <c r="K150" s="103" t="s">
+      <c r="K150" s="102" t="s">
         <v>66</v>
       </c>
       <c r="M150" s="1"/>
@@ -11723,7 +11723,7 @@
       <c r="J151" s="25" t="s">
         <v>366</v>
       </c>
-      <c r="K151" s="115" t="s">
+      <c r="K151" s="114" t="s">
         <v>63</v>
       </c>
       <c r="M151" s="1"/>
@@ -11776,11 +11776,11 @@
       <c r="E153" s="26" t="s">
         <v>1369</v>
       </c>
-      <c r="F153" s="72" t="s">
+      <c r="F153" s="71" t="s">
         <v>1650</v>
       </c>
       <c r="G153" s="10"/>
-      <c r="H153" s="95" t="s">
+      <c r="H153" s="94" t="s">
         <v>787</v>
       </c>
       <c r="I153" s="21" t="s">
@@ -11813,7 +11813,7 @@
       <c r="E154" s="9" t="s">
         <v>1648</v>
       </c>
-      <c r="F154" s="72" t="s">
+      <c r="F154" s="71" t="s">
         <v>1650</v>
       </c>
       <c r="G154" s="10"/>
@@ -11927,7 +11927,7 @@
       </c>
       <c r="G157" s="44"/>
       <c r="H157" s="31"/>
-      <c r="I157" s="21" t="s">
+      <c r="I157" s="73" t="s">
         <v>230</v>
       </c>
       <c r="J157" s="25" t="s">
@@ -11997,7 +11997,7 @@
       </c>
       <c r="G159" s="44"/>
       <c r="H159" s="11"/>
-      <c r="I159" s="21" t="s">
+      <c r="I159" s="73" t="s">
         <v>230</v>
       </c>
       <c r="J159" s="25" t="s">
@@ -12040,7 +12040,7 @@
       <c r="J160" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="K160" s="107" t="s">
+      <c r="K160" s="106" t="s">
         <v>179</v>
       </c>
       <c r="M160" s="1"/>
@@ -12077,7 +12077,7 @@
       <c r="J161" s="25" t="s">
         <v>563</v>
       </c>
-      <c r="K161" s="116" t="s">
+      <c r="K161" s="115" t="s">
         <v>145</v>
       </c>
       <c r="M161" s="1"/>
@@ -12112,7 +12112,7 @@
       <c r="J162" s="25" t="s">
         <v>414</v>
       </c>
-      <c r="K162" s="108" t="s">
+      <c r="K162" s="107" t="s">
         <v>76</v>
       </c>
       <c r="M162" s="1"/>
@@ -12132,7 +12132,7 @@
       </c>
       <c r="D163" s="26"/>
       <c r="E163" s="26"/>
-      <c r="F163" s="72" t="s">
+      <c r="F163" s="71" t="s">
         <v>13</v>
       </c>
       <c r="G163" s="10"/>
@@ -12145,7 +12145,7 @@
       <c r="J163" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="K163" s="100" t="s">
+      <c r="K163" s="99" t="s">
         <v>791</v>
       </c>
       <c r="M163" s="1"/>
@@ -12165,11 +12165,11 @@
       </c>
       <c r="D164" s="9"/>
       <c r="E164" s="9"/>
-      <c r="F164" s="72" t="s">
+      <c r="F164" s="71" t="s">
         <v>8</v>
       </c>
       <c r="G164" s="10"/>
-      <c r="H164" s="95" t="s">
+      <c r="H164" s="94" t="s">
         <v>787</v>
       </c>
       <c r="I164" s="21" t="s">
@@ -12178,7 +12178,7 @@
       <c r="J164" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="K164" s="114" t="s">
+      <c r="K164" s="113" t="s">
         <v>11</v>
       </c>
       <c r="M164" s="1"/>
@@ -12205,13 +12205,13 @@
       </c>
       <c r="G165" s="44"/>
       <c r="H165" s="31"/>
-      <c r="I165" s="21" t="s">
+      <c r="I165" s="73" t="s">
         <v>314</v>
       </c>
       <c r="J165" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="K165" s="108" t="s">
+      <c r="K165" s="107" t="s">
         <v>108</v>
       </c>
       <c r="M165" s="1"/>
@@ -12246,7 +12246,7 @@
       <c r="J166" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="K166" s="108" t="s">
+      <c r="K166" s="107" t="s">
         <v>109</v>
       </c>
       <c r="M166" s="1"/>
@@ -12277,7 +12277,7 @@
       <c r="J167" s="25" t="s">
         <v>655</v>
       </c>
-      <c r="K167" s="108"/>
+      <c r="K167" s="107"/>
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
       <c r="O167" s="1"/>
@@ -12310,7 +12310,7 @@
       <c r="J168" s="25" t="s">
         <v>1477</v>
       </c>
-      <c r="K168" s="108" t="s">
+      <c r="K168" s="107" t="s">
         <v>92</v>
       </c>
       <c r="M168" s="1"/>
@@ -12345,7 +12345,7 @@
       <c r="J169" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="K169" s="108" t="s">
+      <c r="K169" s="107" t="s">
         <v>93</v>
       </c>
       <c r="M169" s="1"/>
@@ -12380,7 +12380,7 @@
       <c r="J170" s="25" t="s">
         <v>797</v>
       </c>
-      <c r="K170" s="116" t="s">
+      <c r="K170" s="115" t="s">
         <v>94</v>
       </c>
       <c r="L170" s="1"/>
@@ -12410,13 +12410,13 @@
       </c>
       <c r="G171" s="44"/>
       <c r="H171" s="31"/>
-      <c r="I171" s="21" t="s">
+      <c r="I171" s="73" t="s">
         <v>272</v>
       </c>
       <c r="J171" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="K171" s="108" t="s">
+      <c r="K171" s="107" t="s">
         <v>95</v>
       </c>
       <c r="L171" s="1"/>
@@ -12452,7 +12452,7 @@
       <c r="J172" s="25" t="s">
         <v>1478</v>
       </c>
-      <c r="K172" s="105" t="s">
+      <c r="K172" s="104" t="s">
         <v>96</v>
       </c>
       <c r="L172" s="1"/>
@@ -12464,24 +12464,24 @@
       <c r="R172" s="1"/>
     </row>
     <row r="173" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B173" s="68" t="s">
+      <c r="B173" s="67" t="s">
         <v>717</v>
       </c>
-      <c r="C173" s="68" t="s">
+      <c r="C173" s="67" t="s">
         <v>808</v>
       </c>
-      <c r="D173" s="68" t="s">
+      <c r="D173" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="E173" s="68" t="s">
+      <c r="E173" s="67" t="s">
         <v>1218</v>
       </c>
-      <c r="F173" s="77" t="s">
+      <c r="F173" s="76" t="s">
         <v>1674</v>
       </c>
-      <c r="G173" s="93"/>
-      <c r="H173" s="69"/>
-      <c r="I173" s="94" t="s">
+      <c r="G173" s="92"/>
+      <c r="H173" s="68"/>
+      <c r="I173" s="93" t="s">
         <v>274</v>
       </c>
       <c r="J173" s="25" t="s">
@@ -12492,42 +12492,43 @@
       </c>
     </row>
     <row r="174" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B174" s="68"/>
+      <c r="B174" s="67"/>
       <c r="C174" s="9"/>
-      <c r="D174" s="67"/>
+      <c r="D174" s="66"/>
       <c r="E174" s="9"/>
       <c r="F174" s="9"/>
-      <c r="G174" s="68"/>
+      <c r="G174" s="67"/>
       <c r="H174" s="11"/>
       <c r="I174" s="21"/>
       <c r="J174" s="9"/>
       <c r="K174" s="11"/>
     </row>
     <row r="175" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B175" s="70"/>
-      <c r="C175" s="70"/>
-      <c r="D175" s="70"/>
-      <c r="E175" s="70"/>
-      <c r="F175" s="70"/>
-      <c r="G175" s="70"/>
-      <c r="H175" s="71"/>
-      <c r="I175" s="71"/>
-      <c r="J175" s="70"/>
-      <c r="K175" s="71"/>
+      <c r="B175" s="69"/>
+      <c r="C175" s="69"/>
+      <c r="D175" s="69"/>
+      <c r="E175" s="69"/>
+      <c r="F175" s="69"/>
+      <c r="G175" s="69"/>
+      <c r="H175" s="70"/>
+      <c r="I175" s="70"/>
+      <c r="J175" s="69"/>
+      <c r="K175" s="70"/>
     </row>
     <row r="176" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B176" s="70"/>
-      <c r="C176" s="70"/>
-      <c r="D176" s="70"/>
-      <c r="E176" s="70"/>
-      <c r="F176" s="70"/>
-      <c r="G176" s="70"/>
-      <c r="H176" s="71"/>
-      <c r="I176" s="71"/>
-      <c r="J176" s="70"/>
-      <c r="K176" s="71"/>
+      <c r="B176" s="69"/>
+      <c r="C176" s="69"/>
+      <c r="D176" s="69"/>
+      <c r="E176" s="69"/>
+      <c r="F176" s="69"/>
+      <c r="G176" s="69"/>
+      <c r="H176" s="70"/>
+      <c r="I176" s="70"/>
+      <c r="J176" s="69"/>
+      <c r="K176" s="70"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:K173" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:K175">
     <sortCondition ref="B4:B175"/>
     <sortCondition ref="C4:C175"/>
@@ -12543,11 +12544,11 @@
   <dimension ref="B2:K269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="J150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
+      <selection pane="bottomRight" activeCell="I196" sqref="I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12560,7 +12561,7 @@
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="77.85546875" style="126" customWidth="1"/>
+    <col min="11" max="11" width="77.85546875" style="125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
@@ -12656,7 +12657,7 @@
       <c r="J6" s="25" t="s">
         <v>1585</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="65" t="s">
         <v>1632</v>
       </c>
     </row>
@@ -12678,7 +12679,7 @@
         <v>1040</v>
       </c>
       <c r="H7" s="9"/>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="59" t="s">
         <v>517</v>
       </c>
       <c r="J7" s="25" t="s">
@@ -12732,7 +12733,7 @@
         <v>1030</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="59" t="s">
         <v>305</v>
       </c>
       <c r="J9" s="25" t="s">
@@ -12760,10 +12761,10 @@
         <v>1047</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="59" t="s">
         <v>544</v>
       </c>
-      <c r="J10" s="143" t="s">
+      <c r="J10" s="142" t="s">
         <v>731</v>
       </c>
       <c r="K10" s="52" t="s">
@@ -12781,14 +12782,14 @@
       <c r="E11" s="59" t="s">
         <v>1530</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="72" t="s">
         <v>1565</v>
       </c>
       <c r="G11" s="59" t="s">
         <v>1055</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="59" t="s">
         <v>544</v>
       </c>
       <c r="J11" s="47" t="s">
@@ -12809,7 +12810,7 @@
       <c r="E12" s="59" t="s">
         <v>1300</v>
       </c>
-      <c r="F12" s="125" t="s">
+      <c r="F12" s="124" t="s">
         <v>1630</v>
       </c>
       <c r="G12" s="59" t="s">
@@ -12837,7 +12838,7 @@
       <c r="E13" s="59" t="s">
         <v>1572</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="72" t="s">
         <v>1591</v>
       </c>
       <c r="G13" s="59" t="s">
@@ -12906,10 +12907,10 @@
         <v>1030</v>
       </c>
       <c r="H15" s="9"/>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="59" t="s">
         <v>495</v>
       </c>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="95" t="s">
         <v>782</v>
       </c>
       <c r="K15" s="52" t="s">
@@ -12937,10 +12938,10 @@
       <c r="I16" s="59" t="s">
         <v>541</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="95" t="s">
         <v>730</v>
       </c>
-      <c r="K16" s="66" t="s">
+      <c r="K16" s="65" t="s">
         <v>1016</v>
       </c>
     </row>
@@ -12955,7 +12956,7 @@
       <c r="E17" s="11" t="s">
         <v>1562</v>
       </c>
-      <c r="F17" s="73" t="s">
+      <c r="F17" s="72" t="s">
         <v>1563</v>
       </c>
       <c r="G17" s="59" t="s">
@@ -13020,7 +13021,7 @@
         <v>1030</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="59" t="s">
         <v>306</v>
       </c>
       <c r="J19" s="25" t="s">
@@ -13032,27 +13033,27 @@
     </row>
     <row r="20" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="25"/>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="63" t="s">
         <v>1147</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>1462</v>
       </c>
-      <c r="F20" s="65"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="59" t="s">
         <v>1072</v>
       </c>
       <c r="H20" s="25"/>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="59" t="s">
         <v>634</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>709</v>
       </c>
-      <c r="K20" s="66" t="s">
+      <c r="K20" s="65" t="s">
         <v>1633</v>
       </c>
     </row>
@@ -13104,7 +13105,7 @@
         <v>1030</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="63" t="s">
+      <c r="I22" s="151" t="s">
         <v>494</v>
       </c>
       <c r="J22" s="25" t="s">
@@ -13221,7 +13222,7 @@
       <c r="I26" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="J26" s="96" t="s">
+      <c r="J26" s="95" t="s">
         <v>588</v>
       </c>
       <c r="K26" s="55" t="s">
@@ -13239,13 +13240,13 @@
       <c r="E27" s="9" t="s">
         <v>1569</v>
       </c>
-      <c r="F27" s="73" t="s">
+      <c r="F27" s="72" t="s">
         <v>1566</v>
       </c>
       <c r="G27" s="59" t="s">
         <v>1055</v>
       </c>
-      <c r="H27" s="121" t="s">
+      <c r="H27" s="120" t="s">
         <v>1567</v>
       </c>
       <c r="I27" s="9" t="s">
@@ -13269,13 +13270,13 @@
       <c r="E28" s="9" t="s">
         <v>1569</v>
       </c>
-      <c r="F28" s="73" t="s">
+      <c r="F28" s="72" t="s">
         <v>1570</v>
       </c>
       <c r="G28" s="59" t="s">
         <v>1055</v>
       </c>
-      <c r="H28" s="121" t="s">
+      <c r="H28" s="120" t="s">
         <v>1567</v>
       </c>
       <c r="I28" s="9" t="s">
@@ -13526,16 +13527,16 @@
     </row>
     <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
-      <c r="C38" s="64" t="s">
+      <c r="C38" s="63" t="s">
         <v>789</v>
       </c>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="63" t="s">
         <v>1380</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="63" t="s">
         <v>1548</v>
       </c>
-      <c r="F38" s="64"/>
+      <c r="F38" s="63"/>
       <c r="G38" s="59" t="s">
         <v>1050</v>
       </c>
@@ -13552,16 +13553,16 @@
     </row>
     <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="63" t="s">
         <v>789</v>
       </c>
-      <c r="D39" s="64" t="s">
+      <c r="D39" s="63" t="s">
         <v>1380</v>
       </c>
-      <c r="E39" s="64" t="s">
+      <c r="E39" s="63" t="s">
         <v>1548</v>
       </c>
-      <c r="F39" s="64"/>
+      <c r="F39" s="63"/>
       <c r="G39" s="59" t="s">
         <v>1050</v>
       </c>
@@ -13652,7 +13653,7 @@
       <c r="J42" s="25" t="s">
         <v>1592</v>
       </c>
-      <c r="K42" s="66" t="s">
+      <c r="K42" s="65" t="s">
         <v>1634</v>
       </c>
     </row>
@@ -13676,7 +13677,7 @@
       <c r="J43" s="24" t="s">
         <v>1595</v>
       </c>
-      <c r="K43" s="66" t="s">
+      <c r="K43" s="65" t="s">
         <v>1635</v>
       </c>
     </row>
@@ -13717,7 +13718,7 @@
       <c r="E45" s="59" t="s">
         <v>1419</v>
       </c>
-      <c r="F45" s="82" t="s">
+      <c r="F45" s="81" t="s">
         <v>1424</v>
       </c>
       <c r="G45" s="59" t="s">
@@ -13804,11 +13805,11 @@
       <c r="F48" s="59" t="s">
         <v>1473</v>
       </c>
-      <c r="G48" s="72" t="s">
+      <c r="G48" s="71" t="s">
         <v>1022</v>
       </c>
       <c r="H48" s="9"/>
-      <c r="I48" s="73" t="s">
+      <c r="I48" s="72" t="s">
         <v>48</v>
       </c>
       <c r="J48" s="25" t="s">
@@ -13834,7 +13835,7 @@
       <c r="F49" s="59" t="s">
         <v>1486</v>
       </c>
-      <c r="G49" s="72" t="s">
+      <c r="G49" s="71" t="s">
         <v>1022</v>
       </c>
       <c r="H49" s="9"/>
@@ -13864,7 +13865,7 @@
       <c r="F50" s="61" t="s">
         <v>1487</v>
       </c>
-      <c r="G50" s="130" t="s">
+      <c r="G50" s="129" t="s">
         <v>1022</v>
       </c>
       <c r="H50" s="9"/>
@@ -13894,14 +13895,14 @@
       <c r="F51" s="61" t="s">
         <v>1482</v>
       </c>
-      <c r="G51" s="130" t="s">
+      <c r="G51" s="129" t="s">
         <v>1022</v>
       </c>
       <c r="H51" s="17"/>
-      <c r="I51" s="11" t="s">
+      <c r="I51" s="72" t="s">
         <v>472</v>
       </c>
-      <c r="J51" s="96" t="s">
+      <c r="J51" s="95" t="s">
         <v>1011</v>
       </c>
       <c r="K51" s="54" t="s">
@@ -13924,7 +13925,7 @@
       <c r="F52" s="61" t="s">
         <v>1483</v>
       </c>
-      <c r="G52" s="130" t="s">
+      <c r="G52" s="129" t="s">
         <v>1022</v>
       </c>
       <c r="H52" s="9"/>
@@ -13954,7 +13955,7 @@
       <c r="F53" s="61" t="s">
         <v>1485</v>
       </c>
-      <c r="G53" s="130" t="s">
+      <c r="G53" s="129" t="s">
         <v>1069</v>
       </c>
       <c r="H53" s="9"/>
@@ -14003,7 +14004,7 @@
       <c r="C55" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="131" t="s">
+      <c r="D55" s="130" t="s">
         <v>55</v>
       </c>
       <c r="E55" s="59"/>
@@ -14048,7 +14049,7 @@
       <c r="J56" s="47" t="s">
         <v>775</v>
       </c>
-      <c r="K56" s="66" t="s">
+      <c r="K56" s="65" t="s">
         <v>1636</v>
       </c>
     </row>
@@ -14162,7 +14163,7 @@
         <v>1073</v>
       </c>
       <c r="H61" s="9"/>
-      <c r="I61" s="9" t="s">
+      <c r="I61" s="59" t="s">
         <v>637</v>
       </c>
       <c r="J61" s="25" t="s">
@@ -14217,7 +14218,7 @@
       <c r="I63" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="J63" s="96" t="s">
+      <c r="J63" s="95" t="s">
         <v>719</v>
       </c>
       <c r="K63" s="52" t="s">
@@ -14238,7 +14239,7 @@
         <v>1073</v>
       </c>
       <c r="H64" s="9"/>
-      <c r="I64" s="9" t="s">
+      <c r="I64" s="59" t="s">
         <v>646</v>
       </c>
       <c r="J64" s="25" t="s">
@@ -14408,7 +14409,7 @@
       <c r="J70" s="25" t="s">
         <v>523</v>
       </c>
-      <c r="K70" s="124" t="s">
+      <c r="K70" s="123" t="s">
         <v>866</v>
       </c>
     </row>
@@ -14431,7 +14432,7 @@
       <c r="I71" s="9" t="s">
         <v>520</v>
       </c>
-      <c r="J71" s="96" t="s">
+      <c r="J71" s="95" t="s">
         <v>521</v>
       </c>
       <c r="K71" s="52" t="s">
@@ -14512,7 +14513,7 @@
         <v>1063</v>
       </c>
       <c r="H74" s="9"/>
-      <c r="I74" s="9" t="s">
+      <c r="I74" s="59" t="s">
         <v>613</v>
       </c>
       <c r="J74" s="25" t="s">
@@ -14542,7 +14543,7 @@
         <v>1025</v>
       </c>
       <c r="H75" s="9"/>
-      <c r="I75" s="9" t="s">
+      <c r="I75" s="59" t="s">
         <v>482</v>
       </c>
       <c r="J75" s="42" t="s">
@@ -14737,10 +14738,10 @@
       <c r="I82" s="9" t="s">
         <v>512</v>
       </c>
-      <c r="J82" s="96" t="s">
+      <c r="J82" s="95" t="s">
         <v>513</v>
       </c>
-      <c r="K82" s="124" t="s">
+      <c r="K82" s="123" t="s">
         <v>859</v>
       </c>
     </row>
@@ -14802,16 +14803,16 @@
     </row>
     <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
-      <c r="C85" s="64" t="s">
+      <c r="C85" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D85" s="64" t="s">
+      <c r="D85" s="63" t="s">
         <v>1147</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>1416</v>
       </c>
-      <c r="F85" s="64"/>
+      <c r="F85" s="63"/>
       <c r="G85" s="59" t="s">
         <v>1060</v>
       </c>
@@ -15148,7 +15149,7 @@
       <c r="J97" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="K97" s="134" t="s">
+      <c r="K97" s="133" t="s">
         <v>848</v>
       </c>
     </row>
@@ -15204,7 +15205,7 @@
       <c r="J99" s="47" t="s">
         <v>1033</v>
       </c>
-      <c r="K99" s="135" t="s">
+      <c r="K99" s="134" t="s">
         <v>1696</v>
       </c>
     </row>
@@ -15232,7 +15233,7 @@
       <c r="J100" s="25" t="s">
         <v>1518</v>
       </c>
-      <c r="K100" s="134" t="s">
+      <c r="K100" s="133" t="s">
         <v>874</v>
       </c>
     </row>
@@ -15252,13 +15253,13 @@
         <v>1044</v>
       </c>
       <c r="H101" s="25"/>
-      <c r="I101" s="76" t="s">
+      <c r="I101" s="75" t="s">
         <v>526</v>
       </c>
       <c r="J101" s="25" t="s">
         <v>525</v>
       </c>
-      <c r="K101" s="134" t="s">
+      <c r="K101" s="133" t="s">
         <v>868</v>
       </c>
     </row>
@@ -15273,7 +15274,7 @@
       <c r="E102" s="9" t="s">
         <v>1189</v>
       </c>
-      <c r="F102" s="65"/>
+      <c r="F102" s="64"/>
       <c r="G102" s="59" t="s">
         <v>1071</v>
       </c>
@@ -15314,7 +15315,7 @@
       <c r="J103" s="25" t="s">
         <v>529</v>
       </c>
-      <c r="K103" s="134" t="s">
+      <c r="K103" s="133" t="s">
         <v>870</v>
       </c>
     </row>
@@ -15342,7 +15343,7 @@
       <c r="J104" s="25" t="s">
         <v>532</v>
       </c>
-      <c r="K104" s="134" t="s">
+      <c r="K104" s="133" t="s">
         <v>873</v>
       </c>
     </row>
@@ -15426,7 +15427,7 @@
       <c r="J107" s="25" t="s">
         <v>1506</v>
       </c>
-      <c r="K107" s="66" t="s">
+      <c r="K107" s="65" t="s">
         <v>1507</v>
       </c>
     </row>
@@ -15526,7 +15527,7 @@
       <c r="J111" s="25" t="s">
         <v>714</v>
       </c>
-      <c r="K111" s="134" t="s">
+      <c r="K111" s="133" t="s">
         <v>880</v>
       </c>
     </row>
@@ -15548,13 +15549,13 @@
         <v>1047</v>
       </c>
       <c r="H112" s="9"/>
-      <c r="I112" s="9" t="s">
+      <c r="I112" s="59" t="s">
         <v>542</v>
       </c>
       <c r="J112" s="25" t="s">
         <v>543</v>
       </c>
-      <c r="K112" s="134" t="s">
+      <c r="K112" s="133" t="s">
         <v>881</v>
       </c>
     </row>
@@ -15582,7 +15583,7 @@
       <c r="J113" s="25" t="s">
         <v>772</v>
       </c>
-      <c r="K113" s="135" t="s">
+      <c r="K113" s="134" t="s">
         <v>1697</v>
       </c>
     </row>
@@ -15602,7 +15603,7 @@
         <v>1072</v>
       </c>
       <c r="H114" s="9"/>
-      <c r="I114" s="9" t="s">
+      <c r="I114" s="59" t="s">
         <v>634</v>
       </c>
       <c r="J114" s="25" t="s">
@@ -15818,7 +15819,7 @@
       <c r="J122" s="25" t="s">
         <v>660</v>
       </c>
-      <c r="K122" s="66" t="s">
+      <c r="K122" s="65" t="s">
         <v>1637</v>
       </c>
     </row>
@@ -15844,7 +15845,7 @@
       <c r="J123" s="20" t="s">
         <v>749</v>
       </c>
-      <c r="K123" s="83" t="s">
+      <c r="K123" s="82" t="s">
         <v>974</v>
       </c>
     </row>
@@ -15973,7 +15974,7 @@
       <c r="I128" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="J128" s="96" t="s">
+      <c r="J128" s="95" t="s">
         <v>623</v>
       </c>
       <c r="K128" s="52" t="s">
@@ -15999,10 +16000,10 @@
       <c r="I129" s="56" t="s">
         <v>622</v>
       </c>
-      <c r="J129" s="123" t="s">
+      <c r="J129" s="122" t="s">
         <v>742</v>
       </c>
-      <c r="K129" s="127" t="s">
+      <c r="K129" s="126" t="s">
         <v>944</v>
       </c>
     </row>
@@ -16278,7 +16279,7 @@
         <v>1052</v>
       </c>
       <c r="H140" s="9"/>
-      <c r="I140" s="9" t="s">
+      <c r="I140" s="59" t="s">
         <v>579</v>
       </c>
       <c r="J140" s="25" t="s">
@@ -16314,7 +16315,7 @@
       <c r="J141" s="45" t="s">
         <v>1488</v>
       </c>
-      <c r="K141" s="83"/>
+      <c r="K141" s="82"/>
     </row>
     <row r="142" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B142" s="8" t="s">
@@ -16362,7 +16363,7 @@
       <c r="F143" s="9" t="s">
         <v>1185</v>
       </c>
-      <c r="G143" s="72" t="s">
+      <c r="G143" s="71" t="s">
         <v>1023</v>
       </c>
       <c r="H143" s="9"/>
@@ -16392,7 +16393,7 @@
       <c r="F144" s="9" t="s">
         <v>1185</v>
       </c>
-      <c r="G144" s="72" t="s">
+      <c r="G144" s="71" t="s">
         <v>1024</v>
       </c>
       <c r="H144" s="9"/>
@@ -16426,7 +16427,7 @@
         <v>1024</v>
       </c>
       <c r="H145" s="9"/>
-      <c r="I145" s="11" t="s">
+      <c r="I145" s="72" t="s">
         <v>40</v>
       </c>
       <c r="J145" s="25" t="s">
@@ -16438,7 +16439,7 @@
     </row>
     <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
-      <c r="C146" s="64" t="s">
+      <c r="C146" s="63" t="s">
         <v>60</v>
       </c>
       <c r="D146" s="9" t="s">
@@ -16447,7 +16448,7 @@
       <c r="E146" s="9" t="s">
         <v>1415</v>
       </c>
-      <c r="F146" s="122" t="s">
+      <c r="F146" s="121" t="s">
         <v>1580</v>
       </c>
       <c r="G146" s="59" t="s">
@@ -16672,7 +16673,7 @@
       <c r="F154" s="61" t="s">
         <v>1509</v>
       </c>
-      <c r="G154" s="78" t="s">
+      <c r="G154" s="77" t="s">
         <v>1039</v>
       </c>
       <c r="H154" s="9"/>
@@ -16716,16 +16717,16 @@
     </row>
     <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B156" s="9"/>
-      <c r="C156" s="64" t="s">
+      <c r="C156" s="63" t="s">
         <v>717</v>
       </c>
-      <c r="D156" s="64" t="s">
+      <c r="D156" s="63" t="s">
         <v>1367</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>1480</v>
       </c>
-      <c r="F156" s="64"/>
+      <c r="F156" s="63"/>
       <c r="G156" s="59" t="s">
         <v>1029</v>
       </c>
@@ -16736,7 +16737,7 @@
       <c r="J156" s="43" t="s">
         <v>707</v>
       </c>
-      <c r="K156" s="66" t="s">
+      <c r="K156" s="65" t="s">
         <v>1638</v>
       </c>
     </row>
@@ -16807,7 +16808,7 @@
       <c r="E159" s="59" t="s">
         <v>1538</v>
       </c>
-      <c r="F159" s="120" t="s">
+      <c r="F159" s="119" t="s">
         <v>1539</v>
       </c>
       <c r="G159" s="59" t="s">
@@ -16926,7 +16927,7 @@
         <v>1050</v>
       </c>
       <c r="H163" s="9"/>
-      <c r="I163" s="9" t="s">
+      <c r="I163" s="59" t="s">
         <v>556</v>
       </c>
       <c r="J163" s="25" t="s">
@@ -17034,7 +17035,7 @@
       <c r="D167" s="9" t="s">
         <v>1406</v>
       </c>
-      <c r="E167" s="120" t="s">
+      <c r="E167" s="119" t="s">
         <v>1536</v>
       </c>
       <c r="F167" s="59" t="s">
@@ -17082,16 +17083,16 @@
     </row>
     <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
-      <c r="C169" s="64" t="s">
+      <c r="C169" s="63" t="s">
         <v>717</v>
       </c>
-      <c r="D169" s="64" t="s">
+      <c r="D169" s="63" t="s">
         <v>1581</v>
       </c>
       <c r="E169" s="9" t="s">
         <v>1582</v>
       </c>
-      <c r="F169" s="64" t="s">
+      <c r="F169" s="63" t="s">
         <v>1583</v>
       </c>
       <c r="G169" s="59" t="s">
@@ -17130,22 +17131,22 @@
       <c r="J170" s="25" t="s">
         <v>708</v>
       </c>
-      <c r="K170" s="66" t="s">
+      <c r="K170" s="65" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B171" s="9"/>
-      <c r="C171" s="64" t="s">
+      <c r="C171" s="63" t="s">
         <v>717</v>
       </c>
-      <c r="D171" s="64" t="s">
+      <c r="D171" s="63" t="s">
         <v>1367</v>
       </c>
       <c r="E171" s="9" t="s">
         <v>1461</v>
       </c>
-      <c r="F171" s="64"/>
+      <c r="F171" s="63"/>
       <c r="G171" s="59" t="s">
         <v>1029</v>
       </c>
@@ -17156,7 +17157,7 @@
       <c r="J171" s="43" t="s">
         <v>771</v>
       </c>
-      <c r="K171" s="66" t="s">
+      <c r="K171" s="65" t="s">
         <v>1639</v>
       </c>
     </row>
@@ -17236,7 +17237,7 @@
         <v>1078</v>
       </c>
       <c r="H174" s="9"/>
-      <c r="I174" s="9" t="s">
+      <c r="I174" s="59" t="s">
         <v>314</v>
       </c>
       <c r="J174" s="25" t="s">
@@ -17302,16 +17303,16 @@
     </row>
     <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B177" s="9"/>
-      <c r="C177" s="64" t="s">
+      <c r="C177" s="63" t="s">
         <v>717</v>
       </c>
-      <c r="D177" s="64" t="s">
+      <c r="D177" s="63" t="s">
         <v>1367</v>
       </c>
       <c r="E177" s="9" t="s">
         <v>1460</v>
       </c>
-      <c r="F177" s="64"/>
+      <c r="F177" s="63"/>
       <c r="G177" s="59" t="s">
         <v>1029</v>
       </c>
@@ -17322,7 +17323,7 @@
       <c r="J177" s="25" t="s">
         <v>706</v>
       </c>
-      <c r="K177" s="66" t="s">
+      <c r="K177" s="65" t="s">
         <v>1640</v>
       </c>
     </row>
@@ -17400,13 +17401,13 @@
         <v>1045</v>
       </c>
       <c r="H180" s="9"/>
-      <c r="I180" s="9" t="s">
+      <c r="I180" s="59" t="s">
         <v>566</v>
       </c>
       <c r="J180" s="43" t="s">
         <v>567</v>
       </c>
-      <c r="K180" s="66" t="s">
+      <c r="K180" s="65" t="s">
         <v>1641</v>
       </c>
     </row>
@@ -17462,7 +17463,7 @@
       <c r="J182" s="25" t="s">
         <v>571</v>
       </c>
-      <c r="K182" s="66" t="s">
+      <c r="K182" s="65" t="s">
         <v>1642</v>
       </c>
     </row>
@@ -17518,7 +17519,7 @@
       <c r="J184" s="25" t="s">
         <v>716</v>
       </c>
-      <c r="K184" s="66" t="s">
+      <c r="K184" s="65" t="s">
         <v>1643</v>
       </c>
     </row>
@@ -17548,7 +17549,7 @@
       <c r="J185" s="47" t="s">
         <v>1094</v>
       </c>
-      <c r="K185" s="66" t="s">
+      <c r="K185" s="65" t="s">
         <v>1644</v>
       </c>
     </row>
@@ -17620,7 +17621,7 @@
         <v>1031</v>
       </c>
       <c r="H188" s="9"/>
-      <c r="I188" s="144" t="s">
+      <c r="I188" s="143" t="s">
         <v>234</v>
       </c>
       <c r="J188" s="25" t="s">
@@ -17814,7 +17815,7 @@
         <v>1052</v>
       </c>
       <c r="H196" s="9"/>
-      <c r="I196" s="9" t="s">
+      <c r="I196" s="59" t="s">
         <v>573</v>
       </c>
       <c r="J196" s="25" t="s">
@@ -17892,7 +17893,7 @@
         <v>1026</v>
       </c>
       <c r="H199" s="9"/>
-      <c r="I199" s="9" t="s">
+      <c r="I199" s="59" t="s">
         <v>488</v>
       </c>
       <c r="J199" s="25" t="s">
@@ -18077,26 +18078,26 @@
       </c>
     </row>
     <row r="207" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B207" s="67"/>
-      <c r="C207" s="82" t="s">
+      <c r="B207" s="66"/>
+      <c r="C207" s="81" t="s">
         <v>1625</v>
       </c>
-      <c r="D207" s="82"/>
-      <c r="E207" s="67" t="s">
+      <c r="D207" s="81"/>
+      <c r="E207" s="66" t="s">
         <v>1424</v>
       </c>
-      <c r="F207" s="82"/>
-      <c r="G207" s="82" t="s">
+      <c r="F207" s="81"/>
+      <c r="G207" s="81" t="s">
         <v>1089</v>
       </c>
-      <c r="H207" s="67"/>
-      <c r="I207" s="67" t="s">
+      <c r="H207" s="66"/>
+      <c r="I207" s="66" t="s">
         <v>694</v>
       </c>
-      <c r="J207" s="96" t="s">
+      <c r="J207" s="95" t="s">
         <v>756</v>
       </c>
-      <c r="K207" s="124" t="s">
+      <c r="K207" s="123" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -18857,6 +18858,7 @@
       <c r="K269" s="52"/>
     </row>
   </sheetData>
+  <autoFilter ref="B4:K208" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:K210">
     <sortCondition ref="C5:C210"/>
     <sortCondition ref="E5:E210"/>

</xml_diff>

<commit_message>
GS 6.1-6.6 and Template files 08/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EEF833-3275-4C89-9035-36E8A8AA7B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E809DB1-1229-4716-9A36-2DF544B57961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -6231,13 +6231,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6312,7 +6313,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>131</v>
@@ -6348,7 +6349,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>131</v>
@@ -6384,7 +6385,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>131</v>
@@ -6420,7 +6421,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
         <v>148</v>
@@ -6458,7 +6459,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>148</v>
@@ -6496,7 +6497,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>148</v>
@@ -6534,7 +6535,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>148</v>
@@ -6553,7 +6554,7 @@
         <v>1129</v>
       </c>
       <c r="H10" s="11"/>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="71" t="s">
         <v>329</v>
       </c>
       <c r="J10" s="46" t="s">
@@ -6570,7 +6571,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>148</v>
@@ -6608,7 +6609,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>148</v>
@@ -6648,7 +6649,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>148</v>
@@ -6686,7 +6687,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>148</v>
@@ -6724,7 +6725,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>148</v>
@@ -6750,7 +6751,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>148</v>
@@ -6786,7 +6787,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>148</v>
@@ -6822,7 +6823,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>148</v>
@@ -6858,7 +6859,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -6894,7 +6895,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>148</v>
@@ -6930,7 +6931,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
         <v>148</v>
@@ -6966,7 +6967,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
         <v>148</v>
@@ -7002,7 +7003,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="s">
         <v>148</v>
@@ -7038,7 +7039,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>148</v>
@@ -7074,7 +7075,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>148</v>
@@ -7112,7 +7113,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
         <v>148</v>
@@ -7150,7 +7151,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
         <v>148</v>
@@ -7188,7 +7189,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9" t="s">
         <v>148</v>
@@ -7226,7 +7227,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9" t="s">
         <v>148</v>
@@ -7262,7 +7263,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>148</v>
@@ -7298,7 +7299,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9" t="s">
         <v>148</v>
@@ -7336,7 +7337,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>148</v>
@@ -7374,7 +7375,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
         <v>148</v>
@@ -7410,7 +7411,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="75.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="9" t="s">
         <v>148</v>
@@ -7446,7 +7447,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="9" t="s">
         <v>148</v>
@@ -7484,7 +7485,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
         <v>148</v>
@@ -7522,7 +7523,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="9" t="s">
         <v>148</v>
@@ -7558,7 +7559,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="9" t="s">
         <v>148</v>
@@ -7594,7 +7595,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
         <v>148</v>
@@ -7632,7 +7633,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
         <v>148</v>
@@ -7668,7 +7669,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="9" t="s">
         <v>148</v>
@@ -7704,7 +7705,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>148</v>
@@ -7740,7 +7741,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
         <v>148</v>
@@ -7776,7 +7777,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="9" t="s">
         <v>148</v>
@@ -7812,7 +7813,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
         <v>148</v>
@@ -7848,7 +7849,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="9" t="s">
         <v>148</v>
@@ -7882,7 +7883,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="9" t="s">
         <v>148</v>
@@ -7920,7 +7921,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
         <v>148</v>
@@ -7956,7 +7957,7 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="9" t="s">
         <v>148</v>
@@ -7992,7 +7993,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="9" t="s">
         <v>148</v>
@@ -8028,7 +8029,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
         <v>148</v>
@@ -8066,7 +8067,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>148</v>
@@ -8104,7 +8105,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
         <v>148</v>
@@ -8142,7 +8143,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
         <v>148</v>
@@ -8180,7 +8181,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
         <v>148</v>
@@ -8218,7 +8219,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
         <v>789</v>
@@ -8256,7 +8257,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
         <v>789</v>
@@ -8290,7 +8291,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="9" t="s">
         <v>789</v>
@@ -8328,7 +8329,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
         <v>789</v>
@@ -8366,7 +8367,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
         <v>789</v>
@@ -8404,7 +8405,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="9" t="s">
         <v>789</v>
@@ -8442,7 +8443,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="8" t="s">
         <v>789</v>
@@ -8476,7 +8477,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="130" t="s">
         <v>15</v>
@@ -8512,7 +8513,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="130" t="s">
         <v>15</v>
@@ -8548,7 +8549,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="130" t="s">
         <v>15</v>
@@ -8584,7 +8585,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="130" t="s">
         <v>15</v>
@@ -8618,7 +8619,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
         <v>98</v>
@@ -8654,7 +8655,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="60.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
         <v>98</v>
@@ -8692,7 +8693,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
         <v>98</v>
@@ -8730,7 +8731,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="9" t="s">
         <v>98</v>
@@ -8766,7 +8767,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="9" t="s">
         <v>98</v>
@@ -8806,7 +8807,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
         <v>98</v>
@@ -8844,7 +8845,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
         <v>98</v>
@@ -8882,7 +8883,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
         <v>1337</v>
@@ -8920,7 +8921,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
         <v>1337</v>
@@ -8958,7 +8959,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
         <v>1337</v>
@@ -8994,7 +8995,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
         <v>1337</v>
@@ -9032,7 +9033,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
         <v>1337</v>
@@ -9070,7 +9071,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
         <v>139</v>
@@ -9108,7 +9109,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
         <v>139</v>
@@ -9146,7 +9147,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
         <v>139</v>
@@ -9167,7 +9168,7 @@
       <c r="H81" s="30" t="s">
         <v>810</v>
       </c>
-      <c r="I81" s="21" t="s">
+      <c r="I81" s="72" t="s">
         <v>324</v>
       </c>
       <c r="J81" s="25" t="s">
@@ -9184,7 +9185,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
         <v>139</v>
@@ -9222,7 +9223,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="9" t="s">
         <v>1316</v>
@@ -9243,7 +9244,7 @@
       <c r="H83" s="11" t="s">
         <v>1662</v>
       </c>
-      <c r="I83" s="21" t="s">
+      <c r="I83" s="72" t="s">
         <v>329</v>
       </c>
       <c r="J83" s="25" t="s">
@@ -9260,7 +9261,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
         <v>1316</v>
@@ -9298,7 +9299,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="9" t="s">
         <v>1316</v>
@@ -9338,7 +9339,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="9" t="s">
         <v>1316</v>
@@ -9376,7 +9377,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="9" t="s">
         <v>1316</v>
@@ -9412,7 +9413,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
         <v>1316</v>
@@ -9448,7 +9449,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
         <v>7</v>
@@ -9484,7 +9485,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="9" t="s">
         <v>7</v>
@@ -9520,7 +9521,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="9" t="s">
         <v>7</v>
@@ -9556,7 +9557,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="9" t="s">
         <v>7</v>
@@ -9592,7 +9593,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
@@ -9628,7 +9629,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="8" t="s">
         <v>7</v>
@@ -9666,7 +9667,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="8" t="s">
         <v>7</v>
@@ -9702,7 +9703,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="9" t="s">
         <v>7</v>
@@ -9740,7 +9741,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="9" t="s">
         <v>7</v>
@@ -9776,7 +9777,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9814,7 +9815,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
         <v>7</v>
@@ -9835,7 +9836,7 @@
       <c r="H99" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="I99" s="21" t="s">
+      <c r="I99" s="72" t="s">
         <v>263</v>
       </c>
       <c r="J99" s="25" t="s">
@@ -9852,7 +9853,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
@@ -9888,7 +9889,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="9" t="s">
         <v>7</v>
@@ -9928,7 +9929,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="9" t="s">
         <v>7</v>
@@ -9966,7 +9967,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="9" t="s">
         <v>7</v>
@@ -10004,7 +10005,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
         <v>7</v>
@@ -10042,7 +10043,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="9" t="s">
         <v>7</v>
@@ -10080,7 +10081,7 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="9" t="s">
         <v>7</v>
@@ -10118,7 +10119,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10156,7 +10157,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>1167</v>
       </c>
@@ -10194,7 +10195,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
         <v>7</v>
@@ -10230,7 +10231,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
         <v>7</v>
@@ -10268,7 +10269,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
         <v>7</v>
@@ -10325,7 +10326,7 @@
         <v>1140</v>
       </c>
       <c r="H112" s="11"/>
-      <c r="I112" s="21" t="s">
+      <c r="I112" s="72" t="s">
         <v>269</v>
       </c>
       <c r="J112" s="25" t="s">
@@ -10342,7 +10343,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
         <v>7</v>
@@ -10382,7 +10383,7 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
         <v>7</v>
@@ -10422,7 +10423,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>7</v>
@@ -10479,7 +10480,7 @@
       </c>
       <c r="G116" s="43"/>
       <c r="H116" s="11"/>
-      <c r="I116" s="21" t="s">
+      <c r="I116" s="72" t="s">
         <v>226</v>
       </c>
       <c r="J116" s="25" t="s">
@@ -10496,7 +10497,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
         <v>7</v>
@@ -10515,7 +10516,7 @@
       </c>
       <c r="G117" s="43"/>
       <c r="H117" s="11"/>
-      <c r="I117" s="21" t="s">
+      <c r="I117" s="72" t="s">
         <v>316</v>
       </c>
       <c r="J117" s="25" t="s">
@@ -10532,7 +10533,7 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
         <v>19</v>
@@ -10572,7 +10573,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="60" t="s">
         <v>19</v>
@@ -10610,7 +10611,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="60" t="s">
         <v>19</v>
@@ -10644,7 +10645,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="60" t="s">
         <v>19</v>
@@ -10678,7 +10679,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="60" t="s">
         <v>19</v>
@@ -10712,7 +10713,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="60" t="s">
         <v>19</v>
@@ -10746,7 +10747,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="60" t="s">
         <v>19</v>
@@ -10780,7 +10781,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="60" t="s">
         <v>19</v>
@@ -10814,7 +10815,7 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="60" t="s">
         <v>19</v>
@@ -10848,7 +10849,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="60" t="s">
         <v>19</v>
@@ -10882,7 +10883,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="60" t="s">
         <v>19</v>
@@ -10916,7 +10917,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="60" t="s">
         <v>19</v>
@@ -10950,7 +10951,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="9" t="s">
         <v>19</v>
@@ -10986,7 +10987,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="9" t="s">
         <v>19</v>
@@ -11022,7 +11023,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="9" t="s">
         <v>19</v>
@@ -11056,7 +11057,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -11090,7 +11091,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="9" t="s">
         <v>19</v>
@@ -11124,7 +11125,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
         <v>19</v>
@@ -11158,7 +11159,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
         <v>19</v>
@@ -11192,7 +11193,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
         <v>19</v>
@@ -11226,7 +11227,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11260,7 +11261,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
         <v>19</v>
@@ -11294,7 +11295,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="9" t="s">
         <v>19</v>
@@ -11330,7 +11331,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
         <v>19</v>
@@ -11366,7 +11367,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
         <v>19</v>
@@ -11402,7 +11403,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
         <v>19</v>
@@ -11438,7 +11439,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="9" t="s">
         <v>19</v>
@@ -11472,7 +11473,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="8" t="s">
         <v>60</v>
@@ -11510,7 +11511,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="8" t="s">
         <v>60</v>
@@ -11548,7 +11549,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="8" t="s">
         <v>60</v>
@@ -11586,7 +11587,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="9" t="s">
         <v>60</v>
@@ -11624,7 +11625,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="9" t="s">
         <v>60</v>
@@ -11645,7 +11646,7 @@
       <c r="H149" s="31" t="s">
         <v>1690</v>
       </c>
-      <c r="I149" s="21" t="s">
+      <c r="I149" s="72" t="s">
         <v>310</v>
       </c>
       <c r="J149" s="25" t="s">
@@ -11661,7 +11662,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="9" t="s">
         <v>60</v>
@@ -11698,7 +11699,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="9" t="s">
         <v>60</v>
@@ -11733,7 +11734,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11764,7 +11765,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="8" t="s">
         <v>60</v>
@@ -11799,7 +11800,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="8" t="s">
         <v>60</v>
@@ -11834,7 +11835,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
         <v>60</v>
@@ -11871,7 +11872,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
         <v>60</v>
@@ -11908,7 +11909,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
         <v>717</v>
@@ -11943,7 +11944,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" ht="30.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>717</v>
@@ -11978,7 +11979,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
         <v>717</v>
@@ -12013,7 +12014,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>717</v>
@@ -12050,7 +12051,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" ht="36.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
         <v>717</v>
@@ -12087,7 +12088,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" ht="46.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
         <v>717</v>
@@ -12122,7 +12123,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
       <c r="B163" s="8" t="s">
         <v>717</v>
@@ -12155,7 +12156,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
       <c r="B164" s="8" t="s">
         <v>717</v>
@@ -12188,7 +12189,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
         <v>717</v>
@@ -12221,7 +12222,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
         <v>717</v>
@@ -12256,7 +12257,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
         <v>717</v>
@@ -12285,7 +12286,7 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
         <v>717</v>
@@ -12304,7 +12305,7 @@
       </c>
       <c r="G168" s="43"/>
       <c r="H168" s="31"/>
-      <c r="I168" s="21" t="s">
+      <c r="I168" s="72" t="s">
         <v>270</v>
       </c>
       <c r="J168" s="25" t="s">
@@ -12320,7 +12321,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" ht="31.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
         <v>717</v>
@@ -12355,7 +12356,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
       <c r="B170" s="9" t="s">
         <v>717</v>
@@ -12391,7 +12392,7 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" ht="46.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
       <c r="B171" s="9" t="s">
         <v>717</v>
@@ -12427,7 +12428,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="9" t="s">
         <v>717</v>
@@ -12463,7 +12464,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B173" s="66" t="s">
         <v>717</v>
       </c>
@@ -12528,7 +12529,14 @@
       <c r="K176" s="69"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:K173" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:K173" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="6.6.3.5"/>
+        <filter val="6.6.5.3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:K175">
     <sortCondition ref="B4:B175"/>
     <sortCondition ref="C4:C175"/>
@@ -12541,14 +12549,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I85" sqref="I85"/>
+      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12609,7 +12618,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="58" t="s">
         <v>131</v>
@@ -12635,7 +12644,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B6" s="9"/>
       <c r="C6" s="58" t="s">
         <v>131</v>
@@ -12661,7 +12670,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="58" t="s">
         <v>131</v>
@@ -12703,7 +12712,7 @@
         <v>1040</v>
       </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="58" t="s">
         <v>518</v>
       </c>
       <c r="J8" s="25" t="s">
@@ -12713,7 +12722,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
@@ -12743,7 +12752,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="58" t="s">
         <v>148</v>
@@ -12771,7 +12780,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="58" t="s">
         <v>148</v>
@@ -12799,7 +12808,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="58" t="s">
         <v>148</v>
@@ -12827,7 +12836,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="45.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="58" t="s">
         <v>148</v>
@@ -12857,7 +12866,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="20.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>148</v>
       </c>
@@ -12887,7 +12896,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>148</v>
       </c>
@@ -12917,7 +12926,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -12945,7 +12954,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
@@ -12973,7 +12982,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -13001,7 +13010,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>148</v>
       </c>
@@ -13031,7 +13040,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B20" s="25"/>
       <c r="C20" s="62" t="s">
         <v>148</v>
@@ -13057,7 +13066,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="58" t="s">
         <v>148</v>
@@ -13085,7 +13094,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>148</v>
       </c>
@@ -13115,7 +13124,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="58" t="s">
         <v>148</v>
@@ -13143,7 +13152,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
         <v>148</v>
@@ -13171,7 +13180,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>148</v>
       </c>
@@ -13201,7 +13210,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
         <v>148</v>
@@ -13229,7 +13238,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="59" t="s">
         <v>148</v>
@@ -13259,7 +13268,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="C28" s="59" t="s">
         <v>148</v>
@@ -13289,7 +13298,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>148</v>
@@ -13313,7 +13322,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="C30" s="59" t="s">
         <v>1626</v>
@@ -13339,7 +13348,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="15"/>
       <c r="C31" s="59" t="s">
         <v>1626</v>
@@ -13363,7 +13372,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="58" t="s">
         <v>1626</v>
@@ -13391,7 +13400,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="C33" s="58" t="s">
         <v>1626</v>
@@ -13415,7 +13424,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="58" t="s">
         <v>1626</v>
@@ -13439,7 +13448,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>789</v>
@@ -13467,7 +13476,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>1463</v>
       </c>
@@ -13497,7 +13506,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9"/>
       <c r="C37" s="58" t="s">
         <v>789</v>
@@ -13525,7 +13534,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="9"/>
       <c r="C38" s="62" t="s">
         <v>789</v>
@@ -13551,7 +13560,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9"/>
       <c r="C39" s="62" t="s">
         <v>789</v>
@@ -13595,7 +13604,7 @@
         <v>1058</v>
       </c>
       <c r="H40" s="9"/>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="58" t="s">
         <v>269</v>
       </c>
       <c r="J40" s="25" t="s">
@@ -13623,7 +13632,7 @@
         <v>1061</v>
       </c>
       <c r="H41" s="9"/>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="58" t="s">
         <v>608</v>
       </c>
       <c r="J41" s="25" t="s">
@@ -13633,7 +13642,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B42" s="9"/>
       <c r="C42" s="58" t="s">
         <v>789</v>
@@ -13657,7 +13666,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:11" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B43" s="9"/>
       <c r="C43" s="58" t="s">
         <v>789</v>
@@ -13681,7 +13690,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="58" t="s">
         <v>1383</v>
@@ -13707,7 +13716,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
       <c r="C45" s="58" t="s">
         <v>1383</v>
@@ -13735,7 +13744,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="58" t="s">
         <v>1383</v>
@@ -13763,7 +13772,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="9"/>
       <c r="C47" s="58" t="s">
         <v>1383</v>
@@ -13789,7 +13798,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>15</v>
       </c>
@@ -13819,7 +13828,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>15</v>
       </c>
@@ -13849,7 +13858,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
@@ -13879,7 +13888,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>15</v>
       </c>
@@ -13909,7 +13918,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="s">
         <v>15</v>
       </c>
@@ -13959,7 +13968,7 @@
         <v>1069</v>
       </c>
       <c r="H53" s="9"/>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="58" t="s">
         <v>475</v>
       </c>
       <c r="J53" s="25" t="s">
@@ -13969,7 +13978,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
         <v>15</v>
       </c>
@@ -13997,7 +14006,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
@@ -14025,7 +14034,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B56" s="9" t="s">
         <v>15</v>
       </c>
@@ -14053,7 +14062,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9"/>
       <c r="C57" s="58" t="s">
         <v>1133</v>
@@ -14077,7 +14086,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
       <c r="C58" s="58" t="s">
         <v>1133</v>
@@ -14101,7 +14110,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="9"/>
       <c r="C59" s="58" t="s">
         <v>1133</v>
@@ -14125,7 +14134,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9"/>
       <c r="C60" s="58" t="s">
         <v>1133</v>
@@ -14139,7 +14148,7 @@
         <v>1073</v>
       </c>
       <c r="H60" s="9"/>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="58" t="s">
         <v>638</v>
       </c>
       <c r="J60" s="25" t="s">
@@ -14149,7 +14158,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="58" t="s">
         <v>1133</v>
@@ -14173,7 +14182,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="58" t="s">
         <v>1133</v>
@@ -14199,7 +14208,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9"/>
       <c r="C63" s="58" t="s">
         <v>1133</v>
@@ -14225,7 +14234,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="9"/>
       <c r="C64" s="58" t="s">
         <v>1133</v>
@@ -14249,7 +14258,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="58" t="s">
         <v>1133</v>
@@ -14277,7 +14286,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
       <c r="C66" s="58" t="s">
         <v>1133</v>
@@ -14303,7 +14312,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
       <c r="C67" s="58" t="s">
         <v>1382</v>
@@ -14331,7 +14340,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="68" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
       <c r="C68" s="58" t="s">
         <v>1337</v>
@@ -14359,7 +14368,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="25"/>
       <c r="C69" s="58" t="s">
         <v>1337</v>
@@ -14385,7 +14394,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="25"/>
       <c r="C70" s="9" t="s">
         <v>1337</v>
@@ -14413,7 +14422,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
       <c r="C71" s="58" t="s">
         <v>1337</v>
@@ -14439,7 +14448,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="25"/>
       <c r="C72" s="57" t="s">
         <v>1337</v>
@@ -14467,7 +14476,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
       <c r="C73" s="58" t="s">
         <v>139</v>
@@ -14485,7 +14494,7 @@
         <v>1063</v>
       </c>
       <c r="H73" s="9"/>
-      <c r="I73" s="9" t="s">
+      <c r="I73" s="58" t="s">
         <v>324</v>
       </c>
       <c r="J73" s="25" t="s">
@@ -14495,7 +14504,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
       <c r="C74" s="58" t="s">
         <v>139</v>
@@ -14523,7 +14532,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>139</v>
       </c>
@@ -14553,7 +14562,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>139</v>
       </c>
@@ -14581,7 +14590,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
         <v>1316</v>
@@ -14609,7 +14618,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
         <v>1316</v>
@@ -14627,7 +14636,7 @@
         <v>1054</v>
       </c>
       <c r="H78" s="9"/>
-      <c r="I78" s="9" t="s">
+      <c r="I78" s="58" t="s">
         <v>329</v>
       </c>
       <c r="J78" s="25" t="s">
@@ -14637,7 +14646,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="58" t="s">
         <v>1316</v>
@@ -14665,7 +14674,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="58" t="s">
         <v>1623</v>
@@ -14691,7 +14700,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="58" t="s">
         <v>1623</v>
@@ -14707,7 +14716,7 @@
         <v>1088</v>
       </c>
       <c r="H81" s="55"/>
-      <c r="I81" s="55" t="s">
+      <c r="I81" s="58" t="s">
         <v>270</v>
       </c>
       <c r="J81" s="25" t="s">
@@ -14717,7 +14726,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -14745,7 +14754,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -14773,7 +14782,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="25"/>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -14801,7 +14810,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="62" t="s">
         <v>7</v>
@@ -14827,7 +14836,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="58" t="s">
         <v>7</v>
@@ -14853,7 +14862,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="58" t="s">
         <v>7</v>
@@ -14879,7 +14888,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="58" t="s">
         <v>7</v>
@@ -14905,7 +14914,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="9" t="s">
         <v>60</v>
       </c>
@@ -14935,7 +14944,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="58" t="s">
         <v>7</v>
@@ -14961,7 +14970,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="91" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="58" t="s">
         <v>7</v>
@@ -14989,7 +14998,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="92" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="58" t="s">
         <v>7</v>
@@ -15015,7 +15024,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="58" t="s">
         <v>7</v>
@@ -15041,7 +15050,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="25"/>
       <c r="C94" s="9" t="s">
         <v>7</v>
@@ -15069,7 +15078,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="95" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="58" t="s">
         <v>7</v>
@@ -15095,7 +15104,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="96" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="25" t="s">
         <v>710</v>
       </c>
@@ -15125,7 +15134,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
         <v>148</v>
       </c>
@@ -15153,7 +15162,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
         <v>19</v>
       </c>
@@ -15181,7 +15190,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>710</v>
       </c>
@@ -15209,7 +15218,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="25"/>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -15237,7 +15246,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="25"/>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -15263,7 +15272,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="25"/>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -15289,7 +15298,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="25" t="s">
         <v>710</v>
       </c>
@@ -15319,7 +15328,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="104" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" s="25" t="s">
         <v>710</v>
       </c>
@@ -15347,7 +15356,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B105" s="9" t="s">
         <v>711</v>
       </c>
@@ -15393,7 +15402,7 @@
         <v>1031</v>
       </c>
       <c r="H106" s="9"/>
-      <c r="I106" s="9" t="s">
+      <c r="I106" s="58" t="s">
         <v>226</v>
       </c>
       <c r="J106" s="25" t="s">
@@ -15403,7 +15412,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15431,7 +15440,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" s="9"/>
       <c r="C108" s="58" t="s">
         <v>7</v>
@@ -15455,7 +15464,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" s="9"/>
       <c r="C109" s="58" t="s">
         <v>7</v>
@@ -15493,7 +15502,7 @@
         <v>1084</v>
       </c>
       <c r="H110" s="9"/>
-      <c r="I110" s="9" t="s">
+      <c r="I110" s="58" t="s">
         <v>673</v>
       </c>
       <c r="J110" s="42" t="s">
@@ -15503,7 +15512,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="9" t="s">
         <v>1261</v>
@@ -15531,7 +15540,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
         <v>1261</v>
@@ -15559,7 +15568,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="113" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" s="25"/>
       <c r="C113" s="9" t="s">
         <v>1261</v>
@@ -15587,7 +15596,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
       <c r="C114" s="58" t="s">
         <v>1552</v>
@@ -15613,7 +15622,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
       <c r="C115" s="58" t="s">
         <v>1552</v>
@@ -15641,7 +15650,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" s="9"/>
       <c r="C116" s="58" t="s">
         <v>1552</v>
@@ -15667,7 +15676,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="117" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" s="9"/>
       <c r="C117" s="58" t="s">
         <v>1552</v>
@@ -15693,7 +15702,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="118" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B118" s="9"/>
       <c r="C118" s="58" t="s">
         <v>1552</v>
@@ -15719,7 +15728,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="119" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="9"/>
       <c r="C119" s="58" t="s">
         <v>1552</v>
@@ -15745,7 +15754,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
       <c r="C120" s="58" t="s">
         <v>1552</v>
@@ -15771,7 +15780,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121" s="9"/>
       <c r="C121" s="58" t="s">
         <v>1552</v>
@@ -15797,7 +15806,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B122" s="9"/>
       <c r="C122" s="58" t="s">
         <v>1552</v>
@@ -15823,7 +15832,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:11" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
       <c r="C123" s="58" t="s">
         <v>1552</v>
@@ -15849,7 +15858,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="9"/>
       <c r="C124" s="58" t="s">
         <v>1552</v>
@@ -15875,7 +15884,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="125" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="9"/>
       <c r="C125" s="58" t="s">
         <v>1552</v>
@@ -15891,7 +15900,7 @@
         <v>1082</v>
       </c>
       <c r="H125" s="9"/>
-      <c r="I125" s="9" t="s">
+      <c r="I125" s="58" t="s">
         <v>669</v>
       </c>
       <c r="J125" s="25" t="s">
@@ -15901,7 +15910,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="126" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126" s="9"/>
       <c r="C126" s="58" t="s">
         <v>1552</v>
@@ -15919,7 +15928,7 @@
         <v>1076</v>
       </c>
       <c r="H126" s="9"/>
-      <c r="I126" s="9" t="s">
+      <c r="I126" s="58" t="s">
         <v>270</v>
       </c>
       <c r="J126" s="25" t="s">
@@ -15929,7 +15938,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="127" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="9"/>
       <c r="C127" s="58" t="s">
         <v>1552</v>
@@ -15971,7 +15980,7 @@
         <v>1066</v>
       </c>
       <c r="H128" s="9"/>
-      <c r="I128" s="9" t="s">
+      <c r="I128" s="58" t="s">
         <v>569</v>
       </c>
       <c r="J128" s="94" t="s">
@@ -15981,7 +15990,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="55"/>
       <c r="C129" s="58" t="s">
         <v>1552</v>
@@ -16007,7 +16016,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="9"/>
       <c r="C130" s="58" t="s">
         <v>1552</v>
@@ -16033,7 +16042,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="9"/>
       <c r="C131" s="58" t="s">
         <v>1552</v>
@@ -16059,7 +16068,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B132" s="9"/>
       <c r="C132" s="58" t="s">
         <v>1552</v>
@@ -16085,7 +16094,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B133" s="9"/>
       <c r="C133" s="58" t="s">
         <v>1552</v>
@@ -16111,7 +16120,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="58" t="s">
         <v>1552</v>
@@ -16137,7 +16146,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="9"/>
       <c r="C135" s="58" t="s">
         <v>1552</v>
@@ -16163,7 +16172,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="9"/>
       <c r="C136" s="58" t="s">
         <v>1552</v>
@@ -16187,7 +16196,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B137" s="9"/>
       <c r="C137" s="58" t="s">
         <v>1552</v>
@@ -16215,7 +16224,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B138" s="9"/>
       <c r="C138" s="58" t="s">
         <v>1552</v>
@@ -16241,7 +16250,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="56" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" s="56" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
       <c r="C139" s="58" t="s">
         <v>1552</v>
@@ -16265,7 +16274,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B140" s="9"/>
       <c r="C140" s="58" t="s">
         <v>1552</v>
@@ -16289,7 +16298,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="s">
         <v>19</v>
       </c>
@@ -16317,7 +16326,7 @@
       </c>
       <c r="K141" s="81"/>
     </row>
-    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B142" s="8" t="s">
         <v>19</v>
       </c>
@@ -16347,7 +16356,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B143" s="8" t="s">
         <v>19</v>
       </c>
@@ -16377,7 +16386,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="s">
         <v>19</v>
       </c>
@@ -16407,7 +16416,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="s">
         <v>19</v>
       </c>
@@ -16437,7 +16446,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B146" s="9"/>
       <c r="C146" s="62" t="s">
         <v>60</v>
@@ -16465,7 +16474,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B147" s="9"/>
       <c r="C147" s="9" t="s">
         <v>60</v>
@@ -16493,7 +16502,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B148" s="9"/>
       <c r="C148" s="58" t="s">
         <v>60</v>
@@ -16521,7 +16530,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B149" s="9"/>
       <c r="C149" s="9" t="s">
         <v>60</v>
@@ -16549,7 +16558,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B150" s="9"/>
       <c r="C150" s="58" t="s">
         <v>60</v>
@@ -16575,7 +16584,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B151" s="9" t="s">
         <v>7</v>
       </c>
@@ -16605,7 +16614,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="9" t="s">
         <v>711</v>
       </c>
@@ -16633,7 +16642,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B153" s="9" t="s">
         <v>711</v>
       </c>
@@ -16661,7 +16670,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="9"/>
       <c r="C154" s="60" t="s">
         <v>60</v>
@@ -16687,7 +16696,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" s="9" t="s">
         <v>1387</v>
       </c>
@@ -16715,7 +16724,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B156" s="9"/>
       <c r="C156" s="62" t="s">
         <v>717</v>
@@ -16741,7 +16750,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B157" s="9"/>
       <c r="C157" s="58" t="s">
         <v>717</v>
@@ -16769,7 +16778,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B158" s="9"/>
       <c r="C158" s="58" t="s">
         <v>717</v>
@@ -16797,7 +16806,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B159" s="43"/>
       <c r="C159" s="58" t="s">
         <v>717</v>
@@ -16825,7 +16834,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B160" s="9"/>
       <c r="C160" s="9" t="s">
         <v>717</v>
@@ -16853,7 +16862,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
         <v>717</v>
@@ -16881,7 +16890,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="58" t="s">
         <v>717</v>
@@ -16909,7 +16918,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="9"/>
       <c r="C163" s="58" t="s">
         <v>717</v>
@@ -16937,7 +16946,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>715</v>
       </c>
@@ -16957,7 +16966,7 @@
         <v>1050</v>
       </c>
       <c r="H164" s="9"/>
-      <c r="I164" s="9" t="s">
+      <c r="I164" s="58" t="s">
         <v>270</v>
       </c>
       <c r="J164" s="25" t="s">
@@ -16967,7 +16976,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>715</v>
       </c>
@@ -16997,7 +17006,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B166" s="9" t="s">
         <v>715</v>
       </c>
@@ -17027,7 +17036,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="9"/>
       <c r="C167" s="9" t="s">
         <v>717</v>
@@ -17055,7 +17064,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="58" t="s">
         <v>717</v>
@@ -17081,7 +17090,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B169" s="9"/>
       <c r="C169" s="62" t="s">
         <v>717</v>
@@ -17109,7 +17118,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B170" s="43"/>
       <c r="C170" s="58" t="s">
         <v>717</v>
@@ -17135,7 +17144,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B171" s="9"/>
       <c r="C171" s="62" t="s">
         <v>717</v>
@@ -17161,7 +17170,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B172" s="9"/>
       <c r="C172" s="9" t="s">
         <v>717</v>
@@ -17187,7 +17196,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>717</v>
       </c>
@@ -17217,7 +17226,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>717</v>
       </c>
@@ -17247,7 +17256,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B175" s="9"/>
       <c r="C175" s="58" t="s">
         <v>717</v>
@@ -17291,7 +17300,7 @@
         <v>1050</v>
       </c>
       <c r="H176" s="9"/>
-      <c r="I176" s="9" t="s">
+      <c r="I176" s="58" t="s">
         <v>534</v>
       </c>
       <c r="J176" s="41" t="s">
@@ -17301,7 +17310,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B177" s="9"/>
       <c r="C177" s="62" t="s">
         <v>717</v>
@@ -17327,7 +17336,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B178" s="9"/>
       <c r="C178" s="58" t="s">
         <v>717</v>
@@ -17355,7 +17364,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B179" s="9"/>
       <c r="C179" s="58" t="s">
         <v>717</v>
@@ -17383,7 +17392,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B180" s="9"/>
       <c r="C180" s="58" t="s">
         <v>717</v>
@@ -17429,7 +17438,7 @@
         <v>1051</v>
       </c>
       <c r="H181" s="9"/>
-      <c r="I181" s="9" t="s">
+      <c r="I181" s="58" t="s">
         <v>569</v>
       </c>
       <c r="J181" s="25" t="s">
@@ -17457,7 +17466,7 @@
         <v>1051</v>
       </c>
       <c r="H182" s="9"/>
-      <c r="I182" s="9" t="s">
+      <c r="I182" s="58" t="s">
         <v>569</v>
       </c>
       <c r="J182" s="25" t="s">
@@ -17467,7 +17476,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="183" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B183" s="9"/>
       <c r="C183" s="58" t="s">
         <v>717</v>
@@ -17495,7 +17504,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B184" s="9"/>
       <c r="C184" s="58" t="s">
         <v>717</v>
@@ -17523,7 +17532,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B185" s="9"/>
       <c r="C185" s="9" t="s">
         <v>60</v>
@@ -17553,7 +17562,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B186" s="9" t="s">
         <v>7</v>
       </c>
@@ -17579,7 +17588,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17605,7 +17614,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B188" s="9" t="s">
         <v>148</v>
       </c>
@@ -17631,7 +17640,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B189" s="9" t="s">
         <v>148</v>
       </c>
@@ -17657,7 +17666,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B190" s="25"/>
       <c r="C190" s="9" t="s">
         <v>717</v>
@@ -17695,7 +17704,7 @@
         <v>1046</v>
       </c>
       <c r="H191" s="43"/>
-      <c r="I191" s="9" t="s">
+      <c r="I191" s="58" t="s">
         <v>534</v>
       </c>
       <c r="J191" s="25" t="s">
@@ -17705,7 +17714,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B192" s="9"/>
       <c r="C192" s="9" t="s">
         <v>717</v>
@@ -17729,7 +17738,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B193" s="9"/>
       <c r="C193" s="9" t="s">
         <v>717</v>
@@ -17753,7 +17762,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>717</v>
@@ -17777,7 +17786,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B195" s="9"/>
       <c r="C195" s="58" t="s">
         <v>717</v>
@@ -17801,7 +17810,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B196" s="9"/>
       <c r="C196" s="58" t="s">
         <v>717</v>
@@ -17825,7 +17834,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B197" s="9"/>
       <c r="C197" s="58" t="s">
         <v>717</v>
@@ -17849,7 +17858,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B198" s="9"/>
       <c r="C198" s="58" t="s">
         <v>717</v>
@@ -17873,7 +17882,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B199" s="9" t="s">
         <v>7</v>
       </c>
@@ -17903,7 +17912,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B200" s="9" t="s">
         <v>7</v>
       </c>
@@ -17947,7 +17956,7 @@
         <v>1089</v>
       </c>
       <c r="H201" s="9"/>
-      <c r="I201" s="9" t="s">
+      <c r="I201" s="58" t="s">
         <v>689</v>
       </c>
       <c r="J201" s="25" t="s">
@@ -17957,7 +17966,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="58" t="s">
         <v>1625</v>
@@ -17981,7 +17990,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B203" s="9"/>
       <c r="C203" s="58" t="s">
         <v>1625</v>
@@ -18005,7 +18014,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B204" s="9"/>
       <c r="C204" s="58" t="s">
         <v>1625</v>
@@ -18029,7 +18038,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B205" s="9"/>
       <c r="C205" s="58" t="s">
         <v>1625</v>
@@ -18053,7 +18062,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B206" s="9"/>
       <c r="C206" s="58" t="s">
         <v>1625</v>
@@ -18077,7 +18086,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="207" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B207" s="65"/>
       <c r="C207" s="80" t="s">
         <v>1625</v>
@@ -18101,7 +18110,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="208" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:11" s="24" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B208" s="9"/>
       <c r="C208" s="58" t="s">
         <v>1625</v>
@@ -18858,7 +18867,21 @@
       <c r="K269" s="51"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:K208" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="B4:K208" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="6.6.1.3"/>
+        <filter val="6.6.2.3"/>
+        <filter val="6.6.3.5"/>
+        <filter val="6.6.4.3"/>
+        <filter val="6.6.4.4"/>
+        <filter val="6.6.4.5"/>
+        <filter val="6.6.5.3"/>
+        <filter val="6.6.7.1"/>
+        <filter val="6.6.9.1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:K210">
     <sortCondition ref="C5:C210"/>
     <sortCondition ref="E5:E210"/>

</xml_diff>

<commit_message>
GS 7 with TS 7 Template files 13/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E809DB1-1229-4716-9A36-2DF544B57961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140B88F-3CF5-428A-8C2C-D82977D1954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jatai" sheetId="1" r:id="rId1"/>
@@ -5644,7 +5644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5951,6 +5951,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6234,11 +6237,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I116" sqref="I116"/>
+      <selection pane="bottomRight" activeCell="I152" sqref="I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8050,7 +8053,7 @@
         <v>1675</v>
       </c>
       <c r="H51" s="11"/>
-      <c r="I51" s="11" t="s">
+      <c r="I51" s="71" t="s">
         <v>323</v>
       </c>
       <c r="J51" s="25" t="s">
@@ -8350,7 +8353,7 @@
       <c r="H59" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="I59" s="71" t="s">
         <v>268</v>
       </c>
       <c r="J59" s="25" t="s">
@@ -9777,7 +9780,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9798,7 +9801,7 @@
       <c r="H98" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="I98" s="21" t="s">
+      <c r="I98" s="72" t="s">
         <v>262</v>
       </c>
       <c r="J98" s="25" t="s">
@@ -10119,7 +10122,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10140,7 +10143,7 @@
       <c r="H107" s="31" t="s">
         <v>1688</v>
       </c>
-      <c r="I107" s="21" t="s">
+      <c r="I107" s="72" t="s">
         <v>233</v>
       </c>
       <c r="J107" s="25" t="s">
@@ -10305,7 +10308,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="18.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
         <v>7</v>
@@ -10461,7 +10464,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
         <v>7</v>
@@ -10698,7 +10701,7 @@
       </c>
       <c r="G122" s="9"/>
       <c r="H122" s="11"/>
-      <c r="I122" s="21" t="s">
+      <c r="I122" s="152" t="s">
         <v>23</v>
       </c>
       <c r="J122" s="127" t="s">
@@ -11006,7 +11009,7 @@
       </c>
       <c r="G131" s="43"/>
       <c r="H131" s="17"/>
-      <c r="I131" s="21" t="s">
+      <c r="I131" s="72" t="s">
         <v>38</v>
       </c>
       <c r="J131" s="25" t="s">
@@ -11042,7 +11045,7 @@
       </c>
       <c r="G132" s="43"/>
       <c r="H132" s="11"/>
-      <c r="I132" s="21" t="s">
+      <c r="I132" s="72" t="s">
         <v>23</v>
       </c>
       <c r="J132" s="25" t="s">
@@ -11076,7 +11079,7 @@
       </c>
       <c r="G133" s="43"/>
       <c r="H133" s="11"/>
-      <c r="I133" s="21" t="s">
+      <c r="I133" s="72" t="s">
         <v>39</v>
       </c>
       <c r="J133" s="25" t="s">
@@ -11227,7 +11230,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11246,7 +11249,7 @@
       </c>
       <c r="G138" s="88"/>
       <c r="H138" s="11"/>
-      <c r="I138" s="21" t="s">
+      <c r="I138" s="72" t="s">
         <v>44</v>
       </c>
       <c r="J138" s="25" t="s">
@@ -11718,7 +11721,7 @@
       <c r="H151" s="31" t="s">
         <v>1689</v>
       </c>
-      <c r="I151" s="21" t="s">
+      <c r="I151" s="72" t="s">
         <v>254</v>
       </c>
       <c r="J151" s="25" t="s">
@@ -11734,7 +11737,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="30.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11749,7 +11752,7 @@
       </c>
       <c r="G152" s="9"/>
       <c r="H152" s="31"/>
-      <c r="I152" s="21" t="s">
+      <c r="I152" s="72" t="s">
         <v>241</v>
       </c>
       <c r="J152" s="25" t="s">
@@ -11944,7 +11947,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>717</v>
@@ -11963,7 +11966,7 @@
       </c>
       <c r="G158" s="43"/>
       <c r="H158" s="11"/>
-      <c r="I158" s="21" t="s">
+      <c r="I158" s="72" t="s">
         <v>229</v>
       </c>
       <c r="J158" s="25" t="s">
@@ -12014,7 +12017,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>717</v>
@@ -12035,7 +12038,7 @@
       <c r="H160" s="11" t="s">
         <v>1693</v>
       </c>
-      <c r="I160" s="21" t="s">
+      <c r="I160" s="72" t="s">
         <v>229</v>
       </c>
       <c r="J160" s="25" t="s">
@@ -12532,8 +12535,11 @@
   <autoFilter ref="A3:K173" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="8">
       <filters>
-        <filter val="6.6.3.5"/>
-        <filter val="6.6.5.3"/>
+        <filter val="7.5.1.5"/>
+        <filter val="7.5.11.2"/>
+        <filter val="7.5.2.1"/>
+        <filter val="7.5.8.4"/>
+        <filter val="7.5.8.5"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -12552,12 +12558,12 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B2:K269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
+      <selection pane="bottomRight" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12698,7 +12704,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
       <c r="C8" s="58" t="s">
         <v>131</v>
@@ -13586,7 +13592,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
       <c r="C40" s="58" t="s">
         <v>789</v>
@@ -13614,7 +13620,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>789</v>
       </c>
@@ -13744,7 +13750,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="9"/>
       <c r="C46" s="58" t="s">
         <v>1383</v>
@@ -13762,7 +13768,7 @@
         <v>1093</v>
       </c>
       <c r="H46" s="9"/>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="58" t="s">
         <v>703</v>
       </c>
       <c r="J46" s="25" t="s">
@@ -13948,7 +13954,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>15</v>
       </c>
@@ -14438,7 +14444,7 @@
         <v>1041</v>
       </c>
       <c r="H71" s="9"/>
-      <c r="I71" s="9" t="s">
+      <c r="I71" s="58" t="s">
         <v>520</v>
       </c>
       <c r="J71" s="94" t="s">
@@ -14466,7 +14472,7 @@
         <v>1042</v>
       </c>
       <c r="H72" s="25"/>
-      <c r="I72" s="9" t="s">
+      <c r="I72" s="58" t="s">
         <v>522</v>
       </c>
       <c r="J72" s="25" t="s">
@@ -15298,7 +15304,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" ht="18" x14ac:dyDescent="0.25">
       <c r="B103" s="25" t="s">
         <v>710</v>
       </c>
@@ -15318,7 +15324,7 @@
         <v>1044</v>
       </c>
       <c r="H103" s="25"/>
-      <c r="I103" s="9" t="s">
+      <c r="I103" s="58" t="s">
         <v>233</v>
       </c>
       <c r="J103" s="25" t="s">
@@ -15386,7 +15392,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" s="9" t="s">
         <v>148</v>
       </c>
@@ -15412,7 +15418,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15430,7 +15436,7 @@
       <c r="H107" s="9" t="s">
         <v>795</v>
       </c>
-      <c r="I107" s="9" t="s">
+      <c r="I107" s="58" t="s">
         <v>1505</v>
       </c>
       <c r="J107" s="25" t="s">
@@ -15488,7 +15494,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B110" s="9"/>
       <c r="C110" s="58" t="s">
         <v>7</v>
@@ -15966,7 +15972,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="128" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="9"/>
       <c r="C128" s="58" t="s">
         <v>1552</v>
@@ -16120,7 +16126,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B134" s="9"/>
       <c r="C134" s="58" t="s">
         <v>1552</v>
@@ -16136,7 +16142,7 @@
         <v>1068</v>
       </c>
       <c r="H134" s="9"/>
-      <c r="I134" s="9" t="s">
+      <c r="I134" s="58" t="s">
         <v>233</v>
       </c>
       <c r="J134" s="25" t="s">
@@ -16714,7 +16720,7 @@
         <v>1092</v>
       </c>
       <c r="H155" s="9"/>
-      <c r="I155" s="9" t="s">
+      <c r="I155" s="58" t="s">
         <v>699</v>
       </c>
       <c r="J155" s="25" t="s">
@@ -17064,7 +17070,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="9"/>
       <c r="C168" s="58" t="s">
         <v>717</v>
@@ -17080,7 +17086,7 @@
         <v>1048</v>
       </c>
       <c r="H168" s="9"/>
-      <c r="I168" s="9" t="s">
+      <c r="I168" s="58" t="s">
         <v>233</v>
       </c>
       <c r="J168" s="25" t="s">
@@ -17284,7 +17290,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" s="9"/>
       <c r="C176" s="58" t="s">
         <v>717</v>
@@ -17420,7 +17426,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B181" s="9"/>
       <c r="C181" s="58" t="s">
         <v>717</v>
@@ -17448,7 +17454,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" hidden="1" x14ac:dyDescent="0.4">
       <c r="B182" s="9"/>
       <c r="C182" s="58" t="s">
         <v>717</v>
@@ -17588,7 +17594,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17604,7 +17610,7 @@
         <v>1031</v>
       </c>
       <c r="H187" s="9"/>
-      <c r="I187" s="9" t="s">
+      <c r="I187" s="58" t="s">
         <v>496</v>
       </c>
       <c r="J187" s="25" t="s">
@@ -17690,7 +17696,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B191" s="43"/>
       <c r="C191" s="9" t="s">
         <v>717</v>
@@ -17942,7 +17948,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="58" t="s">
         <v>1625</v>
@@ -18870,15 +18876,10 @@
   <autoFilter ref="B4:K208" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="7">
       <filters>
-        <filter val="6.6.1.3"/>
-        <filter val="6.6.2.3"/>
-        <filter val="6.6.3.5"/>
-        <filter val="6.6.4.3"/>
-        <filter val="6.6.4.4"/>
-        <filter val="6.6.4.5"/>
-        <filter val="6.6.5.3"/>
-        <filter val="6.6.7.1"/>
-        <filter val="6.6.9.1"/>
+        <filter val="7.5.19.1"/>
+        <filter val="7.5.2.1"/>
+        <filter val="7.5.7.1"/>
+        <filter val="7.5.9.3"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>